<commit_message>
remove default location for the neuwer updated forms
</commit_message>
<xml_diff>
--- a/api/src/main/resources/all-htmlformentry_html_form_13072020.xlsx
+++ b/api/src/main/resources/all-htmlformentry_html_form_13072020.xlsx
@@ -655,7 +655,7 @@
               &lt;/obsgroup&gt;
               &lt;p&gt;
                 &lt;label&gt;Unidade Sanitária:&lt;/label&gt;
-&lt;encounterLocation id="localConsulta" default="5" order="5" /&gt;
+&lt;encounterLocation id="localConsulta" /&gt;
               &lt;/p&gt;
               &lt;relationship type="3" whoAmI="B"  changeExistingRelationship="true" display="search" textLabel="Relacionamento"/&gt;
               &lt;p&gt;
@@ -1077,7 +1077,7 @@
     <t>3ff9fb1a-40fb-4dba-bba4-786be2004d2a</t>
   </si>
   <si>
-    <t>&lt;htmlform&gt;\r\n        &lt;html xmlns=\"http://www.w3.org/1999/xhtml\"&gt;\r\n        &lt;head&gt;\r\n        &lt;meta http-equiv=\"Content-Type\" content=\"text/html; charset=utf-8\" /&gt;\r\n        &lt;title&gt;LIVRO DE REGISTOS DE CONSULTA PRÉ-NATAL&lt;/title&gt;\r\n          &lt;style&gt;\r\n\r\n            .header{\r\n              margin-top: -2px !important;\r\n              margin-bottom: 10px !important;\r\n            }\r\n\r\n            .header label{\r\n              font-weight: bold;\r\n            }\r\n\r\n            .header-info{\r\n              float: right;\r\n              border: 1px dotted #B2DFEE;\r\n              padding: 0px 10px 0px 10px;\r\n            }\r\n\r\n            .header-info h3{\r\n              text-align: center;\r\n            }\r\n\r\n            .header-data{\r\n              float: left;\r\n              border: 1px dotted #B2DFEE;\r\n              margin-bottom: 10px !important;\r\n              padding: 0px 10px 0px 10px;\r\n            }\r\n\r\n            .header-box{\r\n              background: #1aac9b;\r\n              padding: 1px !important;\r\n              color: #fff;\r\n            }\r\n\r\n            .header-box h2{\r\n              margin-left: 10px;\r\n            }\r\n\r\n            .content{\r\n              width: 960px;\r\n              font-size: 8pt;\r\n              margin: 1px auto;\r\n              border: 1px solid #B2DFEE;\r\n              padding: 5px;\r\n            } \r\n\r\n            .demo-data label {\r\n              display: inline-block;\r\n              width: 190px;\r\n            }\r\n\r\n            .demo-data p {\r\n              margin: 3px\r\n            }\r\n\r\n            .demo-data input, .demo-data select {\r\n              width: 140px;\r\n              font-size: 10pt;\r\n            }\r\n\r\n            .clear {\r\n              clear: both;\r\n            }\r\n\r\n            .demo-data-partI{\r\n              float: left;\r\n            }\r\n\r\n            .demo-data-partII{\r\n              float: left;\r\n              margin-left: 100px;\r\n            }\r\n\r\n            #rdp input{\r\n              width: 20px;\r\n            }\r\n\r\n            #rdp label{\r\n              width: 30px;\r\n            }\r\n\r\n            #rdpI{\r\n              width: 150px !important;\r\n            }\r\n\r\n            .tabs ul {\r\n              width: 945px;\r\n              list-style: none;\r\n              float: none;\r\n              position: relative;\r\n              padding: 0;\r\n            }\r\n\r\n            .tabs .rd-visible {\r\n                position: absolute;\r\n                display: none;\r\n            }\r\n\r\n            .tabs label{\r\n              display: block;\r\n              background: #EEE;\r\n              font-weight: bold;\r\n              line-height: 10px;\r\n              padding: 10px 22px;\r\n              font-size: 8pt;\r\n              border: 1px solid #B2DFEE;\r\n              margin-left: -1px;\r\n              cursor: pointer;\r\n            }\r\n\r\n            .tabs li{\r\n              float: left;\r\n            }\r\n\r\n          .tabs [id^=tab]:checked + label{\r\n              background: #1aac9b;\r\n              color: #fff;\r\n            }\r\n\r\n           .tabs [id^=tab]:checked ~ [id^=tab-content] {\r\n                  display: block;\r\n            }\r\n            \r\n           .tabs .tab-content{\r\n                display: none;\r\n                text-align: left;\r\n                width: 100%;\r\n                line-height: 140%;\r\n                padding-top: 10px;\r\n                padding: 11px;\r\n                left: 0;\r\n                position: absolute;\r\n                border: 1px solid #B2DFEE;\r\n                margin: -1px;\r\n                min-height: 150px;\r\n              }\r\n\r\n            \r\n            .tab-data label{\r\n              border: none;\r\n              background: #fff;\r\n              display: inline-block;\r\n              width: 170px;\r\n              padding: 0;\r\n              margin: 0;\r\n              font-weight: normal;\r\n            }\r\n\r\n            .tab-data input, .tab-data select{\r\n              width: 140px;\r\n              font-size: 10pt;\r\n            }\r\n\r\n            .tab-data p {\r\n              margin: 3px;\r\n            }\r\n\r\n            .tab-data-I {\r\n              float: left;\r\n            }\r\n            .tab-data-II {\r\n              float: right;\r\n            }\r\n\r\n            .tab-data-II label {\r\n              width: 300px;\r\n            }\r\n\r\n             \r\n            .rd-tab label{\r\n             width: 60px;\r\n            }\r\n\r\n            .rd-tab input{\r\n             width: 60px;\r\n             margin-top: 0px;\r\n            }\r\n\r\n            .last-details{\r\n              float: none;\r\n              margin-top: 24%;\r\n            }\r\n\r\n            .rd-tab1 input{\r\n             width: 15px !important;\r\n            }\r\n\r\n            &lt;/style&gt;\r\n            &lt;script type=\"text/javascript\"&gt;\r\n              beforeSubmit.push(function() {\r\n\r\n                  var sifilisPartner = getValue(\'sifilisPartner.value\');\r\n                  var testPartner = getValue(\'testPartner.value\');\r\n                  var partner = getValue(\'partner.value\');     \r\n\r\n                  if ((sifilisPartner != \'\' || testPartner != \'\') &amp;amp;&amp;amp; partner == \'\') {\r\n                      getField(\'partner.error\').html(\'obrigatório\').show();\r\n                      return false;\r\n                  }\r\n\r\n                  // var lowWeight = getValue(\'lowWeight.value\');\r\n                  // var brachialPerimeter = getValue(\'brachialPerimeter.value\'); \r\n\r\n                  // if(lowWeight == \"1066\" || brachialPerimeter == \"6371\" || brachialPerimeter == \"6372\"){\r\n                  //   getField(\'cured.error\').html(\'obrigatório\').show();\r\n                  //   return false;\r\n                  // }\r\n\r\n                  var diagnosticITS = getValue(\"diagnosticITS.value\");\r\n                  var itsTreatment = getValue(\'itsTreatment.value\')\r\n\r\n                  if ((diagnosticITS == \"864\" || diagnosticITS == \"5993\") &amp;amp;&amp;amp; itsTreatment == \'\') {\r\n                    getField(\'itsTreatment.error\').html(\'obrigatório\').show();\r\n                    return false;\r\n                  }\r\n\r\n                  var consult = getValue(\'consult.value\');\r\n                  var ageRange = getValue(\'ageRange.value\');\r\n                  var moreThan12weeks = getValue(\'moreThan12weeks.value\');\r\n\r\n                  if (consult === \"6355\" &amp;amp;&amp;amp; (ageRange === \'\' || moreThan12weeks === \'\')) {\r\n                    getField(\"ageRange.error\").html(\"obrigatório\").show();\r\n                    getField(\"moreThan12weeks.error\").html(\"obrigatório\").show();\r\n                    return false;\r\n                  }\r\n\r\n                  var pregnantWeeks = getValue(\'pregnantWeeks.value\');\r\n                  if(pregnantWeeks &gt; 42){\r\n                    getField(\"pregnantWeeks.error\").html(\"o valor não pode ser supererior que 42\").show();\r\n                    return false;\r\n                  }\r\n\r\n                  var weight = getValue(\'weight.value\');\r\n                  if(20 &gt; weight &amp;amp;&amp;amp; weight != 0){\r\n                    getField(\"weight.error\").html(\"peso invalido (20-180 kg)\").show();\r\n                    return false;\r\n                  }\r\n\r\n                  if(weight &gt; 180 &amp;amp;&amp;amp; weight != 0){\r\n                    getField(\"weight.error\").html(\"peso invalido (20-180 kg)\").show();\r\n                    return false;\r\n                  }\r\n\r\n                  // var lastConsult = parseInt(\"&lt;lookup expression=\"fn.latestObs(\'6361\').valueCoded\"/&gt;\");\r\n\r\n                  // if(consult == lastConsult){\r\n                  //   getField(\"consult.error\").html(\"Consulta já existente\").show();\r\n                  //   return false;\r\n                  // }\r\n\r\n                  var startDateTB = new Date(getValue(\'startDateTB.value\'));\r\n                  var endDateTB = new Date(getValue(\'endDateTB.value\'));\r\n\r\n                  if(startDateTB &gt; endDateTB){\r\n                    getField(\"endDateTB.error\").html(\"A data de fim não pode ser inferior a de inicio\").show();\r\n                    return false;\r\n                  }\r\n\r\n                  return true;\r\n              });\r\n\r\n             // consult validator\r\n             jQuery(document).ready(function(){\r\n\r\n                $j(\"#prophilaxysNVP input\").attr(\'disabled\',false);\r\n                var startARV = parseInt(\"&lt;lookup complexExpression=\"#foreach($obs in $fn.allObs(1504)) #if($obs.valueCoded == \'631\') $obs.valueCoded #end #end\"/&gt;\");\r\n                \r\n                if(startARV === 631){\r\n                  $j(\"#prophilaxysNVP input\").attr(\'disabled\',true);\r\n                }\r\n\r\n                $j(\"#prophilaxysAZTNVP input\").attr(\'disabled\',false);\r\n                var nvpAzt = parseInt(\"&lt;lookup complexExpression=\"#foreach($obs in $fn.allObs(1504)) #if($obs.valueCoded == \'1801\') $obs.valueCoded #end #end\"/&gt;\");\r\n                \r\n                if(nvpAzt === 1801){\r\n                  $j(\"#prophilaxysAZTNVP input\").attr(\'disabled\',true);\r\n                }\r\n\r\n                getField(\'consult.value\').live(\'change\', function() {\r\n\r\n                  $j(\"#ageRange select\").attr(\'disabled\',false);\r\n                  $j(\"#moreThan12weeks input:radio\").attr(\'disabled\', false);\r\n                  $j(\"#seroStatus select\").attr(\'disabled\', false);\r\n\r\n                  $j(\"#cured input:radio\").attr(\'disabled\', false);\r\n                  $j(\"#lowWeight input:radio\").attr(\'disabled\', false);\r\n                  $j(\"#abandon input:radio\").attr(\'disabled\', false);\r\n                  $j(\"#prophilaxysARVFOLLOW input\").attr(\'disabled\', false);\r\n\r\n                  if(getValue(\"consult.value\") == \"6355\"){\r\n                    $j(\"#cured input:radio\").attr(\'disabled\', true);\r\n                    $j(\"#lowWeight input:radio\").attr(\'disabled\', true);\r\n                    $j(\"#abandon input:radio\").attr(\'disabled\', true);\r\n                    $j(\"#prophilaxysARVFOLLOW input\").attr(\'disabled\', true);\r\n                  }\r\n\r\n                  if (getValue(\'consult.value\') != \'6355\') {\r\n                    $j(\"#ageRange select\").attr(\'disabled\',true);\r\n                    $j(\"#moreThan12weeks input:radio\").attr(\'disabled\', true);\r\n                    $j(\"#seroStatus select\").attr(\'disabled\', true);\r\n                  }\r\n                  \r\n                });\r\n             \r\n                //serostatus validator\r\n                getField(\'seroStatus.value\').live(\'change\', function(){\r\n                    $j(\"#hivTestCPN select\").attr(\'disabled\', false);\r\n\r\n                    var seroStatus = getValue(\'seroStatus.value\');\r\n          \r\n                    if (seroStatus == \"703\") {\r\n                      $j(\"#hivTestCPN select\").attr(\'disabled\', true);\r\n                    }\r\n                });\r\n\r\n                // validate HIV status if partner present\r\n                $j(\"#testPartner select\").attr(\'disabled\',true);\r\n\r\n                $j(\'#partner input[type=\"radio\"]\').on(\'click change\', function(e) {                 \r\n                    var yesValue = $j(\'#partner input[type=\"radio\"]:checked\').val();\r\n\r\n                    if(yesValue === \'1065\'){\r\n                       $j(\"#testPartner select\").attr(\'disabled\',false);\r\n                       return;\r\n                    }\r\n                    \r\n                    $j(\"#testPartner select\").attr(\'disabled\',true);\r\n                });\r\n\r\n                //validate woman test\r\n                $j(\'#hivTestCPN select\').on(\'change\', function(e) {                 \r\n                    var value =  getValue(\'hivTestCPN.value\');\r\n                    console.log(value);\r\n                    if(value === \'664\'){\r\n                      $j(\"#prophilaxysCZT select\").attr(\'disabled\',true);\r\n                      $j(\"#prophilaxysARV select\").attr(\'disabled\',true);\r\n                      return;\r\n                    }\r\n\r\n                    $j(\"#prophilaxysCZT select\").attr(\'disabled\',false);\r\n                    $j(\"#prophilaxysARV select\").attr(\'disabled\',false);\r\n                });\r\n\r\n                $j(\'#sifilisTest select\').on(\'change\', function(e) {                 \r\n                    var value =  getValue(\'sifilisTest.value\');\r\n\r\n                    if(value === \'1228\'){\r\n                      $j(\"#womanSifilisTest select\").attr(\'disabled\',false);\r\n                      return;\r\n                    }\r\n\r\n                    $j(\"#womanSifilisTest select\").attr(\'disabled\',true);\r\n                });\r\n\r\n               $j(\'#pregnantWeeks\').change(function(){\r\n                  var pregnantWeeks = getValue(\'pregnantWeeks.value\');\r\n                  $j(\"#prophilaxysAZTNVP input\").attr(\'disabled\',false);\r\n\r\n                  if(pregnantWeeks &amp;lt; 14){\r\n                     $j(\"#prophilaxysAZTNVP input\").attr(\'disabled\',true);\r\n                    return;\r\n                  }\r\n                });\r\n\r\n               //Validate sal ferouse\r\n                $j(\'#ferouseOpt input[type=\"radio\"]\').on(\'click change\', function(e) {    \r\n                    var yesValue = $j(\'#ferouseOpt input[type=\"radio\"]:checked\').val();\r\n\r\n                    if(yesValue === \'1066\'){\r\n                       $j(\"#ferouseQtd input\").attr(\'disabled\',true);\r\n                       return;\r\n                    }\r\n                    \r\n                    $j(\"#ferouseQtd input\").attr(\'disabled\',false);\r\n                });\r\n\r\n             });\r\n            &lt;/script&gt;  \r\n        &lt;/head&gt;\r\n\r\n        &lt;body&gt;\r\n        \r\n        &lt;div class=\"header-box content\"&gt;\r\n            &lt;h2&gt;LIVRO DE REGISTOS DE CONSULTA PRÉ-NATAL&lt;/h2&gt;\r\n          &lt;/div&gt;\r\n\r\n        &lt;div class=\"header content\"&gt;\r\n          &lt;div class=\"header-info\"&gt;\r\n            &lt;h3&gt;REPÚBLICA DE MOÇAMBIQUE&lt;/h3&gt;\r\n            &lt;h3&gt;SERVIÇO NACIONAL DE SAÚDE&lt;/h3&gt;\r\n            &lt;h3&gt;MOD - SIS - B01&lt;/h3&gt;\r\n            &lt;p&gt;\r\n              &lt;label&gt;NID/US:&lt;/label&gt;\r\n            &lt;/p&gt;\r\n            &lt;p&gt;\r\n              &lt;label&gt;NID/HDD:&lt;/label&gt;\r\n              &lt;lookup expression=\"patient.getPatientIdentifier(2)\"/&gt;\r\n            &lt;/p&gt;\r\n          &lt;/div&gt;\r\n          &lt;div class=\"header-data\"&gt;\r\n            &lt;p&gt;\r\n              &lt;label&gt;Nome:&lt;/label&gt;\r\n              &lt;lookup expression=\"patient.personName\"/&gt;\r\n            &lt;/p&gt;\r\n            &lt;p&gt;\r\n              &lt;label&gt;Sexo/Data de Nasc./Idade:&lt;/label&gt;\r\n              &lt;lookup expression=\"patient.gender\"/&gt; - &lt;lookup expression=\"patient.birthdate\"/&gt; - &lt;lookup expression=\"patient.age\"/&gt;\r\n            &lt;/p&gt;\r\n            &lt;p&gt;\r\n              &lt;label&gt;Nº de BI/Outra identificação:&lt;/label&gt;\r\n              &lt;lookup expression=\"patient.getPatientIdentifier(3)\"/&gt;/&lt;lookup expression=\"patient.getPatientIdentifier(1)\"/&gt;\r\n            &lt;/p&gt;\r\n            &lt;p&gt;\r\n              &lt;label&gt;Distrito/Cidade:&lt;/label&gt;\r\n              &lt;lookup complexExpression=\"#foreach( $addr in $patient.addresses ) $!addr.countyDistrict #end\"/&gt;\r\n            &lt;/p&gt;\r\n            &lt;p&gt;\r\n              &lt;label&gt;Localidade/Bairro:&lt;/label&gt;\r\n              &lt;lookup complexExpression=\"#foreach( $addr in $patient.addresses ) $!addr.region #end\"/&gt;/&lt;lookup complexExpression=\"#foreach( $addr in $patient.addresses ) $!addr.subregion #end\"/&gt;\r\n            &lt;/p&gt;\r\n            &lt;p&gt;\r\n              &lt;label&gt;Célula/Quarteirão:&lt;/label&gt;\r\n              &lt;lookup complexExpression=\"#foreach( $addr in $patient.addresses ) $!addr.neighborhoodCell #end\"/&gt;\r\n            &lt;/p&gt;\r\n            &lt;p&gt;\r\n              &lt;label&gt;Avenida/Rua/Casa:&lt;/label&gt;\r\n              &lt;lookup complexExpression=\"#foreach( $addr in $patient.addresses ) $!addr.address1 #end\"/&gt;\r\n            &lt;/p&gt;\r\n          &lt;/div&gt;\r\n         \r\n          &lt;div class=\"clear\"/&gt;\r\n          &lt;label &gt;Pessoa de Referência:&lt;/label&gt;&lt;br/&gt;\r\n          &lt;obsgroup groupingConceptId=\"1609\"&gt;\r\n            &lt;obs conceptId=\"1441\" labelText=\"Nome:\" size=\"20\"/&gt; \r\n            &lt;obs conceptId=\"1442\" labelText=\"Apelido:\" size=\"20\"/&gt; \r\n            &lt;obs conceptId=\"1611\" labelText=\"Tel:\" size=\"15\" maxlength=\"9\"/&gt;\r\n          &lt;/obsgroup&gt;\r\n          &lt;p&gt;\r\n            &lt;label&gt;Unidade Sanitária:&lt;/label&gt;&lt;br/&gt;\r\n            \r\n&lt;encounterLocation id=\"localConsulta\" default=\"5\" order=\"5\" /&gt;\r\n          &lt;/p&gt;\r\n          &lt;p&gt;\r\n            &lt;obs conceptId=\"a26e8692-d65c-47c7-9284-8e78eb86802f\" labelText=\"Número do Livro:\" size=\"20\"/&gt; |==|\r\n            &lt;obs conceptId=\"9fdb2c0b-e33a-42c1-9ade-6c57c702c284\" labelText=\"Número da página:\" size=\"20\" /&gt;\r\n          &lt;/p&gt;\r\n        &lt;/div&gt;\r\n         &lt;div class=\"content\"&gt;\r\n            &lt;div class=\"demo-data demo-data-partI\"&gt;\r\n              &lt;p&gt;\r\n                &lt;label&gt;Data da consulta:&lt;/label&gt;\r\n                &lt;encounterDate id=\"dataConsulta\"/&gt;\r\n              &lt;/p&gt;\r\n              &lt;p&gt;\r\n                &lt;label&gt;Consultas:&lt;/label&gt;\r\n                &lt;obs conceptId=\"6361\" id=\"consult\" answerConceptIds=\"6355,6356,6357,6358,6359,6360\" answerLabels=\"1ª,2ª,3ª,4ª,5ª,6ª\"/&gt;\r\n              &lt;/p&gt;\r\n              &lt;p&gt;\r\n                &lt;label&gt;Faixa Etária:&lt;/label&gt;\r\n                &lt;obs conceptId=\"6366\" id=\"ageRange\" answerConceptIds=\"6362,6363,6364,6365\" answerLabels=\"10-14,15-19,20-24,25+\"/&gt;\r\n              &lt;/p&gt;\r\n              &lt;p&gt;\r\n                &lt;label&gt;Data da última mestruação:&lt;/label&gt;\r\n                &lt;obs conceptId=\"e1dc0dd0-1d5f-11e0-b929-000c29ad1d07\" /&gt;\r\n              &lt;/p&gt;\r\n            &lt;/div&gt;\r\n            &lt;div class=\"demo-data demo-data-partII\"&gt;\r\n              &lt;p&gt;\r\n                &lt;label&gt;Idade Gestacional (em semanas):&lt;/label&gt;\r\n                &lt;obs conceptId=\"1279\" size=\"10\" required=\"true\" id=\"pregnantWeeks\"/&gt; \r\n              &lt;/p&gt;\r\n              &lt;p id=\"rdp\"&gt;\r\n                &lt;label id=\"rdpI\"&gt; &amp;lt;12 semanas:&lt;/label&gt;\r\n                &lt;obs conceptId=\"6367\" id=\"moreThan12weeks\" answerConceptIds=\"1065,1066\" answerLabels=\"Sim, Não\" style=\"radio\"/&gt;\r\n              &lt;/p&gt;\r\n              &lt;p id=\"rdp\"&gt;\r\n                &lt;label id=\"rdpI\"&gt;Parceiro Presente ?&lt;/label&gt;\r\n                &lt;obs conceptId=\"6368\" id=\"partner\" answerConceptIds=\"1065,1066\" answerLabels=\"Sim, Não\" style=\"radio\"/&gt;\r\n              &lt;/p&gt;\r\n              &lt;p&gt;\r\n                &lt;label id=\"rdpI\"&gt;Data provável do parto:&lt;/label&gt;\r\n                &lt;obs conceptId=\"e1e76284-1d5f-11e0-b929-000c29ad1d07\" size=\"10\"/&gt;\r\n              &lt;/p&gt;\r\n            &lt;/div&gt;\r\n            &lt;div class=\"clear\" /&gt;\r\n            &lt;div class=\"tabs\"&gt;\r\n              &lt;ul&gt;\r\n                &lt;li&gt;\r\n                  &lt;input type=\"radio\" checked=\"true\" name=\"tabs\" id=\"tab1\" class=\"rd-visible\" /&gt;\r\n                  &lt;label for=\"tab1\"&gt;Nutrição&lt;/label&gt;\r\n                  &lt;div id=\"tab-content-I\" class=\"tab-content\"&gt;\r\n                    &lt;div class=\"tab-data tab-data-I\"&gt;\r\n                      &lt;p&gt;\r\n                        &lt;label&gt;Peso(KG):&lt;/label&gt;\r\n                         &lt;obs conceptId=\"5089\" size=\"10\" id=\"weight\"/&gt;\r\n                      &lt;/p&gt;\r\n                      &lt;p&gt;\r\n                        &lt;label&gt;Perímetro Braquial:&lt;/label&gt;\r\n                         &lt;obs conceptId=\"6373\" id=\"brachialPerimeter\" answerConceptIds=\"6370,6371,6372\" answerLabels=\"˂21 cm (DAG), menor ou igual a 21cm e menor que 23 cm (DAM)s, &amp;gt;23 cm (normal)\"/&gt;\r\n                      &lt;/p&gt;\r\n                    &lt;/div&gt;\r\n                    &lt;div class=\"tab-data tab-data-II\"&gt;\r\n                     &lt;p &gt;\r\n                        &lt;label&gt;Ganho ≥1.5 Kg/mês a partir 2º trimestre ?&lt;/label&gt;\r\n                        &lt;obs conceptId=\"6369\" id=\"lowWeight\" answerConceptIds=\"1065,1066\" answerLabels=\"Sim, Não\" style=\"radio\" class=\"rd-tab\"/&gt;\r\n                     &lt;/p&gt;\r\n                     &lt;p&gt;\r\n                        &lt;label&gt;Recebeu suplementos nutricionais ?&lt;/label&gt;\r\n                        &lt;obs conceptId=\"2152\" answerConceptIds=\"1065,1066\" answerLabels=\"Sim, Não\" style=\"radio\" class=\"rd-tab\"/&gt;\r\n                     &lt;/p&gt;\r\n                     &lt;p&gt;\r\n                        &lt;label&gt;Suplementos nutricionais:&lt;/label&gt;\r\n                        &lt;obs conceptId=\"e1e205f0-1d5f-11e0-b929-000c29ad1d07\" class=\"rd-tab\"/&gt;\r\n                     &lt;/p&gt;\r\n                      &lt;p &gt;\r\n                        &lt;label&gt;Recebeu desparasitante ?&lt;/label&gt;\r\n                        &lt;obs conceptId=\"6377\" answerConceptIds=\"1065,1066\" answerLabels=\"Sim, Não\" style=\"radio\" class=\"rd-tab\"/&gt;\r\n                     &lt;/p&gt;\r\n                     &lt;p&gt;\r\n                        &lt;label&gt;Sal Ferroso com Ácido Fólico?&lt;/label&gt;\r\n                        &lt;obs conceptId=\"6378\" id=\"ferouseOpt\" answerConceptIds=\"1065,1066\" answerLabels=\"Sim, Não\" style=\"radio\" class=\"rd-tab\"/&gt;\r\n                     &lt;/p&gt;\r\n                     &lt;p&gt;\r\n                        &lt;label&gt;Quantidade de Sal Ferroso&lt;/label&gt;\r\n                        &lt;obs conceptId=\"35fba30b-a7da-4f39-a7e0-2cef36a06348\" id=\"ferouseQtd\" class=\"rd-tab\"/&gt;\r\n                     &lt;/p&gt;\r\n                    &lt;/div&gt;\r\n                    &lt;div class=\"clear\" /&gt;\r\n                    &lt;div class=\"tab-data tab-data-I\"&gt;\r\n                      &lt;p&gt;\r\n                        &lt;label style=\"font-weight:bold; width:150px;\"&gt;Resultado:&lt;/label&gt;\r\n                      &lt;/p&gt;\r\n                      &lt;p &gt;\r\n                        &lt;label&gt;Curado ?&lt;/label&gt;\r\n                        &lt;obs conceptId=\"6375\" id=\"cured\" answerConceptIds=\"1065,1066\" answerLabels=\"Sim, Não\" style=\"radio\" class=\"rd-tab\"/&gt;\r\n                      &lt;/p&gt;\r\n                      &lt;p&gt;\r\n                        &lt;label&gt;Abandono ?&lt;/label&gt;\r\n                        &lt;obs conceptId=\"6376\" id=\"abandon\" answerConceptIds=\"1065,1066\" answerLabels=\"Sim, Não\" style=\"radio\" class=\"rd-tab\"/&gt;\r\n                      &lt;/p&gt;\r\n                    &lt;/div&gt;\r\n                  &lt;/div&gt;\r\n                &lt;/li&gt;\r\n                &lt;li&gt;\r\n                  &lt;input type=\"radio\" name=\"tabs\" id=\"tab2\" class=\"rd-visible\" /&gt;\r\n                  &lt;label for=\"tab2\"&gt;Exames&lt;/label&gt;\r\n                  &lt;div id=\"tab-content-II\" class=\"tab-content\"&gt;\r\n                    &lt;div class=\"tab-data tab-data-I\"&gt;\r\n                      &lt;p&gt;\r\n                        &lt;label&gt;Tensão Arterial (TA ≥ 140/90mmHg) ?&lt;/label&gt;\r\n                        &lt;obs conceptId=\"6379\" required=\"true\" answerConceptIds=\"1065,1066,1118\" answerLabels=\"Sim, Não, Não Fez\"/&gt;\r\n                      &lt;/p&gt;\r\n                      &lt;p&gt;\r\n                        &lt;label&gt;Hemoglobina (HGB ˂11g/dL)?&lt;/label&gt;\r\n                        &lt;obs conceptId=\"6380\" answerConceptIds=\"1065,1066,1118\" answerLabels=\"Sim, Não, Não Fez\"/&gt;\r\n                      &lt;/p&gt;\r\n                       &lt;p&gt;\r\n                        &lt;label&gt;Proteinúria ?&lt;/label&gt;\r\n                        &lt;obs conceptId=\"6381\" answerConceptIds=\"1065,1066,1118\" answerLabels=\"Sim, Não, Não Fez\"/&gt;\r\n                      &lt;/p&gt;\r\n                       &lt;p&gt;\r\n                        &lt;label&gt;Glicosúria ?&lt;/label&gt;\r\n                        &lt;obs conceptId=\"6382\" answerConceptIds=\"1065,1066,1118\" answerLabels=\"Sim, Não, Não Fez\"/&gt;\r\n                      &lt;/p&gt;\r\n                    &lt;/div&gt;\r\n                  &lt;/div&gt;\r\n                &lt;/li&gt;\r\n                &lt;li&gt;\r\n                  &lt;input type=\"radio\" name=\"tabs\" id=\"tab3\" class=\"rd-visible\"/&gt;\r\n                  &lt;label for=\"tab3\"&gt;Sífilis e outras ITS\'s&lt;/label&gt;\r\n                  &lt;div id=\"tab-content-III\" class=\"tab-content\"&gt;\r\n                    &lt;div class=\"tab-data tab-data-I\"&gt;\r\n                      &lt;p&gt;\r\n                        &lt;label style=\"font-weight:bold; width:150px;\"&gt;Diagnóstico de ITS&lt;/label&gt;\r\n                      &lt;/p&gt;\r\n                      &lt;p&gt;\r\n                        &lt;obs conceptId=\"1080\" answerConceptId=\"864\" style=\"checkbox\" answerLabel=\"Ulceras Genitais\"/&gt;\r\n                      &lt;/p&gt;\r\n                      &lt;p&gt;\r\n                        &lt;obs conceptId=\"1080\" answerConceptId=\"5993\" style=\"checkbox\" answerLabel=\"Leucorreias\" /&gt;\r\n                      &lt;/p&gt;\r\n                      &lt;p&gt;\r\n                        &lt;label&gt;Teste de Sífilis:&lt;/label&gt;\r\n                        &lt;obs conceptId=\"299\" id=\"sifilisTest\" answerConceptIds=\"1228,1229,1118\" answerLabels=\"Positivo, Negativo, Não Feito\"/&gt;\r\n                      &lt;/p&gt;\r\n                    &lt;/div&gt;\r\n                    &lt;div class=\"tab-data tab-data-II\"&gt;\r\n                     &lt;p &gt;\r\n                        &lt;label&gt;Tratamento Sindrómico de ITS ?&lt;/label&gt;\r\n                        &lt;obs conceptId=\"1975\" id=\"itsTreatment\" answerConceptIds=\"1065,1066\" answerLabels=\"Sim, Não\" style=\"radio\" class=\"rd-tab\"/&gt;\r\n                     &lt;/p&gt;\r\n                    &lt;/div&gt;\r\n                    &lt;div class=\"clear\" /&gt;\r\n                    &lt;br/&gt;\r\n                    &lt;div class=\"tab-data tab-data-I\"&gt;\r\n                      &lt;p&gt;\r\n                        &lt;label style=\"font-weight:bold; width:150px;\"&gt;Tratamento para Sífilis:&lt;/label&gt;\r\n                      &lt;/p&gt;\r\n                      &lt;p &gt;\r\n                        &lt;label&gt;Mulher ?&lt;/label&gt;\r\n                        &lt;obs conceptId=\"6383\" id=\"womanSifilisTest\" answerConceptIds=\"1182,2084\" answerLabels=\"1ª dose,3ª dose\"/&gt;\r\n                      &lt;/p&gt;\r\n                      &lt;p&gt;\r\n                        &lt;label&gt;Parceiro ?&lt;/label&gt;\r\n                        &lt;obs conceptId=\"6384\" id=\"sifilisPartner\" answerConceptIds=\"1065,1066,1118\" answerLabels=\"Sim, Não, Não Feito\" /&gt;\r\n                      &lt;/p&gt;\r\n                    &lt;/div&gt;\r\n                  &lt;/div&gt;\r\n                &lt;/li&gt;\r\n                 &lt;li&gt;\r\n                  &lt;input type=\"radio\" name=\"tabs\" id=\"tab4\" class=\"rd-visible\"/&gt;\r\n                  &lt;label for=\"tab4\"&gt;PTV de HIV&lt;/label&gt;\r\n                  &lt;div id=\"tab-content-IV\" class=\"tab-content\"&gt;\r\n                    &lt;div class=\"tab-data tab-data-I\"&gt;\r\n                      &lt;p&gt;\r\n                        &lt;label&gt;Seroestado entrada a 1ª CPN:&lt;/label&gt;\r\n                        &lt;obs conceptId=\"6385\" id=\"seroStatus\" answerConceptIds=\"664,703,1067\" answerLabels=\"Negativo, Positivo, Desconhecido\"/&gt;\r\n                      &lt;/p&gt;\r\n                      &lt;p&gt;\r\n                        &lt;label&gt;Teste de HIV na CPN:&lt;/label&gt;\r\n                        &lt;obs conceptId=\"2079\" id=\"hivTestCPN\" answerConceptIds=\"664,703,1138,1118\" answerLabels=\"Negativo, Positivo, Ideterminado, Não Feito\"/&gt;\r\n                      &lt;/p&gt;\r\n                      &lt;p&gt;\r\n                        &lt;label&gt;Teste do Parceiro:&lt;/label&gt;\r\n                        &lt;obs conceptId=\"2074\" id=\"testPartner\" answerConceptIds=\"664,703,1138,1118\" answerLabels=\"Negativo, Positivo, Ideterminado, Não Feito\"/&gt;\r\n                      &lt;/p&gt;\r\n                    &lt;/div&gt;\r\n                    &lt;div class=\"tab-data tab-data-II\"&gt;\r\n                      &lt;p&gt;\r\n                        &lt;label style=\"font-weight:bold; width:150px;\"&gt;Profilaxias:&lt;/label&gt;\r\n                      &lt;/p&gt;\r\n                      &lt;p&gt;\r\n                        &lt;obs conceptId=\"6121\" id=\"prophilaxysCZT\" answerConceptId=\"6386\" answerLabel=\"Em CTZ a entrada\" style=\"checkbox\"/&gt;\r\n                      &lt;/p&gt;\r\n                      &lt;p&gt;\r\n                        &lt;label&gt;Profilaxia CTZ:&lt;/label&gt;\r\n                        &lt;obs conceptId=\"6121\" id=\"prophilaxysCZT\" answerConceptIds=\"1256,1257\" answerLabels=\"Início, Continuação\"/&gt;\r\n                      &lt;/p&gt;\r\n\r\n                      &lt;p&gt;\r\n                        &lt;obs conceptId=\"1504\" id=\"prophilaxysARV\" answerConceptId=\"6388\" answerLabel=\"Em TARV a entrada\" style=\"checkbox\" /&gt;\r\n                      &lt;/p&gt;\r\n\r\n                      &lt;p&gt;\r\n                        &lt;obs conceptId=\"1504\" id=\"prophilaxysNVP\" answerConceptId=\"631\" answerLabel=\"Entrega de Monoprofilaxia (NVP) nesta visita\" style=\"checkbox\"/&gt;\r\n                      &lt;/p&gt;\r\n\r\n                      &lt;p&gt;\r\n                        &lt;obs conceptId=\"1504\" id=\"prophilaxysAZTNVP\" answerConceptId=\"1801\" answerLabel=\"Inicia biprofilaxia (AZT+NVP) nesta visita\" style=\"checkbox\"/&gt;\r\n                      &lt;/p&gt;\r\n\r\n                      &lt;p&gt;\r\n                        &lt;obs conceptId=\"1504\" id=\"prophilaxysARVSTART\" answerConceptId=\"1256\" answerLabel=\"Inicia o TARV nesta visita\" style=\"checkbox\" /&gt;\r\n                      &lt;/p&gt;\r\n\r\n                      &lt;p&gt;\r\n                        &lt;obs conceptId=\"1504\" id=\"prophilaxysARVFOLLOW\" answerConceptId=\"1257\" answerLabel=\"Continua ARV nesta visita\" style=\"checkbox\" /&gt;\r\n                      &lt;/p&gt;\r\n\r\n                    &lt;/div&gt;\r\n                  &lt;/div&gt;\r\n                &lt;/li&gt;\r\n                 &lt;li&gt;\r\n                  &lt;input type=\"radio\" name=\"tabs\" id=\"tab5\" class=\"rd-visible\"/&gt;\r\n                  &lt;label for=\"tab5\"&gt;Malaria&lt;/label&gt;\r\n                  &lt;div id=\"tab-content-V\" class=\"tab-content\"&gt;\r\n                    &lt;div class=\"tab-data tab-data-I\"&gt;\r\n                      &lt;p&gt;\r\n                        &lt;label&gt;Prevenção da Malária (TIP) :&lt;/label&gt;\r\n                        &lt;obs conceptId=\"6389\" answerConceptIds=\"1182,1183,2084,2085\" answerLabels=\"1ª, 2ª, 3ª, 4ª+\"/&gt;\r\n                      &lt;/p&gt;\r\n                    &lt;/div&gt;\r\n                    &lt;div class=\"tab-data tab-data-II\"&gt;\r\n                      &lt;p &gt;\r\n                        &lt;label&gt;Recebeu Rede Mosquiteira?&lt;/label&gt;\r\n                        &lt;obs conceptId=\"1863\" answerConceptIds=\"1065,1066\" answerLabels=\"Sim, Não\" style = \"radio\" class=\"rd-tab\"/&gt;\r\n                      &lt;/p&gt;\r\n                      &lt;p &gt;\r\n                        &lt;label&gt;Testadas para Malaria:&lt;/label&gt;\r\n                        &lt;obs conceptId=\"6392\" answerConceptIds=\"6390,6391\" answerLabels=\"HTZ, TDR\" style = \"radio\" class=\"rd-tab\"/&gt;\r\n                      &lt;/p&gt;\r\n                    &lt;/div&gt;\r\n                    &lt;div class=\"clear\" /&gt;\r\n                    &lt;br/&gt;\r\n                    &lt;div class=\"tab-data tab-data-I\"&gt;\r\n                      &lt;p&gt;\r\n                        &lt;label style=\"font-weight:bold; width:250px;\"&gt;Diagnóstico e Tratamento de Malária:&lt;/label&gt;\r\n                      &lt;/p&gt;\r\n                      &lt;p &gt;\r\n                        &lt;label&gt;Resultado TDR ou HTZ:&lt;/label&gt;\r\n                        &lt;obs conceptId=\"32\" answerConceptIds=\"664,703,1138,1118\" answerLabels=\"Negativo, Positivo, Indeterminado, Não Feito\"/&gt;\r\n                      &lt;/p&gt;\r\n                      &lt;p&gt;\r\n                        &lt;label&gt;Mulheres com teste de Malária Positivo e Tratadas:&lt;/label&gt;\r\n                        &lt;obs conceptId=\"6393\" answerConceptIds=\"1065,1066,1364\" answerLabels=\"Sim, Não, Não elegivel\" /&gt;\r\n                      &lt;/p&gt;\r\n                    &lt;/div&gt;\r\n                  &lt;/div&gt;\r\n                &lt;/li&gt;\r\n                &lt;li&gt;\r\n                  &lt;input type=\"radio\" name=\"tabs\" id=\"tab6\" class=\"rd-visible\"/&gt;\r\n                  &lt;label for=\"tab6\"&gt;HPP e VAT&lt;/label&gt;\r\n                  &lt;div id=\"tab-content-VI\" class=\"tab-content\"&gt;\r\n                    &lt;div class=\"tab-data tab-data-I\"&gt;\r\n                     &lt;p &gt;\r\n                      &lt;label&gt;Recebeu Misoprostol?&lt;/label&gt;\r\n                      &lt;obs conceptId=\"6351\" answerConceptIds=\"1065,1066\" answerLabels=\"Sim, Não\" style=\"radio\" class=\"rd-tab rd-tab1\"/&gt;\r\n                    &lt;/p&gt;\r\n                    &lt;p&gt;\r\n                      &lt;label&gt;VAT:&lt;/label&gt;\r\n                      &lt;obs conceptId=\"54\" answerConceptIds=\"1182,1184, 1118\" answerLabels=\"1ª dose,</t>
+    <t>&lt;htmlform&gt;\r\n        &lt;html xmlns=\"http://www.w3.org/1999/xhtml\"&gt;\r\n        &lt;head&gt;\r\n        &lt;meta http-equiv=\"Content-Type\" content=\"text/html; charset=utf-8\" /&gt;\r\n        &lt;title&gt;LIVRO DE REGISTOS DE CONSULTA PRÉ-NATAL&lt;/title&gt;\r\n          &lt;style&gt;\r\n\r\n            .header{\r\n              margin-top: -2px !important;\r\n              margin-bottom: 10px !important;\r\n            }\r\n\r\n            .header label{\r\n              font-weight: bold;\r\n            }\r\n\r\n            .header-info{\r\n              float: right;\r\n              border: 1px dotted #B2DFEE;\r\n              padding: 0px 10px 0px 10px;\r\n            }\r\n\r\n            .header-info h3{\r\n              text-align: center;\r\n            }\r\n\r\n            .header-data{\r\n              float: left;\r\n              border: 1px dotted #B2DFEE;\r\n              margin-bottom: 10px !important;\r\n              padding: 0px 10px 0px 10px;\r\n            }\r\n\r\n            .header-box{\r\n              background: #1aac9b;\r\n              padding: 1px !important;\r\n              color: #fff;\r\n            }\r\n\r\n            .header-box h2{\r\n              margin-left: 10px;\r\n            }\r\n\r\n            .content{\r\n              width: 960px;\r\n              font-size: 8pt;\r\n              margin: 1px auto;\r\n              border: 1px solid #B2DFEE;\r\n              padding: 5px;\r\n            } \r\n\r\n            .demo-data label {\r\n              display: inline-block;\r\n              width: 190px;\r\n            }\r\n\r\n            .demo-data p {\r\n              margin: 3px\r\n            }\r\n\r\n            .demo-data input, .demo-data select {\r\n              width: 140px;\r\n              font-size: 10pt;\r\n            }\r\n\r\n            .clear {\r\n              clear: both;\r\n            }\r\n\r\n            .demo-data-partI{\r\n              float: left;\r\n            }\r\n\r\n            .demo-data-partII{\r\n              float: left;\r\n              margin-left: 100px;\r\n            }\r\n\r\n            #rdp input{\r\n              width: 20px;\r\n            }\r\n\r\n            #rdp label{\r\n              width: 30px;\r\n            }\r\n\r\n            #rdpI{\r\n              width: 150px !important;\r\n            }\r\n\r\n            .tabs ul {\r\n              width: 945px;\r\n              list-style: none;\r\n              float: none;\r\n              position: relative;\r\n              padding: 0;\r\n            }\r\n\r\n            .tabs .rd-visible {\r\n                position: absolute;\r\n                display: none;\r\n            }\r\n\r\n            .tabs label{\r\n              display: block;\r\n              background: #EEE;\r\n              font-weight: bold;\r\n              line-height: 10px;\r\n              padding: 10px 22px;\r\n              font-size: 8pt;\r\n              border: 1px solid #B2DFEE;\r\n              margin-left: -1px;\r\n              cursor: pointer;\r\n            }\r\n\r\n            .tabs li{\r\n              float: left;\r\n            }\r\n\r\n          .tabs [id^=tab]:checked + label{\r\n              background: #1aac9b;\r\n              color: #fff;\r\n            }\r\n\r\n           .tabs [id^=tab]:checked ~ [id^=tab-content] {\r\n                  display: block;\r\n            }\r\n            \r\n           .tabs .tab-content{\r\n                display: none;\r\n                text-align: left;\r\n                width: 100%;\r\n                line-height: 140%;\r\n                padding-top: 10px;\r\n                padding: 11px;\r\n                left: 0;\r\n                position: absolute;\r\n                border: 1px solid #B2DFEE;\r\n                margin: -1px;\r\n                min-height: 150px;\r\n              }\r\n\r\n            \r\n            .tab-data label{\r\n              border: none;\r\n              background: #fff;\r\n              display: inline-block;\r\n              width: 170px;\r\n              padding: 0;\r\n              margin: 0;\r\n              font-weight: normal;\r\n            }\r\n\r\n            .tab-data input, .tab-data select{\r\n              width: 140px;\r\n              font-size: 10pt;\r\n            }\r\n\r\n            .tab-data p {\r\n              margin: 3px;\r\n            }\r\n\r\n            .tab-data-I {\r\n              float: left;\r\n            }\r\n            .tab-data-II {\r\n              float: right;\r\n            }\r\n\r\n            .tab-data-II label {\r\n              width: 300px;\r\n            }\r\n\r\n             \r\n            .rd-tab label{\r\n             width: 60px;\r\n            }\r\n\r\n            .rd-tab input{\r\n             width: 60px;\r\n             margin-top: 0px;\r\n            }\r\n\r\n            .last-details{\r\n              float: none;\r\n              margin-top: 24%;\r\n            }\r\n\r\n            .rd-tab1 input{\r\n             width: 15px !important;\r\n            }\r\n\r\n            &lt;/style&gt;\r\n            &lt;script type=\"text/javascript\"&gt;\r\n              beforeSubmit.push(function() {\r\n\r\n                  var sifilisPartner = getValue(\'sifilisPartner.value\');\r\n                  var testPartner = getValue(\'testPartner.value\');\r\n                  var partner = getValue(\'partner.value\');     \r\n\r\n                  if ((sifilisPartner != \'\' || testPartner != \'\') &amp;amp;&amp;amp; partner == \'\') {\r\n                      getField(\'partner.error\').html(\'obrigatório\').show();\r\n                      return false;\r\n                  }\r\n\r\n                  // var lowWeight = getValue(\'lowWeight.value\');\r\n                  // var brachialPerimeter = getValue(\'brachialPerimeter.value\'); \r\n\r\n                  // if(lowWeight == \"1066\" || brachialPerimeter == \"6371\" || brachialPerimeter == \"6372\"){\r\n                  //   getField(\'cured.error\').html(\'obrigatório\').show();\r\n                  //   return false;\r\n                  // }\r\n\r\n                  var diagnosticITS = getValue(\"diagnosticITS.value\");\r\n                  var itsTreatment = getValue(\'itsTreatment.value\')\r\n\r\n                  if ((diagnosticITS == \"864\" || diagnosticITS == \"5993\") &amp;amp;&amp;amp; itsTreatment == \'\') {\r\n                    getField(\'itsTreatment.error\').html(\'obrigatório\').show();\r\n                    return false;\r\n                  }\r\n\r\n                  var consult = getValue(\'consult.value\');\r\n                  var ageRange = getValue(\'ageRange.value\');\r\n                  var moreThan12weeks = getValue(\'moreThan12weeks.value\');\r\n\r\n                  if (consult === \"6355\" &amp;amp;&amp;amp; (ageRange === \'\' || moreThan12weeks === \'\')) {\r\n                    getField(\"ageRange.error\").html(\"obrigatório\").show();\r\n                    getField(\"moreThan12weeks.error\").html(\"obrigatório\").show();\r\n                    return false;\r\n                  }\r\n\r\n                  var pregnantWeeks = getValue(\'pregnantWeeks.value\');\r\n                  if(pregnantWeeks &gt; 42){\r\n                    getField(\"pregnantWeeks.error\").html(\"o valor não pode ser supererior que 42\").show();\r\n                    return false;\r\n                  }\r\n\r\n                  var weight = getValue(\'weight.value\');\r\n                  if(20 &gt; weight &amp;amp;&amp;amp; weight != 0){\r\n                    getField(\"weight.error\").html(\"peso invalido (20-180 kg)\").show();\r\n                    return false;\r\n                  }\r\n\r\n                  if(weight &gt; 180 &amp;amp;&amp;amp; weight != 0){\r\n                    getField(\"weight.error\").html(\"peso invalido (20-180 kg)\").show();\r\n                    return false;\r\n                  }\r\n\r\n                  // var lastConsult = parseInt(\"&lt;lookup expression=\"fn.latestObs(\'6361\').valueCoded\"/&gt;\");\r\n\r\n                  // if(consult == lastConsult){\r\n                  //   getField(\"consult.error\").html(\"Consulta já existente\").show();\r\n                  //   return false;\r\n                  // }\r\n\r\n                  var startDateTB = new Date(getValue(\'startDateTB.value\'));\r\n                  var endDateTB = new Date(getValue(\'endDateTB.value\'));\r\n\r\n                  if(startDateTB &gt; endDateTB){\r\n                    getField(\"endDateTB.error\").html(\"A data de fim não pode ser inferior a de inicio\").show();\r\n                    return false;\r\n                  }\r\n\r\n                  return true;\r\n              });\r\n\r\n             // consult validator\r\n             jQuery(document).ready(function(){\r\n\r\n                $j(\"#prophilaxysNVP input\").attr(\'disabled\',false);\r\n                var startARV = parseInt(\"&lt;lookup complexExpression=\"#foreach($obs in $fn.allObs(1504)) #if($obs.valueCoded == \'631\') $obs.valueCoded #end #end\"/&gt;\");\r\n                \r\n                if(startARV === 631){\r\n                  $j(\"#prophilaxysNVP input\").attr(\'disabled\',true);\r\n                }\r\n\r\n                $j(\"#prophilaxysAZTNVP input\").attr(\'disabled\',false);\r\n                var nvpAzt = parseInt(\"&lt;lookup complexExpression=\"#foreach($obs in $fn.allObs(1504)) #if($obs.valueCoded == \'1801\') $obs.valueCoded #end #end\"/&gt;\");\r\n                \r\n                if(nvpAzt === 1801){\r\n                  $j(\"#prophilaxysAZTNVP input\").attr(\'disabled\',true);\r\n                }\r\n\r\n                getField(\'consult.value\').live(\'change\', function() {\r\n\r\n                  $j(\"#ageRange select\").attr(\'disabled\',false);\r\n                  $j(\"#moreThan12weeks input:radio\").attr(\'disabled\', false);\r\n                  $j(\"#seroStatus select\").attr(\'disabled\', false);\r\n\r\n                  $j(\"#cured input:radio\").attr(\'disabled\', false);\r\n                  $j(\"#lowWeight input:radio\").attr(\'disabled\', false);\r\n                  $j(\"#abandon input:radio\").attr(\'disabled\', false);\r\n                  $j(\"#prophilaxysARVFOLLOW input\").attr(\'disabled\', false);\r\n\r\n                  if(getValue(\"consult.value\") == \"6355\"){\r\n                    $j(\"#cured input:radio\").attr(\'disabled\', true);\r\n                    $j(\"#lowWeight input:radio\").attr(\'disabled\', true);\r\n                    $j(\"#abandon input:radio\").attr(\'disabled\', true);\r\n                    $j(\"#prophilaxysARVFOLLOW input\").attr(\'disabled\', true);\r\n                  }\r\n\r\n                  if (getValue(\'consult.value\') != \'6355\') {\r\n                    $j(\"#ageRange select\").attr(\'disabled\',true);\r\n                    $j(\"#moreThan12weeks input:radio\").attr(\'disabled\', true);\r\n                    $j(\"#seroStatus select\").attr(\'disabled\', true);\r\n                  }\r\n                  \r\n                });\r\n             \r\n                //serostatus validator\r\n                getField(\'seroStatus.value\').live(\'change\', function(){\r\n                    $j(\"#hivTestCPN select\").attr(\'disabled\', false);\r\n\r\n                    var seroStatus = getValue(\'seroStatus.value\');\r\n          \r\n                    if (seroStatus == \"703\") {\r\n                      $j(\"#hivTestCPN select\").attr(\'disabled\', true);\r\n                    }\r\n                });\r\n\r\n                // validate HIV status if partner present\r\n                $j(\"#testPartner select\").attr(\'disabled\',true);\r\n\r\n                $j(\'#partner input[type=\"radio\"]\').on(\'click change\', function(e) {                 \r\n                    var yesValue = $j(\'#partner input[type=\"radio\"]:checked\').val();\r\n\r\n                    if(yesValue === \'1065\'){\r\n                       $j(\"#testPartner select\").attr(\'disabled\',false);\r\n                       return;\r\n                    }\r\n                    \r\n                    $j(\"#testPartner select\").attr(\'disabled\',true);\r\n                });\r\n\r\n                //validate woman test\r\n                $j(\'#hivTestCPN select\').on(\'change\', function(e) {                 \r\n                    var value =  getValue(\'hivTestCPN.value\');\r\n                    console.log(value);\r\n                    if(value === \'664\'){\r\n                      $j(\"#prophilaxysCZT select\").attr(\'disabled\',true);\r\n                      $j(\"#prophilaxysARV select\").attr(\'disabled\',true);\r\n                      return;\r\n                    }\r\n\r\n                    $j(\"#prophilaxysCZT select\").attr(\'disabled\',false);\r\n                    $j(\"#prophilaxysARV select\").attr(\'disabled\',false);\r\n                });\r\n\r\n                $j(\'#sifilisTest select\').on(\'change\', function(e) {                 \r\n                    var value =  getValue(\'sifilisTest.value\');\r\n\r\n                    if(value === \'1228\'){\r\n                      $j(\"#womanSifilisTest select\").attr(\'disabled\',false);\r\n                      return;\r\n                    }\r\n\r\n                    $j(\"#womanSifilisTest select\").attr(\'disabled\',true);\r\n                });\r\n\r\n               $j(\'#pregnantWeeks\').change(function(){\r\n                  var pregnantWeeks = getValue(\'pregnantWeeks.value\');\r\n                  $j(\"#prophilaxysAZTNVP input\").attr(\'disabled\',false);\r\n\r\n                  if(pregnantWeeks &amp;lt; 14){\r\n                     $j(\"#prophilaxysAZTNVP input\").attr(\'disabled\',true);\r\n                    return;\r\n                  }\r\n                });\r\n\r\n               //Validate sal ferouse\r\n                $j(\'#ferouseOpt input[type=\"radio\"]\').on(\'click change\', function(e) {    \r\n                    var yesValue = $j(\'#ferouseOpt input[type=\"radio\"]:checked\').val();\r\n\r\n                    if(yesValue === \'1066\'){\r\n                       $j(\"#ferouseQtd input\").attr(\'disabled\',true);\r\n                       return;\r\n                    }\r\n                    \r\n                    $j(\"#ferouseQtd input\").attr(\'disabled\',false);\r\n                });\r\n\r\n             });\r\n            &lt;/script&gt;  \r\n        &lt;/head&gt;\r\n\r\n        &lt;body&gt;\r\n        \r\n        &lt;div class=\"header-box content\"&gt;\r\n            &lt;h2&gt;LIVRO DE REGISTOS DE CONSULTA PRÉ-NATAL&lt;/h2&gt;\r\n          &lt;/div&gt;\r\n\r\n        &lt;div class=\"header content\"&gt;\r\n          &lt;div class=\"header-info\"&gt;\r\n            &lt;h3&gt;REPÚBLICA DE MOÇAMBIQUE&lt;/h3&gt;\r\n            &lt;h3&gt;SERVIÇO NACIONAL DE SAÚDE&lt;/h3&gt;\r\n            &lt;h3&gt;MOD - SIS - B01&lt;/h3&gt;\r\n            &lt;p&gt;\r\n              &lt;label&gt;NID/US:&lt;/label&gt;\r\n            &lt;/p&gt;\r\n            &lt;p&gt;\r\n              &lt;label&gt;NID/HDD:&lt;/label&gt;\r\n              &lt;lookup expression=\"patient.getPatientIdentifier(2)\"/&gt;\r\n            &lt;/p&gt;\r\n          &lt;/div&gt;\r\n          &lt;div class=\"header-data\"&gt;\r\n            &lt;p&gt;\r\n              &lt;label&gt;Nome:&lt;/label&gt;\r\n              &lt;lookup expression=\"patient.personName\"/&gt;\r\n            &lt;/p&gt;\r\n            &lt;p&gt;\r\n              &lt;label&gt;Sexo/Data de Nasc./Idade:&lt;/label&gt;\r\n              &lt;lookup expression=\"patient.gender\"/&gt; - &lt;lookup expression=\"patient.birthdate\"/&gt; - &lt;lookup expression=\"patient.age\"/&gt;\r\n            &lt;/p&gt;\r\n            &lt;p&gt;\r\n              &lt;label&gt;Nº de BI/Outra identificação:&lt;/label&gt;\r\n              &lt;lookup expression=\"patient.getPatientIdentifier(3)\"/&gt;/&lt;lookup expression=\"patient.getPatientIdentifier(1)\"/&gt;\r\n            &lt;/p&gt;\r\n            &lt;p&gt;\r\n              &lt;label&gt;Distrito/Cidade:&lt;/label&gt;\r\n              &lt;lookup complexExpression=\"#foreach( $addr in $patient.addresses ) $!addr.countyDistrict #end\"/&gt;\r\n            &lt;/p&gt;\r\n            &lt;p&gt;\r\n              &lt;label&gt;Localidade/Bairro:&lt;/label&gt;\r\n              &lt;lookup complexExpression=\"#foreach( $addr in $patient.addresses ) $!addr.region #end\"/&gt;/&lt;lookup complexExpression=\"#foreach( $addr in $patient.addresses ) $!addr.subregion #end\"/&gt;\r\n            &lt;/p&gt;\r\n            &lt;p&gt;\r\n              &lt;label&gt;Célula/Quarteirão:&lt;/label&gt;\r\n              &lt;lookup complexExpression=\"#foreach( $addr in $patient.addresses ) $!addr.neighborhoodCell #end\"/&gt;\r\n            &lt;/p&gt;\r\n            &lt;p&gt;\r\n              &lt;label&gt;Avenida/Rua/Casa:&lt;/label&gt;\r\n              &lt;lookup complexExpression=\"#foreach( $addr in $patient.addresses ) $!addr.address1 #end\"/&gt;\r\n            &lt;/p&gt;\r\n          &lt;/div&gt;\r\n         \r\n          &lt;div class=\"clear\"/&gt;\r\n          &lt;label &gt;Pessoa de Referência:&lt;/label&gt;&lt;br/&gt;\r\n          &lt;obsgroup groupingConceptId=\"1609\"&gt;\r\n            &lt;obs conceptId=\"1441\" labelText=\"Nome:\" size=\"20\"/&gt; \r\n            &lt;obs conceptId=\"1442\" labelText=\"Apelido:\" size=\"20\"/&gt; \r\n            &lt;obs conceptId=\"1611\" labelText=\"Tel:\" size=\"15\" maxlength=\"9\"/&gt;\r\n          &lt;/obsgroup&gt;\r\n          &lt;p&gt;\r\n            &lt;label&gt;Unidade Sanitária:&lt;/label&gt;&lt;br/&gt;\r\n            \r\n&lt;encounterLocation id=\"localConsulta\" /&gt;\r\n          &lt;/p&gt;\r\n          &lt;p&gt;\r\n            &lt;obs conceptId=\"a26e8692-d65c-47c7-9284-8e78eb86802f\" labelText=\"Número do Livro:\" size=\"20\"/&gt; |==|\r\n            &lt;obs conceptId=\"9fdb2c0b-e33a-42c1-9ade-6c57c702c284\" labelText=\"Número da página:\" size=\"20\" /&gt;\r\n          &lt;/p&gt;\r\n        &lt;/div&gt;\r\n         &lt;div class=\"content\"&gt;\r\n            &lt;div class=\"demo-data demo-data-partI\"&gt;\r\n              &lt;p&gt;\r\n                &lt;label&gt;Data da consulta:&lt;/label&gt;\r\n                &lt;encounterDate id=\"dataConsulta\"/&gt;\r\n              &lt;/p&gt;\r\n              &lt;p&gt;\r\n                &lt;label&gt;Consultas:&lt;/label&gt;\r\n                &lt;obs conceptId=\"6361\" id=\"consult\" answerConceptIds=\"6355,6356,6357,6358,6359,6360\" answerLabels=\"1ª,2ª,3ª,4ª,5ª,6ª\"/&gt;\r\n              &lt;/p&gt;\r\n              &lt;p&gt;\r\n                &lt;label&gt;Faixa Etária:&lt;/label&gt;\r\n                &lt;obs conceptId=\"6366\" id=\"ageRange\" answerConceptIds=\"6362,6363,6364,6365\" answerLabels=\"10-14,15-19,20-24,25+\"/&gt;\r\n              &lt;/p&gt;\r\n              &lt;p&gt;\r\n                &lt;label&gt;Data da última mestruação:&lt;/label&gt;\r\n                &lt;obs conceptId=\"e1dc0dd0-1d5f-11e0-b929-000c29ad1d07\" /&gt;\r\n              &lt;/p&gt;\r\n            &lt;/div&gt;\r\n            &lt;div class=\"demo-data demo-data-partII\"&gt;\r\n              &lt;p&gt;\r\n                &lt;label&gt;Idade Gestacional (em semanas):&lt;/label&gt;\r\n                &lt;obs conceptId=\"1279\" size=\"10\" required=\"true\" id=\"pregnantWeeks\"/&gt; \r\n              &lt;/p&gt;\r\n              &lt;p id=\"rdp\"&gt;\r\n                &lt;label id=\"rdpI\"&gt; &amp;lt;12 semanas:&lt;/label&gt;\r\n                &lt;obs conceptId=\"6367\" id=\"moreThan12weeks\" answerConceptIds=\"1065,1066\" answerLabels=\"Sim, Não\" style=\"radio\"/&gt;\r\n              &lt;/p&gt;\r\n              &lt;p id=\"rdp\"&gt;\r\n                &lt;label id=\"rdpI\"&gt;Parceiro Presente ?&lt;/label&gt;\r\n                &lt;obs conceptId=\"6368\" id=\"partner\" answerConceptIds=\"1065,1066\" answerLabels=\"Sim, Não\" style=\"radio\"/&gt;\r\n              &lt;/p&gt;\r\n              &lt;p&gt;\r\n                &lt;label id=\"rdpI\"&gt;Data provável do parto:&lt;/label&gt;\r\n                &lt;obs conceptId=\"e1e76284-1d5f-11e0-b929-000c29ad1d07\" size=\"10\"/&gt;\r\n              &lt;/p&gt;\r\n            &lt;/div&gt;\r\n            &lt;div class=\"clear\" /&gt;\r\n            &lt;div class=\"tabs\"&gt;\r\n              &lt;ul&gt;\r\n                &lt;li&gt;\r\n                  &lt;input type=\"radio\" checked=\"true\" name=\"tabs\" id=\"tab1\" class=\"rd-visible\" /&gt;\r\n                  &lt;label for=\"tab1\"&gt;Nutrição&lt;/label&gt;\r\n                  &lt;div id=\"tab-content-I\" class=\"tab-content\"&gt;\r\n                    &lt;div class=\"tab-data tab-data-I\"&gt;\r\n                      &lt;p&gt;\r\n                        &lt;label&gt;Peso(KG):&lt;/label&gt;\r\n                         &lt;obs conceptId=\"5089\" size=\"10\" id=\"weight\"/&gt;\r\n                      &lt;/p&gt;\r\n                      &lt;p&gt;\r\n                        &lt;label&gt;Perímetro Braquial:&lt;/label&gt;\r\n                         &lt;obs conceptId=\"6373\" id=\"brachialPerimeter\" answerConceptIds=\"6370,6371,6372\" answerLabels=\"˂21 cm (DAG), menor ou igual a 21cm e menor que 23 cm (DAM)s, &amp;gt;23 cm (normal)\"/&gt;\r\n                      &lt;/p&gt;\r\n                    &lt;/div&gt;\r\n                    &lt;div class=\"tab-data tab-data-II\"&gt;\r\n                     &lt;p &gt;\r\n                        &lt;label&gt;Ganho ≥1.5 Kg/mês a partir 2º trimestre ?&lt;/label&gt;\r\n                        &lt;obs conceptId=\"6369\" id=\"lowWeight\" answerConceptIds=\"1065,1066\" answerLabels=\"Sim, Não\" style=\"radio\" class=\"rd-tab\"/&gt;\r\n                     &lt;/p&gt;\r\n                     &lt;p&gt;\r\n                        &lt;label&gt;Recebeu suplementos nutricionais ?&lt;/label&gt;\r\n                        &lt;obs conceptId=\"2152\" answerConceptIds=\"1065,1066\" answerLabels=\"Sim, Não\" style=\"radio\" class=\"rd-tab\"/&gt;\r\n                     &lt;/p&gt;\r\n                     &lt;p&gt;\r\n                        &lt;label&gt;Suplementos nutricionais:&lt;/label&gt;\r\n                        &lt;obs conceptId=\"e1e205f0-1d5f-11e0-b929-000c29ad1d07\" class=\"rd-tab\"/&gt;\r\n                     &lt;/p&gt;\r\n                      &lt;p &gt;\r\n                        &lt;label&gt;Recebeu desparasitante ?&lt;/label&gt;\r\n                        &lt;obs conceptId=\"6377\" answerConceptIds=\"1065,1066\" answerLabels=\"Sim, Não\" style=\"radio\" class=\"rd-tab\"/&gt;\r\n                     &lt;/p&gt;\r\n                     &lt;p&gt;\r\n                        &lt;label&gt;Sal Ferroso com Ácido Fólico?&lt;/label&gt;\r\n                        &lt;obs conceptId=\"6378\" id=\"ferouseOpt\" answerConceptIds=\"1065,1066\" answerLabels=\"Sim, Não\" style=\"radio\" class=\"rd-tab\"/&gt;\r\n                     &lt;/p&gt;\r\n                     &lt;p&gt;\r\n                        &lt;label&gt;Quantidade de Sal Ferroso&lt;/label&gt;\r\n                        &lt;obs conceptId=\"35fba30b-a7da-4f39-a7e0-2cef36a06348\" id=\"ferouseQtd\" class=\"rd-tab\"/&gt;\r\n                     &lt;/p&gt;\r\n                    &lt;/div&gt;\r\n                    &lt;div class=\"clear\" /&gt;\r\n                    &lt;div class=\"tab-data tab-data-I\"&gt;\r\n                      &lt;p&gt;\r\n                        &lt;label style=\"font-weight:bold; width:150px;\"&gt;Resultado:&lt;/label&gt;\r\n                      &lt;/p&gt;\r\n                      &lt;p &gt;\r\n                        &lt;label&gt;Curado ?&lt;/label&gt;\r\n                        &lt;obs conceptId=\"6375\" id=\"cured\" answerConceptIds=\"1065,1066\" answerLabels=\"Sim, Não\" style=\"radio\" class=\"rd-tab\"/&gt;\r\n                      &lt;/p&gt;\r\n                      &lt;p&gt;\r\n                        &lt;label&gt;Abandono ?&lt;/label&gt;\r\n                        &lt;obs conceptId=\"6376\" id=\"abandon\" answerConceptIds=\"1065,1066\" answerLabels=\"Sim, Não\" style=\"radio\" class=\"rd-tab\"/&gt;\r\n                      &lt;/p&gt;\r\n                    &lt;/div&gt;\r\n                  &lt;/div&gt;\r\n                &lt;/li&gt;\r\n                &lt;li&gt;\r\n                  &lt;input type=\"radio\" name=\"tabs\" id=\"tab2\" class=\"rd-visible\" /&gt;\r\n                  &lt;label for=\"tab2\"&gt;Exames&lt;/label&gt;\r\n                  &lt;div id=\"tab-content-II\" class=\"tab-content\"&gt;\r\n                    &lt;div class=\"tab-data tab-data-I\"&gt;\r\n                      &lt;p&gt;\r\n                        &lt;label&gt;Tensão Arterial (TA ≥ 140/90mmHg) ?&lt;/label&gt;\r\n                        &lt;obs conceptId=\"6379\" required=\"true\" answerConceptIds=\"1065,1066,1118\" answerLabels=\"Sim, Não, Não Fez\"/&gt;\r\n                      &lt;/p&gt;\r\n                      &lt;p&gt;\r\n                        &lt;label&gt;Hemoglobina (HGB ˂11g/dL)?&lt;/label&gt;\r\n                        &lt;obs conceptId=\"6380\" answerConceptIds=\"1065,1066,1118\" answerLabels=\"Sim, Não, Não Fez\"/&gt;\r\n                      &lt;/p&gt;\r\n                       &lt;p&gt;\r\n                        &lt;label&gt;Proteinúria ?&lt;/label&gt;\r\n                        &lt;obs conceptId=\"6381\" answerConceptIds=\"1065,1066,1118\" answerLabels=\"Sim, Não, Não Fez\"/&gt;\r\n                      &lt;/p&gt;\r\n                       &lt;p&gt;\r\n                        &lt;label&gt;Glicosúria ?&lt;/label&gt;\r\n                        &lt;obs conceptId=\"6382\" answerConceptIds=\"1065,1066,1118\" answerLabels=\"Sim, Não, Não Fez\"/&gt;\r\n                      &lt;/p&gt;\r\n                    &lt;/div&gt;\r\n                  &lt;/div&gt;\r\n                &lt;/li&gt;\r\n                &lt;li&gt;\r\n                  &lt;input type=\"radio\" name=\"tabs\" id=\"tab3\" class=\"rd-visible\"/&gt;\r\n                  &lt;label for=\"tab3\"&gt;Sífilis e outras ITS\'s&lt;/label&gt;\r\n                  &lt;div id=\"tab-content-III\" class=\"tab-content\"&gt;\r\n                    &lt;div class=\"tab-data tab-data-I\"&gt;\r\n                      &lt;p&gt;\r\n                        &lt;label style=\"font-weight:bold; width:150px;\"&gt;Diagnóstico de ITS&lt;/label&gt;\r\n                      &lt;/p&gt;\r\n                      &lt;p&gt;\r\n                        &lt;obs conceptId=\"1080\" answerConceptId=\"864\" style=\"checkbox\" answerLabel=\"Ulceras Genitais\"/&gt;\r\n                      &lt;/p&gt;\r\n                      &lt;p&gt;\r\n                        &lt;obs conceptId=\"1080\" answerConceptId=\"5993\" style=\"checkbox\" answerLabel=\"Leucorreias\" /&gt;\r\n                      &lt;/p&gt;\r\n                      &lt;p&gt;\r\n                        &lt;label&gt;Teste de Sífilis:&lt;/label&gt;\r\n                        &lt;obs conceptId=\"299\" id=\"sifilisTest\" answerConceptIds=\"1228,1229,1118\" answerLabels=\"Positivo, Negativo, Não Feito\"/&gt;\r\n                      &lt;/p&gt;\r\n                    &lt;/div&gt;\r\n                    &lt;div class=\"tab-data tab-data-II\"&gt;\r\n                     &lt;p &gt;\r\n                        &lt;label&gt;Tratamento Sindrómico de ITS ?&lt;/label&gt;\r\n                        &lt;obs conceptId=\"1975\" id=\"itsTreatment\" answerConceptIds=\"1065,1066\" answerLabels=\"Sim, Não\" style=\"radio\" class=\"rd-tab\"/&gt;\r\n                     &lt;/p&gt;\r\n                    &lt;/div&gt;\r\n                    &lt;div class=\"clear\" /&gt;\r\n                    &lt;br/&gt;\r\n                    &lt;div class=\"tab-data tab-data-I\"&gt;\r\n                      &lt;p&gt;\r\n                        &lt;label style=\"font-weight:bold; width:150px;\"&gt;Tratamento para Sífilis:&lt;/label&gt;\r\n                      &lt;/p&gt;\r\n                      &lt;p &gt;\r\n                        &lt;label&gt;Mulher ?&lt;/label&gt;\r\n                        &lt;obs conceptId=\"6383\" id=\"womanSifilisTest\" answerConceptIds=\"1182,2084\" answerLabels=\"1ª dose,3ª dose\"/&gt;\r\n                      &lt;/p&gt;\r\n                      &lt;p&gt;\r\n                        &lt;label&gt;Parceiro ?&lt;/label&gt;\r\n                        &lt;obs conceptId=\"6384\" id=\"sifilisPartner\" answerConceptIds=\"1065,1066,1118\" answerLabels=\"Sim, Não, Não Feito\" /&gt;\r\n                      &lt;/p&gt;\r\n                    &lt;/div&gt;\r\n                  &lt;/div&gt;\r\n                &lt;/li&gt;\r\n                 &lt;li&gt;\r\n                  &lt;input type=\"radio\" name=\"tabs\" id=\"tab4\" class=\"rd-visible\"/&gt;\r\n                  &lt;label for=\"tab4\"&gt;PTV de HIV&lt;/label&gt;\r\n                  &lt;div id=\"tab-content-IV\" class=\"tab-content\"&gt;\r\n                    &lt;div class=\"tab-data tab-data-I\"&gt;\r\n                      &lt;p&gt;\r\n                        &lt;label&gt;Seroestado entrada a 1ª CPN:&lt;/label&gt;\r\n                        &lt;obs conceptId=\"6385\" id=\"seroStatus\" answerConceptIds=\"664,703,1067\" answerLabels=\"Negativo, Positivo, Desconhecido\"/&gt;\r\n                      &lt;/p&gt;\r\n                      &lt;p&gt;\r\n                        &lt;label&gt;Teste de HIV na CPN:&lt;/label&gt;\r\n                        &lt;obs conceptId=\"2079\" id=\"hivTestCPN\" answerConceptIds=\"664,703,1138,1118\" answerLabels=\"Negativo, Positivo, Ideterminado, Não Feito\"/&gt;\r\n                      &lt;/p&gt;\r\n                      &lt;p&gt;\r\n                        &lt;label&gt;Teste do Parceiro:&lt;/label&gt;\r\n                        &lt;obs conceptId=\"2074\" id=\"testPartner\" answerConceptIds=\"664,703,1138,1118\" answerLabels=\"Negativo, Positivo, Ideterminado, Não Feito\"/&gt;\r\n                      &lt;/p&gt;\r\n                    &lt;/div&gt;\r\n                    &lt;div class=\"tab-data tab-data-II\"&gt;\r\n                      &lt;p&gt;\r\n                        &lt;label style=\"font-weight:bold; width:150px;\"&gt;Profilaxias:&lt;/label&gt;\r\n                      &lt;/p&gt;\r\n                      &lt;p&gt;\r\n                        &lt;obs conceptId=\"6121\" id=\"prophilaxysCZT\" answerConceptId=\"6386\" answerLabel=\"Em CTZ a entrada\" style=\"checkbox\"/&gt;\r\n                      &lt;/p&gt;\r\n                      &lt;p&gt;\r\n                        &lt;label&gt;Profilaxia CTZ:&lt;/label&gt;\r\n                        &lt;obs conceptId=\"6121\" id=\"prophilaxysCZT\" answerConceptIds=\"1256,1257\" answerLabels=\"Início, Continuação\"/&gt;\r\n                      &lt;/p&gt;\r\n\r\n                      &lt;p&gt;\r\n                        &lt;obs conceptId=\"1504\" id=\"prophilaxysARV\" answerConceptId=\"6388\" answerLabel=\"Em TARV a entrada\" style=\"checkbox\" /&gt;\r\n                      &lt;/p&gt;\r\n\r\n                      &lt;p&gt;\r\n                        &lt;obs conceptId=\"1504\" id=\"prophilaxysNVP\" answerConceptId=\"631\" answerLabel=\"Entrega de Monoprofilaxia (NVP) nesta visita\" style=\"checkbox\"/&gt;\r\n                      &lt;/p&gt;\r\n\r\n                      &lt;p&gt;\r\n                        &lt;obs conceptId=\"1504\" id=\"prophilaxysAZTNVP\" answerConceptId=\"1801\" answerLabel=\"Inicia biprofilaxia (AZT+NVP) nesta visita\" style=\"checkbox\"/&gt;\r\n                      &lt;/p&gt;\r\n\r\n                      &lt;p&gt;\r\n                        &lt;obs conceptId=\"1504\" id=\"prophilaxysARVSTART\" answerConceptId=\"1256\" answerLabel=\"Inicia o TARV nesta visita\" style=\"checkbox\" /&gt;\r\n                      &lt;/p&gt;\r\n\r\n                      &lt;p&gt;\r\n                        &lt;obs conceptId=\"1504\" id=\"prophilaxysARVFOLLOW\" answerConceptId=\"1257\" answerLabel=\"Continua ARV nesta visita\" style=\"checkbox\" /&gt;\r\n                      &lt;/p&gt;\r\n\r\n                    &lt;/div&gt;\r\n                  &lt;/div&gt;\r\n                &lt;/li&gt;\r\n                 &lt;li&gt;\r\n                  &lt;input type=\"radio\" name=\"tabs\" id=\"tab5\" class=\"rd-visible\"/&gt;\r\n                  &lt;label for=\"tab5\"&gt;Malaria&lt;/label&gt;\r\n                  &lt;div id=\"tab-content-V\" class=\"tab-content\"&gt;\r\n                    &lt;div class=\"tab-data tab-data-I\"&gt;\r\n                      &lt;p&gt;\r\n                        &lt;label&gt;Prevenção da Malária (TIP) :&lt;/label&gt;\r\n                        &lt;obs conceptId=\"6389\" answerConceptIds=\"1182,1183,2084,2085\" answerLabels=\"1ª, 2ª, 3ª, 4ª+\"/&gt;\r\n                      &lt;/p&gt;\r\n                    &lt;/div&gt;\r\n                    &lt;div class=\"tab-data tab-data-II\"&gt;\r\n                      &lt;p &gt;\r\n                        &lt;label&gt;Recebeu Rede Mosquiteira?&lt;/label&gt;\r\n                        &lt;obs conceptId=\"1863\" answerConceptIds=\"1065,1066\" answerLabels=\"Sim, Não\" style = \"radio\" class=\"rd-tab\"/&gt;\r\n                      &lt;/p&gt;\r\n                      &lt;p &gt;\r\n                        &lt;label&gt;Testadas para Malaria:&lt;/label&gt;\r\n                        &lt;obs conceptId=\"6392\" answerConceptIds=\"6390,6391\" answerLabels=\"HTZ, TDR\" style = \"radio\" class=\"rd-tab\"/&gt;\r\n                      &lt;/p&gt;\r\n                    &lt;/div&gt;\r\n                    &lt;div class=\"clear\" /&gt;\r\n                    &lt;br/&gt;\r\n                    &lt;div class=\"tab-data tab-data-I\"&gt;\r\n                      &lt;p&gt;\r\n                        &lt;label style=\"font-weight:bold; width:250px;\"&gt;Diagnóstico e Tratamento de Malária:&lt;/label&gt;\r\n                      &lt;/p&gt;\r\n                      &lt;p &gt;\r\n                        &lt;label&gt;Resultado TDR ou HTZ:&lt;/label&gt;\r\n                        &lt;obs conceptId=\"32\" answerConceptIds=\"664,703,1138,1118\" answerLabels=\"Negativo, Positivo, Indeterminado, Não Feito\"/&gt;\r\n                      &lt;/p&gt;\r\n                      &lt;p&gt;\r\n                        &lt;label&gt;Mulheres com teste de Malária Positivo e Tratadas:&lt;/label&gt;\r\n                        &lt;obs conceptId=\"6393\" answerConceptIds=\"1065,1066,1364\" answerLabels=\"Sim, Não, Não elegivel\" /&gt;\r\n                      &lt;/p&gt;\r\n                    &lt;/div&gt;\r\n                  &lt;/div&gt;\r\n                &lt;/li&gt;\r\n                &lt;li&gt;\r\n                  &lt;input type=\"radio\" name=\"tabs\" id=\"tab6\" class=\"rd-visible\"/&gt;\r\n                  &lt;label for=\"tab6\"&gt;HPP e VAT&lt;/label&gt;\r\n                  &lt;div id=\"tab-content-VI\" class=\"tab-content\"&gt;\r\n                    &lt;div class=\"tab-data tab-data-I\"&gt;\r\n                     &lt;p &gt;\r\n                      &lt;label&gt;Recebeu Misoprostol?&lt;/label&gt;\r\n                      &lt;obs conceptId=\"6351\" answerConceptIds=\"1065,1066\" answerLabels=\"Sim, Não\" style=\"radio\" class=\"rd-tab rd-tab1\"/&gt;\r\n                    &lt;/p&gt;\r\n                    &lt;p&gt;\r\n                      &lt;label&gt;VAT:&lt;/label&gt;\r\n                      &lt;obs conceptId=\"54\" answerConceptIds=\"1182,1184, 1118\" answerLabels=\"1ª dose,</t>
   </si>
   <si>
     <t>7d8a6c2e-6398-49ab-aa22-3125718013b8</t>
@@ -2596,7 +2596,7 @@
       <c r="B41" s="1">
         <v>159.0</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D41" s="6" t="s">
         <v>92</v>
       </c>
       <c r="E41" s="1">

</xml_diff>

<commit_message>
added metadata introduced in release 3.4.0
</commit_message>
<xml_diff>
--- a/api/src/main/resources/all-htmlformentry_html_form_13072020.xlsx
+++ b/api/src/main/resources/all-htmlformentry_html_form_13072020.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowHeight="29730" tabRatio="500"/>
+    <workbookView windowWidth="27195" windowHeight="13125" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="htmlformentry_html_form" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
   <si>
     <t>id</t>
   </si>
@@ -102,7 +102,7 @@
     <t>68d88215-7b9e-4eeb-a452-cebccd7b7933</t>
   </si>
   <si>
-    <t>&lt;htmlform&gt;  &lt;html xmlns="http://www.w3.org/1999/xhtml"&gt; &lt;head&gt; &lt;meta http-equiv="Content-Type" content="text/html; charset=utf-8" /&gt; &lt;title&gt;FICHA DE LABORATÓRIO&lt;/title&gt; &lt;style&gt;    h2 { border-bottom: 3px solid red; }    p { border: 1px solid black; }    table{     border-color: #600;     border-width: 0 0 1px 1px;     border-style: solid;}     td{     border-color: #600;     border-width: 1px 1px 0 0;     border-style: solid;     margin: 0;     padding: 4px;     background-color: #B2DFEE;}     .style1 {  font-size: 14px;  font-weight: bold;  } &lt;/style&gt; &lt;/head&gt;  &lt;body&gt; &lt;table width="55%" border="1" align="center"&gt; &lt;tbody align="left" style="font-family:verdana; font-size:12px"&gt;   &lt;tr&gt;     &lt;td colspan="3"&gt;&lt;div align="center" class="style1"&gt;FICHA DE LABORATÓRIO&lt;/div&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td colspan="3"&gt;&lt;div align="center"&gt;&lt;strong&gt;PACIENTE&lt;/strong&gt;&lt;/div&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td width="70%"&gt;&lt;div align="right"&gt;Nome&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;lookup expression="patient.personName"/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;sexo&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;lookup expression="patient.gender"/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;NID&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;lookup expression="patient.getPatientIdentifier(2)"/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td colspan="3"&gt;&lt;div align="center"&gt;&lt;strong&gt;EXAME&lt;/strong&gt;&lt;/div&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Data do Pedido&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="6246" labelText=""/&gt;&lt;/td&gt;   &lt;/tr&gt; &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Data da Colheita&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="23821" labelText=""/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Data do Resultado&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;encounterDate/&gt;&lt;/td&gt;       &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Unidade Sanitária&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;encounterLocation id="localConsulta" default="GlobalProperty:default_location" order="5,17,67,68,69,71,90,70,389,408,409" type="autocomplete"/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Técnico&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;encounterProvider role="Provider" type="autocomplete"/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td colspan="3"&gt;&lt;div align="center"&gt;&lt;strong&gt;RESULTADOS&lt;/strong&gt;&lt;/div&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td colspan="3"&gt;&lt;div align="center"&gt;&lt;strong&gt;HEMATOLOGIA&lt;/strong&gt;&lt;/div&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;obsgroup groupingConceptId="1723"&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Globulos Brancos (WBC)&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="678" labelText=""/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Globulos Vermelhos (RBC)&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="679" labelText=""/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Hemoglobina (HGB ou HB)&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="21" labelText=""/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Hematócrito (HCT, PCV)&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="1015" labelText=""/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Volume Corpuscular Médio (HCV, VCM, VGM)&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="851" labelText=""/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Volume Corpuscular Hemoglobina (MCH, HGM, HCM)&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="1018" labelText=""/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Concentração Média de Hemoglobina Corpuscular (MCHC, CHCM, CMHG)&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="1017" labelText=""/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Plaquetas (PLT)&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="729" labelText=""/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Largura de Distribuição de Globulos Vermelhos (RDW)&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="1016" labelText=""/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Velocidade de Sedimentação dos Globulos Vermelhos (VS, VHS)&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="855" labelText=""/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Volume médio de Plaquetas (MPV)&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="1307" labelText=""/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Tipagem Sanguinea&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="300" labelText="" answerConceptIds="690,692,694,696,699,701,1230,1231" answerLabels="A POSITIVO,A NEGATIVO,B POSITIVO, B NEGATIVO,O POSITIVO,O NEGATIVO,AB POSITIVO, AB NEGATIVO"/&gt;&lt;/td&gt;   &lt;/tr&gt;      &lt;tr&gt;     &lt;td&gt;&lt;/td&gt;         &lt;td width="14%"&gt;&lt;strong&gt;Percentual (%)&lt;/strong&gt;&lt;/td&gt;  &lt;td width="13%"&gt;&lt;strong&gt;Absoluto (#)&lt;/strong&gt;&lt;/td&gt;   &lt;/tr&gt;     &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Linfocitos (LYM)&lt;/div&gt;&lt;/td&gt;         &lt;td&gt;&lt;obs conceptId="1021" labelText=""/&gt;&lt;/td&gt;  &lt;td&gt;&lt;obs conceptId="952" labelText=""/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Neutrofilos (NEUT)&lt;/div&gt;&lt;/td&gt;         &lt;td&gt;&lt;obs conceptId="1022" labelText=""/&gt;&lt;/td&gt;  &lt;td&gt;&lt;obs conceptId="1330" labelText=""/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Eosinofilo&lt;/div&gt;&lt;/td&gt;        &lt;td&gt;&lt;obs conceptId="1024" labelText=""/&gt;&lt;/td&gt;   &lt;td&gt;&lt;obs conceptId="1332" labelText=""/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Basofilo&lt;/div&gt;&lt;/td&gt;  &lt;td&gt;&lt;obs conceptId="1025" labelText=""/&gt;&lt;/td&gt;     &lt;td&gt;&lt;obs conceptId="1333" labelText=""/&gt;&lt;/td&gt;       &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Monocito&lt;/div&gt;&lt;/td&gt;     &lt;td&gt;&lt;obs conceptId="1023" labelText=""/&gt;&lt;/td&gt;  &lt;td&gt;&lt;obs conceptId="1331" labelText=""/&gt;&lt;/td&gt;       &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Teste de VDRL&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="299" labelText="" answerConceptIds="1228,1229" answerLabels="Positivo,Negativo" style="radio"/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;/obsgroup&gt;   &lt;obsgroup groupingConceptId="1639"&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;RPR&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="1655" labelText="" answerConceptIds="1228,1229" answerLabels="Positivo,Negativo" style="radio"/&gt;&lt;/td&gt;   &lt;/tr&gt;      &lt;tr&gt;     &lt;td&gt;&lt;/td&gt;     &lt;td&gt;&lt;strong&gt;Absoluto&lt;/strong&gt;&lt;/td&gt;     &lt;td&gt;&lt;strong&gt;Percentual&lt;/strong&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;CD4&lt;/div&gt;&lt;/td&gt;     &lt;td&gt;&lt;obs conceptId="5497" labelText=""/&gt;&lt;/td&gt;     &lt;td&gt;&lt;obs conceptId="730" labelText=""/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;/obsgroup&gt;   &lt;obsgroup groupingConceptId="1632"&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Carga Viral&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="856" labelText=""/&gt;Cópias/ml&lt;br/&gt;&lt;br/&gt; &lt;obs conceptId="1518" labelText=""/&gt;Log&lt;/td&gt;   &lt;/tr&gt;   &lt;/obsgroup&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Baciloscopia&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="307" labelText="" answerConceptIds="703,664" answerLabels="Positivo,Negativo" style="radio"/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td colspan="3"&gt;&lt;div align="center"&gt;&lt;strong&gt;BIOQUIMICA&lt;/strong&gt;&lt;/div&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;obsgroup groupingConceptId="1633"&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Albumina (ALB)&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="848" labelText=""/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Aspartato Aminotransferase (AST, SGOT, GOT)&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="653" labelText=""/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Alanina Aminotransferase (ALT, SGT, GPT)&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="654" labelText=""/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Amilase (AMI)&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="1299" labelText=""/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Bilirrubina (BIL)&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="655" labelText=""/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Bilirrubina Direita (CBIL)&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="1297" labelText=""/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Colesterol Total (COL)&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="1006" labelText=""/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Lipoproteina de Alta Densidade (HDL Colesterol)&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="1007" labelText=""/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Lipoproteina de Baixa Densidade (LDL Colesterol)&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="1008" labelText=""/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Creatinina (Cr)&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="790" labelText=""/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Creatinina Quinase (CK ou CPK)&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="1011" labelText=""/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Fosfatase Alcalina&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="785" labelText=""/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Gama-Glutamil transpeptidase (GGT)&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="2077" labelText=""/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Glucose (GLC)&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="887" labelText=""/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Lactato Desidrogenase (LDH)&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="1014" labelText=""/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Lactato&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="1012" labelText=""/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Lipase&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="1013" labelText=""/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Total Proteina&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="717" labelText=""/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Triglicerides (TG)&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="1009" labelText=""/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Ureia&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="857" labelText=""/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Cloreto&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="1134" labelText=""/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Potassio&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="1133" labelText=""/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Sódio&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="1132" labelText=""/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;Globulinas&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="1520" labelText=""/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;/obsgroup&gt;   &lt;tr&gt;     &lt;td&gt;&lt;div align="right"&gt;PCR&lt;/div&gt;&lt;/td&gt;     &lt;td colspan="2"&gt;&lt;obs conceptId="1030" labelText="" answerConceptIds="703,664,1138" answerLabels="Pos.,Neg.,Ind." style="radio"/&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;tr&gt;     &lt;td colspan="3"&gt;     &lt;div align="center"&gt;&lt;submit submitLabel="Submeter"/&gt;&lt;/div&gt;&lt;/td&gt;   &lt;/tr&gt;   &lt;/tbody&gt; &lt;/table&gt; &lt;/body&gt; &lt;/html&gt;   &lt;/htmlform&gt;</t>
+    <t>&lt;htmlform&gt;\r\n  &lt;html xmlns=\"http://www.w3.org/1999/xhtml\"&gt;\r\n\r\n  &lt;head&gt;\r\n    &lt;meta http-equiv=\"Content-Type\" content=\"text/html; charset=utf-8\" /&gt;\r\n    &lt;title&gt;FICHA DE LABORATÓRIO&lt;/title&gt;\r\n    &lt;style&gt;\r\n      h2 {\r\n        border-bottom: 3px solid red;\r\n      }\r\n\r\n      p {\r\n        border: 1px solid black;\r\n      }\r\n\r\n      table {\r\n        border-color: #600;\r\n        border-width: 0 0 1px 1px;\r\n        border-style: solid;\r\n      }\r\n\r\n      td {\r\n        border-color: #600;\r\n        border-width: 1px 1px 0 0;\r\n        border-style: solid;\r\n        margin: 0;\r\n        padding: 4px;\r\n        background-color: #B2DFEE;\r\n      }\r\n\r\n      .style1 {\r\n        font-size: 14px;\r\n        font-weight: bold;\r\n      }\r\n\r\n    &lt;/style&gt;\r\n    &lt;script type=\"text/javascript\"&gt;\r\n  \r\n      function findAutoCompleteErrors() {\r\n        /* see if there are  errors in option fields */\r\n        var containError = false;\r\n        var ary = $j(\".optionAutoCompleteHidden\");\r\n        $j.each(ary, function (index, value) {\r\n          if (value.value == \"ERROR\") {\r\n            containError = true;\r\n          }\r\n        });\r\n        return containError;\r\n      }\r\n      $j(function () {\r\n        $j(\'.submitButton\').click(function (event) {\r\n          if (!findAutoCompleteErrors()) {\r\n            $j(\'.submitButton\').prop(\'disabled\', true);\r\n          }\r\n        });\r\n      });\r\n\r\n      $j(document).ready(function() {\r\n        if($j(\".nivelDePositividade input:radio:checked\").length&gt;0){\r\n          $j(\".nivelDePositividade :input\").attr(\"disabled\", false);\r\n        }else{\r\n        $j(\".nivelDePositividade :input\").attr(\"disabled\", true);\r\n        }\r\n\r\n        if($j(\".nivelMtbDetectado input:radio:checked\").length&gt;0){\r\n          $j(\".nivelMtbDetectado :input\").attr(\"disabled\", false);\r\n        }else{\r\n        $j(\".nivelMtbDetectado :input\").attr(\"disabled\", true);\r\n        }\r\n\r\n        if($j(\".resistencia input:radio:checked\").length&gt;0){\r\n          $j(\".resistencia :input\").attr(\"disabled\", false);\r\n        }else{\r\n        $j(\".resistencia :input\").attr(\"disabled\", true);\r\n        }\r\n\r\n        jQuery(function () {\r\n        if($j(\"#cargaViralSelection :selected\").val()!== \'\'){\r\n         $j(\"#cargaViralNumeric input\").attr(\'disabled\', true);\r\n        }\r\n\r\n        if (getValue(\'cargaViralNumeric.value\') !== \'\') {\r\n            $j(\'.cargaViralSelection\').hide();\r\n         }\r\n\r\n        getField(\'cargaViralNumeric.value\').change(function () {\r\n          if (getValue(\'cargaViralNumeric.value\') === \"\") {\r\n            $j(\'.cargaViralSelection\').show();\r\n          }\r\n          else {\r\n            $j(\'.cargaViralSelection\').hide();\r\n          }\r\n        })\r\n\r\n        getField(\'cargaViralSelection.value\').change(function () {\r\n          if (getValue(\'cargaViralSelection.value\') === \"\") {\r\n            $j(\"#cargaViralNumeric input\").attr(\'disabled\', false);\r\n          }\r\n          else {\r\n            $j(\"#cargaViralNumeric input\").attr(\'disabled\', true);\r\n          }\r\n        })\r\n      });\r\n\r\n    });\r\n\r\n      function radioClicked(radio) {\r\n        var parentElId = radio.parentNode.id\r\n        if (parentElId === \"baciloscopia\") {\r\n          if (radio.value == 703) {\r\n            $j(\".nivelDePositividade :input\").attr(\"disabled\", false);\r\n            $j(\".nivelDePositividade input:radio:checked\").removeAttr(\'checked\');\r\n          } else {\r\n            $j(\".nivelDePositividade input:radio:checked\").removeAttr(\'checked\');\r\n            $j(\".nivelDePositividade :input\").attr(\"disabled\", true);\r\n          }\r\n        }\r\n\r\n        if (parentElId === \"mtbDetectada\") {\r\n          if (radio.value == 1065) {\r\n            $j(\".nivelMtbDetectado :input\").attr(\"disabled\", false);\r\n            $j(\".nivelMtbDetectado input:radio:checked\").removeAttr(\'checked\');\r\n            $j(\".resistencia :input\").attr(\"disabled\", false);\r\n            $j(\".resistencia input:radio:checked\").removeAttr(\'checked\');\r\n          } else {\r\n            $j(\".nivelMtbDetectado input:radio:checked\").removeAttr(\'checked\');\r\n            $j(\".nivelMtbDetectado :input\").attr(\"disabled\", true);\r\n            $j(\".resistencia input:radio:checked\").removeAttr(\'checked\');\r\n            $j(\".resistencia :input\").attr(\"disabled\", true);\r\n          }\r\n        }\r\n      }\r\n    &lt;/script&gt;\r\n  &lt;/head&gt;\r\n\r\n  &lt;body&gt;\r\n    &lt;table width=\"55%\" border=\"1\" align=\"center\"&gt;\r\n      &lt;tbody align=\"left\" style=\"font-family:verdana; font-size:12px\"&gt;\r\n        &lt;tr&gt;\r\n          &lt;td colspan=\"3\"&gt;\r\n            &lt;div align=\"center\" class=\"style1\"&gt;FICHA DE LABORATÓRIO&lt;/div&gt;\r\n          &lt;/td&gt;\r\n        &lt;/tr&gt;\r\n        &lt;tr&gt;\r\n          &lt;td colspan=\"3\"&gt;\r\n            &lt;div align=\"center\"&gt;&lt;strong&gt;PACIENTE&lt;/strong&gt;&lt;/div&gt;\r\n          &lt;/td&gt;\r\n        &lt;/tr&gt;\r\n        &lt;tr&gt;\r\n          &lt;td width=\"70%\"&gt;\r\n            &lt;div align=\"right\"&gt;Nome&lt;/div&gt;\r\n          &lt;/td&gt;\r\n          &lt;td colspan=\"2\"&gt;\r\n            &lt;lookup expression=\"patient.personName\" /&gt;\r\n          &lt;/td&gt;\r\n        &lt;/tr&gt;\r\n        &lt;tr&gt;\r\n          &lt;td&gt;\r\n            &lt;div align=\"right\"&gt;sexo&lt;/div&gt;\r\n          &lt;/td&gt;\r\n          &lt;td colspan=\"2\"&gt;\r\n            &lt;lookup expression=\"patient.gender\" /&gt;\r\n          &lt;/td&gt;\r\n        &lt;/tr&gt;\r\n        &lt;tr&gt;\r\n          &lt;td&gt;\r\n            &lt;div align=\"right\"&gt;NID&lt;/div&gt;\r\n          &lt;/td&gt;\r\n          &lt;td colspan=\"2\"&gt;\r\n            &lt;lookup expression=\"patient.getPatientIdentifier(2)\" /&gt;\r\n          &lt;/td&gt;\r\n        &lt;/tr&gt;\r\n        &lt;tr&gt;\r\n          &lt;td colspan=\"3\"&gt;\r\n            &lt;div align=\"center\"&gt;&lt;strong&gt;EXAME&lt;/strong&gt;&lt;/div&gt;\r\n          &lt;/td&gt;\r\n        &lt;/tr&gt;\r\n        &lt;tr&gt;\r\n          &lt;td&gt;\r\n            &lt;div align=\"right\"&gt;Data do Pedido&lt;/div&gt;\r\n          &lt;/td&gt;\r\n          &lt;td colspan=\"2\"&gt;\r\n            &lt;obs conceptId=\"6246\" labelText=\"\" /&gt;\r\n          &lt;/td&gt;\r\n        &lt;/tr&gt;\r\n        &lt;tr&gt;\r\n          &lt;td&gt;\r\n            &lt;div align=\"right\"&gt;Data da Colheita de Amostra&lt;/div&gt;\r\n          &lt;/td&gt;\r\n          &lt;td colspan=\"2\"&gt;\r\n            &lt;obs conceptId=\"23821\" labelText=\"\" /&gt;\r\n          &lt;/td&gt;\r\n        &lt;/tr&gt;\r\n        &lt;tr&gt;\r\n          &lt;td&gt;\r\n            &lt;div align=\"right\"&gt;Data do Resultado&lt;/div&gt;\r\n          &lt;/td&gt;\r\n          &lt;td colspan=\"2\"&gt;\r\n            &lt;encounterDate /&gt;\r\n          &lt;/td&gt;\r\n        &lt;/tr&gt;\r\n        &lt;tr&gt;\r\n          &lt;td&gt;\r\n            &lt;div align=\"right\"&gt;Unidade Sanitária&lt;/div&gt;\r\n          &lt;/td&gt;\r\n          &lt;td colspan=\"2\"&gt;\r\n            &lt;encounterLocation id=\"localConsulta\" default=\"GlobalProperty:default_location\" /&gt;\r\n          &lt;/td&gt;\r\n        &lt;/tr&gt;\r\n        &lt;tr&gt;\r\n          &lt;td&gt;\r\n            &lt;div align=\"right\"&gt;Técnico&lt;/div&gt;\r\n          &lt;/td&gt;\r\n          &lt;td colspan=\"2\"&gt;\r\n            &lt;encounterProvider role=\"Provider\" type=\"autocomplete\" /&gt;\r\n          &lt;/td&gt;\r\n        &lt;/tr&gt;\r\n        &lt;tr&gt;\r\n          &lt;td colspan=\"3\"&gt;\r\n            &lt;div align=\"center\"&gt;&lt;strong&gt;RESULTADOS&lt;/strong&gt;&lt;/div&gt;\r\n          &lt;/td&gt;\r\n        &lt;/tr&gt;\r\n        &lt;tr&gt;\r\n          &lt;td colspan=\"3\"&gt;\r\n            &lt;div align=\"center\"&gt;&lt;strong&gt;HEMATOLOGIA&lt;/strong&gt;&lt;/div&gt;\r\n          &lt;/td&gt;\r\n        &lt;/tr&gt;\r\n        &lt;obsgroup groupingConceptId=\"1723\"&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Globulos Brancos (WBC)&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td colspan=\"2\"&gt;\r\n              &lt;obs conceptId=\"678\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Globulos Vermelhos (RBC)&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td colspan=\"2\"&gt;\r\n              &lt;obs conceptId=\"679\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Hemoglobina (HGB ou HB)&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td colspan=\"2\"&gt;\r\n              &lt;obs conceptId=\"21\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Hematócrito (HCT, PCV)&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td colspan=\"2\"&gt;\r\n              &lt;obs conceptId=\"1015\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Volume Corpuscular Médio (HCV, VCM, VGM)&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td colspan=\"2\"&gt;\r\n              &lt;obs conceptId=\"851\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Volume Corpuscular Hemoglobina (MCH, HGM, HCM)&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td colspan=\"2\"&gt;\r\n              &lt;obs conceptId=\"1018\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Concentração Média de Hemoglobina Corpuscular (MCHC, CHCM, CMHG)&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td colspan=\"2\"&gt;\r\n              &lt;obs conceptId=\"1017\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Plaquetas (PLT)&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td colspan=\"2\"&gt;\r\n              &lt;obs conceptId=\"729\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Largura de Distribuição de Globulos Vermelhos (RDW)&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td colspan=\"2\"&gt;\r\n              &lt;obs conceptId=\"1016\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Velocidade de Sedimentação dos Globulos Vermelhos (VS, VHS)&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td colspan=\"2\"&gt;\r\n              &lt;obs conceptId=\"855\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Volume médio de Plaquetas (MPV)&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td colspan=\"2\"&gt;\r\n              &lt;obs conceptId=\"1307\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Tipagem Sanguinea&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td colspan=\"2\"&gt;\r\n              &lt;obs conceptId=\"300\" labelText=\"\" answerConceptIds=\"690,692,694,696,699,701,1230,1231\"\r\n                answerLabels=\"A POSITIVO,A NEGATIVO,B POSITIVO, B NEGATIVO,O POSITIVO,O NEGATIVO,AB POSITIVO, AB NEGATIVO\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n\r\n          &lt;tr&gt;\r\n            &lt;td&gt;&lt;/td&gt;\r\n            &lt;td width=\"14%\"&gt;&lt;strong&gt;Percentual (%)&lt;/strong&gt;&lt;/td&gt;\r\n            &lt;td width=\"13%\"&gt;&lt;strong&gt;Absoluto (#)&lt;/strong&gt;&lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Linfocitos (LYM)&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td&gt;\r\n              &lt;obs conceptId=\"1021\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n            &lt;td&gt;\r\n              &lt;obs conceptId=\"952\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Neutrofilos (NEUT)&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td&gt;\r\n              &lt;obs conceptId=\"1022\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n            &lt;td&gt;\r\n              &lt;obs conceptId=\"1330\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Eosinofilo&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td&gt;\r\n              &lt;obs conceptId=\"1024\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n            &lt;td&gt;\r\n              &lt;obs conceptId=\"1332\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Basofilo&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td&gt;\r\n              &lt;obs conceptId=\"1025\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n            &lt;td&gt;\r\n              &lt;obs conceptId=\"1333\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Monocito&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td&gt;\r\n              &lt;obs conceptId=\"1023\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n            &lt;td&gt;\r\n              &lt;obs conceptId=\"1331\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td colspan=\"3\"&gt;\r\n              &lt;div align=\"center\"&gt;&lt;strong&gt;Diagnóstico Laboratorial para ITS&lt;/strong&gt;&lt;/div&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Teste de VDRL&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td colspan=\"2\"&gt;\r\n              &lt;obs conceptId=\"299\" labelText=\"\" answerConceptIds=\"1228,1229\" answerLabels=\"Positivo,Negativo\"\r\n                style=\"radio\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n        &lt;/obsgroup&gt;\r\n        &lt;obsgroup groupingConceptId=\"1639\"&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;RPR&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td colspan=\"2\"&gt;\r\n              &lt;obs conceptId=\"1655\" labelText=\"\" answerConceptIds=\"1228,1229\" answerLabels=\"Positivo,Negativo\"\r\n                style=\"radio\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n\r\n          &lt;tr&gt;\r\n            &lt;td&gt;&lt;/td&gt;\r\n            &lt;td&gt;&lt;strong&gt;Absoluto&lt;/strong&gt;&lt;/td&gt;\r\n            &lt;td&gt;&lt;strong&gt;Percentual&lt;/strong&gt;&lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;CD4&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td&gt;\r\n              &lt;obs conceptId=\"5497\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n            &lt;td&gt;\r\n              &lt;obs conceptId=\"730\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n        &lt;/obsgroup&gt;\r\n        &lt;obsgroup groupingConceptId=\"1632\"&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Carga Viral&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td colspan=\"2\"&gt;\r\n              &lt;obs id=\"cargaViralNumeric\" conceptId=\"856\" labelText=\"\" /&gt; |\r\n              &lt;obs class=\"cargaViralSelection\" id=\"cargaViralSelection\" conceptId=\"e1da2704-1d5f-11e0-b929-000c29ad1d07\"\r\n                answerConceptIds=\"e1da2812-1d5f-11e0-b929-000c29ad1d07, cc8ef88c-6ab6-4404-a036-d415bc42cc1c, 78a76661-50c0-41cf-b566-de275f17b648, ae6c048f-8b04-46cb-903e-51d5670db525, 1321eeac-5832-4076-88e9-b1f2cd351ada, d6eb4797-2c01-4b6e-b43f-be15cd2fdcc2, 7c8e0a9b-3606-4a72-b8cc-89566521fac2\"\r\n                answerLabels=\"Nivel baixo de detecção, Indetectável, Menor que 10 copias/ml, Menor que 20 copias/ml, Menor que 40 copias/ml, Menor que 400 copias/ml, Menor que 839 copias/ml\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n        &lt;/obsgroup&gt;\r\n        &lt;tr&gt;\r\n          &lt;td colspan=\"3\"&gt;\r\n            &lt;div align=\"center\"&gt;&lt;strong&gt;Diagnóstico Laboratorial para TB&lt;/strong&gt;&lt;/div&gt;\r\n          &lt;/td&gt;\r\n        &lt;/tr&gt;\r\n        &lt;tr&gt;\r\n          &lt;td&gt;\r\n            &lt;div align=\"right\"&gt;GeneXpert&lt;/div&gt;\r\n          &lt;/td&gt;\r\n          &lt;td colspan=\"2\"&gt;\r\n            &lt;obs conceptId=\"23723\" labelText=\"\" answerConceptIds=\"703,664\" answerLabels=\"Positivo,Negativo\"\r\n              style=\"radio\" /&gt;\r\n          &lt;/td&gt;\r\n        &lt;/tr&gt;\r\n        &lt;tr&gt;\r\n          &lt;td&gt;\r\n            &lt;div align=\"right\"&gt;XPert MTB/RIF. Presença de MTB detectada&lt;/div&gt;\r\n          &lt;/td&gt;\r\n          &lt;td colspan=\"2\"&gt;&lt;span id=\"mtbDetectada\" class=\"mtbDetectada\"&gt;\r\n              &lt;obs conceptId=\"8dc1afbd-c10b-4834-a327-396c73848c73\" labelText=\"\" answerConceptIds=\"1065,1066\"\r\n                answerLabels=\"Sim,Não\" style=\"radio\" /&gt;&lt;/span&gt;&lt;/td&gt;\r\n        &lt;/tr&gt;\r\n        &lt;tr&gt;\r\n          &lt;td&gt;\r\n            &lt;div align=\"right\"&gt;Nível de MTB detectado&lt;/div&gt;\r\n          &lt;/td&gt;\r\n          &lt;td colspan=\"2\"&gt;&lt;span class=\"nivelMtbDetectado\"&gt;\r\n              &lt;obs conceptId=\"8e748300-f842-439f-ba32-1b5cf630a23d\" labelText=\"\"\r\n                answerConceptIds=\"6230,6229,6228,77719331-67c9-4ca6-bd4f-c7538ae730af\"\r\n                answerLabels=\"Alto,Médio,Baixo,Traço\" style=\"radio\" /&gt;&lt;/span&gt;&lt;/td&gt;\r\n        &lt;/tr&gt;\r\n        &lt;tr&gt;\r\n          &lt;td&gt;\r\n            &lt;div align=\"right\"&gt;Se MTB detectado: Resistência a Rifampin&lt;/div&gt;\r\n          &lt;/td&gt;\r\n          &lt;td colspan=\"2\"&gt;&lt;span class=\"resistencia\"&gt;\r\n              &lt;obs conceptId=\"cc7e60cc-b9e6-4083-bb6d-8b9caa070f26\" labelText=\"\" answerConceptIds=\"1065,1066,1138\"\r\n                answerLabels=\"Sim,Não,Indeterminado\" style=\"radio\" /&gt;&lt;/span&gt;&lt;/td&gt;\r\n        &lt;/tr&gt;\r\n        &lt;tr&gt;\r\n          &lt;td&gt;\r\n            &lt;div align=\"right\"&gt;Cultura&lt;/div&gt;\r\n          &lt;/td&gt;\r\n          &lt;td colspan=\"2\"&gt;\r\n            &lt;obs conceptId=\"23774\" labelText=\"\" answerConceptIds=\"703,664\" answerLabels=\"Positivo,Negativo\"\r\n              style=\"radio\" /&gt;\r\n          &lt;/td&gt;\r\n        &lt;/tr&gt;\r\n        &lt;tr&gt;\r\n          &lt;td&gt;\r\n            &lt;div align=\"right\"&gt;TB LAM&lt;/div&gt;\r\n          &lt;/td&gt;\r\n          &lt;td colspan=\"2\"&gt;\r\n            &lt;obs conceptId=\"23951\" labelText=\"\" answerConceptIds=\"703,664,1138\"\r\n              answerLabels=\"Positivo,Negativo,Indeterminado\" style=\"radio\" /&gt;\r\n          &lt;/td&gt;\r\n        &lt;/tr&gt;\r\n        &lt;tr&gt;\r\n          &lt;td&gt;\r\n            &lt;div align=\"right\"&gt;CRAG&lt;/div&gt;\r\n          &lt;/td&gt;\r\n          &lt;td colspan=\"2\"&gt;\r\n            &lt;obs conceptId=\"23952\" labelText=\"\" answerConceptIds=\"703,664\" answerLabels=\"Positivo,Negativo\"\r\n              style=\"radio\" /&gt;\r\n          &lt;/td&gt;\r\n        &lt;/tr&gt;\r\n        &lt;tr&gt;\r\n          &lt;td&gt;\r\n            &lt;div align=\"right\"&gt;Smear Microscopy for TB(Baciloscopia)&lt;/div&gt;\r\n          &lt;/td&gt;\r\n          &lt;td colspan=\"2\"&gt;\r\n            &lt;obs class=\"baciloscopia\" id=\"baciloscopia\" conceptId=\"307\" labelText=\"\"\r\n              answerConceptIds=\"703,8ee04ec1-9a35-43ba-9a61-4f7927300f87\" answerLabels=\"Positivo,Não encontrado\"\r\n              style=\"radio\" /&gt;\r\n          &lt;/td&gt;\r\n        &lt;/tr&gt;\r\n        &lt;tr&gt;\r\n          &lt;td&gt;\r\n            &lt;div align=\"right\"&gt;Nível de positividade&lt;/div&gt;\r\n          &lt;/td&gt;\r\n          &lt;td colspan=\"2\"&gt;\r\n            &lt;span class=\"nivelDePositividade\"&gt;\r\n            &lt;obs conceptId=\"303a4480-f2b3-4192-a446-725a401ebb09\"\r\n              labelText=\"\" answerConceptIds=\"a4e43a4d-37ea-4767-a700-9fe1d43a8042\r\n        ,79f4bd59-0dbb-41ba-9d78-3efc0b737b75,03d4b7c8-c8cd-4f84-be40-67975bd5b667\" answerLabels=\"3+,2+,1+\"\r\n              style=\"radio\" /&gt;\r\n              &lt;/span&gt;\r\n          &lt;/td&gt;\r\n        &lt;/tr&gt;\r\n        &lt;tr&gt;\r\n          &lt;td colspan=\"3\"&gt;\r\n            &lt;div align=\"center\"&gt;&lt;strong&gt;BIOQUIMICA&lt;/strong&gt;&lt;/div&gt;\r\n          &lt;/td&gt;\r\n        &lt;/tr&gt;\r\n        &lt;obsgroup groupingConceptId=\"1633\"&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Albumina (ALB)&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td colspan=\"2\"&gt;\r\n              &lt;obs conceptId=\"848\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Aspartato Aminotransferase (AST, SGOT, GOT)&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td colspan=\"2\"&gt;\r\n              &lt;obs conceptId=\"653\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Alanina Aminotransferase (ALT, SGT, GPT)&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td colspan=\"2\"&gt;\r\n              &lt;obs conceptId=\"654\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Amilase (AMI)&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td colspan=\"2\"&gt;\r\n              &lt;obs conceptId=\"1299\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Bilirrubina (BIL)&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td colspan=\"2\"&gt;\r\n              &lt;obs conceptId=\"655\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Bilirrubina Direita (CBIL)&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td colspan=\"2\"&gt;\r\n              &lt;obs conceptId=\"1297\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Colesterol Total (COL)&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td colspan=\"2\"&gt;\r\n              &lt;obs conceptId=\"1006\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Lipoproteina de Alta Densidade (HDL Colesterol)&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td colspan=\"2\"&gt;\r\n              &lt;obs conceptId=\"1007\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Lipoproteina de Baixa Densidade (LDL Colesterol)&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td colspan=\"2\"&gt;\r\n              &lt;obs conceptId=\"1008\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Creatinina (Cr)&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td colspan=\"2\"&gt;\r\n              &lt;obs conceptId=\"790\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Creatinina Quinase (CK ou CPK)&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td colspan=\"2\"&gt;\r\n              &lt;obs conceptId=\"1011\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Fosfatase Alcalina&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td colspan=\"2\"&gt;\r\n              &lt;obs conceptId=\"785\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Gama-Glutamil transpeptidase (GGT)&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td colspan=\"2\"&gt;\r\n              &lt;obs conceptId=\"2077\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Glucose (GLC)&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td colspan=\"2\"&gt;\r\n              &lt;obs conceptId=\"887\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Lactato Desidrogenase (LDH)&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td colspan=\"2\"&gt;\r\n              &lt;obs conceptId=\"1014\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Lactato&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td colspan=\"2\"&gt;\r\n              &lt;obs conceptId=\"1012\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Lipase&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td colspan=\"2\"&gt;\r\n              &lt;obs conceptId=\"1013\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Total Proteina&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td colspan=\"2\"&gt;\r\n              &lt;obs conceptId=\"717\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Triglicerides (TG)&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td colspan=\"2\"&gt;\r\n              &lt;obs conceptId=\"1009\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Ureia&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td colspan=\"2\"&gt;\r\n              &lt;obs conceptId=\"857\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Cloreto&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td colspan=\"2\"&gt;\r\n              &lt;obs conceptId=\"1134\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Potassio&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td colspan=\"2\"&gt;\r\n              &lt;obs conceptId=\"1133\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Sódio&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td colspan=\"2\"&gt;\r\n              &lt;obs conceptId=\"1132\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;\r\n              &lt;div align=\"right\"&gt;Globulinas&lt;/div&gt;\r\n            &lt;/td&gt;\r\n            &lt;td colspan=\"2\"&gt;\r\n              &lt;obs conceptId=\"1520\" labelText=\"\" /&gt;\r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n        &lt;/obsgroup&gt;\r\n        &lt;tr&gt;\r\n          &lt;td&gt;\r\n            &lt;div align=\"right\"&gt;PCR&lt;/div&gt;\r\n          &lt;/td&gt;\r\n          &lt;td colspan=\"2\"&gt;\r\n            &lt;obs conceptId=\"1030\" labelText=\"\" answerConceptIds=\"703,664,1138\" answerLabels=\"Pos.,Neg.,Ind.\"\r\n              style=\"radio\" /&gt;\r\n          &lt;/td&gt;\r\n        &lt;/tr&gt;\r\n        &lt;tr&gt;\r\n          &lt;td colspan=\"3\"&gt;\r\n            &lt;div align=\"center\"&gt;\r\n              &lt;submit submitLabel=\"Submeter\" /&gt;\r\n            &lt;/div&gt;\r\n          &lt;/td&gt;\r\n        &lt;/tr&gt;\r\n      &lt;/tbody&gt;\r\n    &lt;/table&gt;\r\n  &lt;/body&gt;\r\n\r\n  &lt;/html&gt;\r\n\r\n\r\n&lt;/htmlform&gt;</t>
   </si>
   <si>
     <t>45acd87b-3daa-49a6-8f50-9cc38f318761</t>
@@ -246,7 +246,7 @@
     <t>204c4988-91b6-47c0-a8ec-25280f769b48</t>
   </si>
   <si>
-    <t>&lt;htmlform&gt;\r\n&lt;script type=\"text/javascript\"&gt;\r\n\r\njQuery(function() {\r\n  getField(\'levaCamp.value\').change(function(){\r\n   if(getValue(\'levaCamp.value\') == 1065) {\r\n      getField(\'nomeCamp.value\').show();\r\n    } \r\n    else{\r\n     setValue(\'nomeCamp.value\',\'\');\r\n      getField(\'nomeCamp.value\').hide();\r\n    }\r\n  })\r\n});\r\n    \r\n  //Validações antes de submter\r\n beforeSubmit.push(function() {  \r\n    \r\n    //Data de proximo levantamento  \r\n    var dataProximoLev = new Date(getValue(\'dataProxima.value\'));\r\n   \r\n    //Data da consulta seleccionada\r\n   var dataConsulta = new Date(getValue(\'dataConsulta.value\'));\r\n\r\n    //Ultimo estadio do paciente\r\n    var lastRegime = parseInt(\"&lt;lookup expression=\"fn.latestObs(1088).valueCoded\"/&gt;\");\r\n    //Estadio Seleccionado\r\n    var selectedRegime = parseInt(getValue(\'regime.value\'));  \r\n    \r\n    //Data de Nascimento  \r\n    var dataNascimento = new Date(Date.parse(\"&lt;lookup expression=\"patient.birthdate\"/&gt;\"));\r\n    \r\n    //Data de inicio de TARV\r\n    //var dataInicioTARV = \"&lt;lookup expression=\"fn.latestObs(1190).valueDatetime\"/&gt;\";\r\n   \r\n    var estadoProgramaTarvConceptID = parseInt(\"&lt;lookup expression=\"fn.currentProgramWorkflowStatus(2).state.concept.id\" /&gt;\")\r\n\r\n       \r\n    if (isNaN(estadoProgramaTarvConceptID)){      \r\n      getField(\'dataConsulta.error\').html(\'Deve admitir este paciente no programa de TARV - TRATAMENTO\').show();\r\n      return false;     \r\n    }else{\r\n      if(!((estadoProgramaTarvConceptID==6269) || (estadoProgramaTarvConceptID==1369))){\r\n        getField(\'dataConsulta.error\').html(\'Este paciente não está no estado activo no programa, coloque-o como activo primeiro\').show();\r\n        return false; \r\n      }\r\n   }\r\n   \r\n    \r\n    //Compara se a data de levantamento e menor que data de nascimento\r\n    //if (dataInicioTARV == \'\') {         \r\n    //    getField(\'dataConsulta.error\').html(\'O Paciente não tem data de inicio de TARV registado na Ficha de Seguimento (Antigo) ou Ficha Resumo (Master Card)\').show();\r\n    //    return false;           \r\n    //}\r\n   \r\n    //Compara se a data da proxima é menor que a data de levantamento \r\n    if (dataProximoLev &amp;lt;=  dataConsulta) {         \r\n        getField(\'dataProxima.error\').html(\'A data do proximo levantamento não deve ser menor ou igual que a data de levantamento\').show();\r\n       return false;           \r\n    }\r\n\r\n   //Compara se a data de levantamento e menor que data de nascimento\r\n    if (dataConsulta &amp;lt;  dataNascimento) {          \r\n        getField(\'dataConsulta.error\').html(\'A data do levantamento não deve ser menor que a data de nascimento\').show();\r\n       return false;           \r\n    }   \r\n    \r\n    \r\n      \r\n      if(lastRegime != selectedRegime){\r\n       var confirmacao=window.confirm(\'Confirma a mudança de regime deste paciente?\');\r\n       if(confirmacao == false)\r\n        return false;\r\n     }\r\n   \r\n        $j(\'.submitButton\').prop(\'disabled\', true);   \r\n            \r\n    return true;\r\n  }); \r\n  \r\n&lt;/script&gt;\r\n&lt;html xmlns=\"http://www.w3.org/1999/xhtml\"&gt;\r\n&lt;head&gt;\r\n&lt;meta http-equiv=\"Content-Type\" content=\"text/html; charset=utf-8\" /&gt;\r\n&lt;title&gt;FILA&lt;/title&gt;\r\n  \r\n  &lt;style&gt;\r\n     h2 { border-bottom: 3px solid red; }\r\n      p { border: 1px solid black; }\r\n      table{\r\n        border-color: #600;\r\n       border-width: 0 0 1px 1px;\r\n        border-style: solid;}\r\n\r\n     td{\r\n       border-color: #600;\r\n       border-width: 1px 1px 0 0;\r\n        border-style: solid;\r\n        margin: 0;\r\n        padding: 4px;\r\n       background-color: #B2DFEE;}\r\n     .style1 {\r\n       font-size: 14px;\r\n        font-weight: bold;}\r\n     .section {\r\n        border: 1px solid $headerColor;\r\n       padding: 2px;\r\n       text-align: center;\r\n       margin-bottom: 1em;\r\n       border-width:thin;\r\n        width:50%;\r\n        vertical-align:middle;\r\n        azimuth:center;}\r\n      .sectionHeader {\r\n        background-color: $headerColor;\r\n       color: $fontOnHeaderColor;\r\n        display: block;\r\n       padding: 2px;\r\n       font-weight: bold;}\r\n     table.baseline-aligned td {\r\n       vertical-align: baseline;}\r\n  &lt;/style&gt;\r\n&lt;/head&gt;\r\n&lt;body&gt;\r\n&lt;table width=\"900\" border=\"1\" align=\"center\"&gt;\r\n  &lt;tbody align=\"left\" style=\"font-family:verdana; font-size:12px\"&gt;\r\n  &lt;tr&gt;\r\n    &lt;td width=\"285\" rowspan=\"4\"&gt;REPÚBLICA DE MOÇAMBIQUE&lt;br/&gt;Serviço Nacional de Saúde&lt;/td&gt;\r\n    &lt;td colspan=\"2\"&gt;&lt;div align=\"center\" class=\"style1\"&gt;Ficha Individual de Levantamento de ARVs (FILA)&lt;/div&gt;&lt;/td&gt;\r\n  &lt;/tr&gt;\r\n  &lt;tr&gt;\r\n    &lt;td colspan=\"2\"&gt;\r\n     Nº do Livro TARV:&lt;lookup expression=\"fn.latestObs(6264).getValueAsString($!{locale})\"/&gt;   \r\n     Pag: &lt;lookup expression=\"fn.latestObs(6266).getValueAsString($!{locale})\"/&gt;  \r\n     Linha: &lt;lookup expression=\"fn.latestObs(6268).getValueAsString($!{locale})\"/&gt;  \r\n    &lt;/td&gt;\r\n    &lt;/tr&gt;\r\n  &lt;tr&gt;\r\n    &lt;td width=\"245\"&gt;&lt;div align=\"right\"&gt;Nome:&lt;/div&gt;&lt;/td&gt;\r\n    &lt;td width=\"348\"&gt;&lt;lookup expression=\"patient.personName\"/&gt;&lt;/td&gt;\r\n  &lt;/tr&gt;\r\n  &lt;tr&gt;\r\n    &lt;td&gt;&lt;div align=\"right\"&gt;Contacto:&lt;/div&gt;&lt;/td&gt;\r\n    &lt;td&gt;&lt;lookup expression=\"patient.getAttribute(9)\"/&gt;&lt;/td&gt;\r\n  &lt;/tr&gt;\r\n  &lt;tr&gt;\r\n    &lt;td&gt;NID: &lt;lookup expression=\"patient.getPatientIdentifier(2)\"/&gt;\r\n                    &lt;lookup expression=\"patient.getPatientIdentifier(14)\"/&gt;\r\n\r\n&lt;/td&gt;\r\n    &lt;td&gt;&lt;div align=\"right\"&gt;Endereço:&lt;/div&gt;&lt;/td&gt;\r\n    &lt;td&gt;&lt;lookup complexExpression=\"#foreach( $addr in $patient.addresses ) $!addr.subregion #end\"/&gt;&lt;/td&gt;\r\n  &lt;/tr&gt;\r\n  \r\n  &lt;/tbody&gt;\r\n&lt;/table&gt;\r\n\r\n&lt;br/&gt;\r\n\r\n&lt;table width=\"900\" border=\"1\" align=\"center\"&gt;\r\n  &lt;tbody align=\"left\" style=\"font-family:verdana; font-size:12px\"&gt;\r\n  \r\n  \r\n  &lt;tr&gt;\r\n    &lt;td&gt;&lt;div align=\"right\"&gt;Data de Levantamento:&lt;/div&gt;&lt;/td&gt;\r\n    &lt;td&gt;&lt;encounterDate id=\"dataConsulta\"/&gt;&lt;/td&gt;\r\n  &lt;/tr&gt;\r\n  &lt;tr&gt;\r\n    &lt;td&gt;&lt;div align=\"right\"&gt;Provedor:&lt;/div&gt;&lt;/td&gt;\r\n    &lt;td&gt;&lt;encounterProvider role=\"Provider\" type=\"autocomplete\"/&gt;&lt;/td&gt;\r\n  &lt;/tr&gt;\r\n  &lt;tr&gt;\r\n    &lt;td&gt;&lt;div align=\"right\"&gt;Unidade Sanitária:&lt;/div&gt;&lt;/td&gt;\r\n    &lt;td&gt;\r\n &lt;encounterLocation id=\"localConsulta\" default=\"GlobalProperty:default_location\" type=\"autocomplete\"/&gt;\r\n &lt;/td&gt;\r\n  &lt;/tr&gt;\r\n  &lt;tr&gt;\r\n    &lt;td width=\"40%\"&gt;&lt;div align=\"right\"&gt;Medicamentos ARVs:&lt;/div&gt;&lt;/td&gt;\r\n    &lt;td width=\"60%\"&gt;Ultimo Regime:\r\n      &lt;strong&gt;\r\n      &lt;lookup expression=\"fn.latestObs(1088).getValueAsString($!{locale})\"/&gt;&lt;/strong&gt;&lt;br /&gt;\r\n      \r\n   \r\n    &lt;obs id=\"regime\" conceptId=\"e1d83e4e-1d5f-11e0-b929-000c29ad1d07\" answerConceptIds=\"\r\n                                            e1de19fe-1d5f-11e0-b929-000c29ad1d07,\r\n                                            28b28521-b6cd-454e-9ec5-f2c6c9c58468,\r\n                                            e1dd2f44-1d5f-11e0-b929-000c29ad1d07,\r\n                                            9dc17c1b-7b6d-488e-a38d-505a7b65ec82,\r\n                                            2e44e77e-eac4-4f64-84d2-73d32abf94d5,\r\n                                            78419317-cdda-42e9-92a3-13cb0cbf0020,\r\n                                            e3f6bb60-e2cf-46cb-a9da-27d634ba8607,\r\n                                            af15246d-30b8-4aff-8391-ca2b58e2c88b,\r\n                                            3e7f46c7-a971-4c0c-82aa-a65589fd518e,\r\n                                            cf05347e-063c-4896-91a4-097741cf6be6,\r\n                                            e11be52e-0da1-4d32-ab5c-e0feb9b6abd6,\r\n                                            f8c5d365-7636-4449-9acd-c83c4fd2ea01,\r\n                                            d5f9d629-67bc-4f60-9e12-629e6d2c1d08,\r\n                                            7bf5a88d-6db6-4899-a01a-bfd14ce77b53,\r\n                                            e8b741b3-463c-46b1-8423-a16f736af8d4,\r\n                                            ba25f2b5-4216-4605-9e6b-1f591033dc3e,\r\n                                            7d18d08c-d1a8-4dc8-8d65-02197b42acf7,\r\n                                            c22c4431-a27e-4054-92bb-a1563482003e,\r\n                                            c4a56680-ac6e-4538-8126-e3097b7b4789,\r\n                                            8f9c4e58-0d70-4b09-a109-e776d325e9fd,\r\n                                            9cb63f72-4c08-4543-878a-537dcabe5670,\r\n                                            46b8a2ab-36a7-4072-ab62-0af9b3b58e72,\r\n                                            552dd71f-d1de-426a-a19c-49b8706a4a7f,\r\n                                            f32e013c-38c8-483a-8012-88596e8b13da,\r\n                                            c30f826d-9433-4e63-ac91-dbbc158686ff,\r\n                                            e1e59e0e-1d5f-11e0-b929-000c29ad1d07\" labelText=\"\" answerLabels=\"AZT+3TC+EFV,\r\n                                                                                                            AZT+3TC+LPV/r,\r\n                                                                                                            AZT+3TC+NVP,\r\n                                                                                                            TDF+3TC+EFV,\r\n                                                                                                            TDF+3TC+NVP,\r\n                                                                                                            ABC+3TC+EFV,\r\n                                                                                                            TDF+3TC+DTG,\r\n                                                                                                            ABC+3TC+DTG,\r\n                                                                                                            AZT+3TC+ABC,\r\n                                                                                                            ABC+3TC+LPV/r,\r\n                                                                                                            ABC+3TC+NVP,\r\n                                                                                                            TDF+3TC+LPV/r,\r\n                                                                                                            TDF+3TC+LPV/r+RTV,\r\n                                                                                                            TDF+3TC+ATV/r,\r\n                                                                                                            ABC+3TC+ATV/r,\r\n                                                                                                            AZT+3TC+ATV/r,\r\n                                                                                                            ABC+3TC+ATV/r+RAL,\r\n                                                                                                            TDF+3TC+ATV/r+RAL,\r\n                                                                                                            AZT+3TC+RAL,\r\n                                                                                                            AZT+3TC+DRV/r,\r\n                                                                                                            AZT+3TC+DTG,\r\n                                                                                                            TDF+3TC+RAL+DRV/r,\r\n                                                                                                            ABC+3TC++RAL+DRV/r,\r\n                                                                                                            3TC+RAL+DRV/r,\r\n                                                                                                            AZT+3TC+RAL+DRV/r,\r\n                                                                                                            OUTRO\" required=\"true\"/&gt;\r\n   \r\n    \r\n    &lt;/td&gt;\r\n  &lt;/tr&gt;  \r\n  &lt;tr&gt;\r\n    &lt;td&gt;&lt;div align=\"right\"&gt;Quantidade Aviada:&lt;/div&gt;&lt;/td&gt;\r\n    &lt;td&gt;&lt;obs id=\"quantidadeAviada\" conceptId=\"1715\" labelText=\"\" answers=\"15,30,45,60,90,120,180\" answerLabels=\"15,30,45,60,90,120,180\"/&gt; - &lt;obs conceptId=\"1715\" labelText=\"Outra:\"/&gt;&lt;/td&gt;\r\n  &lt;/tr&gt;\r\n  &lt;tr&gt;\r\n    &lt;td&gt;&lt;div align=\"right\"&gt;Dosagem:&lt;/div&gt;&lt;/td&gt;\r\n    &lt;td&gt;&lt;obs id=\"posologia\" conceptId=\"1711\" labelText=\"\" answers=\"1-0-1,0-0-1,1-0-0,2-0-2,3-0-3,0-0-3,1-0-2,1-0-1.5\" answerLabels=\"1-0-1,0-0-1,1-0-0,2-0-2,3-0-3,0-0-3,1-0-2,1-0-1.5\"/&gt; - &lt;obs conceptId=\"1711\" labelText=\"Outra:\" size=\"8\"/&gt;&lt;/td&gt;\r\n  &lt;/tr&gt;\r\n  &lt;tr&gt;\r\n    &lt;td&gt;&lt;div align=\"right\"&gt;Data do próximo Levantamento:&lt;/div&gt;&lt;/td&gt;\r\n    &lt;td&gt;&lt;obs id=\"dataProxima\" conceptId=\"5096\" labelText=\"\" allowFutureDates=\"true\" required=\"true\"/&gt;&lt;/td&gt;\r\n  &lt;/tr&gt;\r\n   &lt;tr&gt;\r\n    &lt;td&gt;&lt;div align=\"right\"&gt;Levantamento efectuado num campo de acomodação?&lt;/div&gt;&lt;/td&gt;\r\n    &lt;td&gt;&lt;obs id=\"levaCamp\" conceptId=\"23856\" labelText=\"\" answerConceptIds=\"1065,1066\" answerLabels=\"Sim, Não\"/&gt;&lt;/td&gt;\r\n  &lt;/tr&gt;\r\n  &lt;tr&gt;\r\n    &lt;td&gt;&lt;div align=\"right\"&gt;Qual é o número do campo?&lt;/div&gt;&lt;/td&gt;\r\n    &lt;td&gt;&lt;obs id=\"nomeCamp\" conceptId=\"23857\" labelText=\"\"/&gt;&lt;/td&gt;\r\n  &lt;/tr&gt;\r\n  \r\n  &lt;tr&gt;\r\n    &lt;td colspan=\"2\"&gt;&lt;div align=\"center\"&gt;\r\n   &lt;submit submitLabel=\"Submeter\"/&gt;\r\n  &lt;/div&gt;\r\n    &lt;/td&gt;\r\n  &lt;/tr&gt;\r\n  &lt;/tbody&gt;\r\n&lt;/table&gt;\r\n\r\n&lt;/body&gt;\r\n&lt;/html&gt;\r\n&lt;/htmlform&gt;</t>
+    <t>&lt;htmlform&gt;\r\n  &lt;script type=\"text/javascript\"&gt;\r\n  \r\n  jQuery(function() {\r\n    getField(\'levaCamp.value\').change(function(){\r\n     if(getValue(\'levaCamp.value\') == 1065) {\r\n        getField(\'nomeCamp.value\').show();\r\n      } \r\n      else{\r\n       setValue(\'nomeCamp.value\',\'\');\r\n        getField(\'nomeCamp.value\').hide();\r\n      }\r\n    })\r\n  });\r\n      \r\n    //Validações antes de submter\r\n   beforeSubmit.push(function() {  \r\n      \r\n      //Data de proximo levantamento  \r\n      var dataProximoLev = new Date(getValue(\'dataProxima.value\'));\r\n     \r\n      //Data da consulta seleccionada\r\n     var dataConsulta = new Date(getValue(\'dataConsulta.value\'));\r\n  \r\n      //Ultimo estadio do paciente\r\n      var lastRegime = parseInt(\"&lt;lookup expression=\"fn.latestObs(1088).valueCoded\"/&gt;\");\r\n      //Estadio Seleccionado\r\n      var selectedRegime = parseInt(getValue(\'regime.value\'));  \r\n      \r\n      //Data de Nascimento  \r\n      var dataNascimento = new Date(Date.parse(\"&lt;lookup expression=\"patient.birthdate\"/&gt;\"));\r\n\r\n           //Modo de dispensa seleccionado\r\n    var selectedDispenseMode = parseInt(getValue(\'modoDeDispensa.value\'));  \r\n\r\nif (isNaN(selectedDispenseMode)){      \r\n    alert(\"Modo de dispensa não foi seleccionado!\")\r\n  }\r\n      \r\n      //Data de inicio de TARV\r\n      //var dataInicioTARV = \"&lt;lookup expression=\"fn.latestObs(1190).valueDatetime\"/&gt;\";\r\n     \r\n      var estadoProgramaTarvConceptID = parseInt(\"&lt;lookup expression=\"fn.currentProgramWorkflowStatus(2).state.concept.id\" /&gt;\")\r\n  \r\n         \r\n      if (isNaN(estadoProgramaTarvConceptID)){      \r\n        getField(\'dataConsulta.error\').html(\'Deve admitir este paciente no programa de TARV - TRATAMENTO\').show();\r\n        return false;     \r\n      }else{\r\n        if(!((estadoProgramaTarvConceptID==6269) || (estadoProgramaTarvConceptID==1369))){\r\n          getField(\'dataConsulta.error\').html(\'Este paciente não está no estado activo no programa, coloque-o como activo primeiro\').show();\r\n          return false; \r\n        }\r\n     }\r\n     \r\n      \r\n      //Compara se a data de levantamento e menor que data de nascimento\r\n      //if (dataInicioTARV == \'\') {         \r\n      //    getField(\'dataConsulta.error\').html(\'O Paciente não tem data de inicio de TARV registado na Ficha de Seguimento (Antigo) ou Ficha Resumo (Master Card)\').show();\r\n      //    return false;           \r\n      //}\r\n     \r\n      //Compara se a data da proxima é menor que a data de levantamento \r\n      if (dataProximoLev &amp;lt;=  dataConsulta) {         \r\n          getField(\'dataProxima.error\').html(\'A data do proximo levantamento não deve ser menor ou igual que a data de levantamento\').show();\r\n         return false;           \r\n      }\r\n  \r\n     //Compara se a data de levantamento e menor que data de nascimento\r\n      if (dataConsulta &amp;lt;  dataNascimento) {          \r\n          getField(\'dataConsulta.error\').html(\'A data do levantamento não deve ser menor que a data de nascimento\').show();\r\n         return false;           \r\n      }   \r\n      \r\n      \r\n        \r\n        if(lastRegime != selectedRegime){\r\n         var confirmacao=window.confirm(\'Confirma a mudança de regime deste paciente?\');\r\n         if(confirmacao == false)\r\n          return false;\r\n       }\r\n     \r\n          $j(\'.submitButton\').prop(\'disabled\', true);   \r\n              \r\n      return true;\r\n    }); \r\n    \r\n  &lt;/script&gt;\r\n  &lt;html xmlns=\"http://www.w3.org/1999/xhtml\"&gt;\r\n  &lt;head&gt;\r\n  &lt;meta http-equiv=\"Content-Type\" content=\"text/html; charset=utf-8\" /&gt;\r\n  &lt;title&gt;FILA&lt;/title&gt;\r\n    \r\n    &lt;style&gt;\r\n       h2 { border-bottom: 3px solid red; }\r\n        p { border: 1px solid black; }\r\n        table{\r\n          border-color: #600;\r\n         border-width: 0 0 1px 1px;\r\n          border-style: solid;}\r\n  \r\n       td{\r\n         border-color: #600;\r\n         border-width: 1px 1px 0 0;\r\n          border-style: solid;\r\n          margin: 0;\r\n          padding: 4px;\r\n         background-color: #B2DFEE;}\r\n       .style1 {\r\n         font-size: 14px;\r\n          font-weight: bold;}\r\n       .section {\r\n          border: 1px solid $headerColor;\r\n         padding: 2px;\r\n         text-align: center;\r\n         margin-bottom: 1em;\r\n         border-width:thin;\r\n          width:50%;\r\n          vertical-align:middle;\r\n          azimuth:center;}\r\n        .sectionHeader {\r\n          background-color: $headerColor;\r\n         color: $fontOnHeaderColor;\r\n          display: block;\r\n         padding: 2px;\r\n         font-weight: bold;}\r\n       table.baseline-aligned td {\r\n         vertical-align: baseline;}\r\n    &lt;/style&gt;\r\n  &lt;/head&gt;\r\n  &lt;body&gt;\r\n  &lt;table width=\"900\" border=\"1\" align=\"center\"&gt;\r\n    &lt;tbody align=\"left\" style=\"font-family:verdana; font-size:12px\"&gt;\r\n    &lt;tr&gt;\r\n      &lt;td width=\"285\" rowspan=\"4\"&gt;REPÚBLICA DE MOÇAMBIQUE&lt;br/&gt;Serviço Nacional de Saúde&lt;/td&gt;\r\n      &lt;td colspan=\"2\"&gt;&lt;div align=\"center\" class=\"style1\"&gt;Ficha Individual de Levantamento de ARVs (FILA)&lt;/div&gt;&lt;/td&gt;\r\n    &lt;/tr&gt;\r\n    &lt;tr&gt;\r\n      &lt;td colspan=\"2\"&gt;\r\n       Nº do Livro TARV:&lt;lookup expression=\"fn.latestObs(6264).getValueAsString($!{locale})\"/&gt;   \r\n       Pag: &lt;lookup expression=\"fn.latestObs(6266).getValueAsString($!{locale})\"/&gt;  \r\n       Linha: &lt;lookup expression=\"fn.latestObs(6268).getValueAsString($!{locale})\"/&gt;  \r\n      &lt;/td&gt;\r\n      &lt;/tr&gt;\r\n    &lt;tr&gt;\r\n      &lt;td width=\"245\"&gt;&lt;div align=\"right\"&gt;Nome:&lt;/div&gt;&lt;/td&gt;\r\n      &lt;td width=\"348\"&gt;&lt;lookup expression=\"patient.personName\"/&gt;&lt;/td&gt;\r\n    &lt;/tr&gt;\r\n    &lt;tr&gt;\r\n      &lt;td&gt;&lt;div align=\"right\"&gt;Contacto:&lt;/div&gt;&lt;/td&gt;\r\n      &lt;td&gt;&lt;lookup expression=\"patient.getAttribute(9)\"/&gt;&lt;/td&gt;\r\n    &lt;/tr&gt;\r\n    &lt;tr&gt;\r\n      &lt;td&gt;NID: &lt;lookup expression=\"patient.getPatientIdentifier(2)\"/&gt;\r\n                      &lt;lookup expression=\"patient.getPatientIdentifier(14)\"/&gt;\r\n  \r\n  &lt;/td&gt;\r\n      &lt;td&gt;&lt;div align=\"right\"&gt;Endereço:&lt;/div&gt;&lt;/td&gt;\r\n      &lt;td&gt;&lt;lookup complexExpression=\"#foreach( $addr in $patient.addresses ) $!addr.subregion #end\"/&gt;&lt;/td&gt;\r\n    &lt;/tr&gt;\r\n    \r\n    &lt;/tbody&gt;\r\n  &lt;/table&gt;\r\n  \r\n  &lt;br/&gt;\r\n  \r\n  &lt;table width=\"900\" border=\"1\" align=\"center\"&gt;\r\n    &lt;tbody align=\"left\" style=\"font-family:verdana; font-size:12px\"&gt;\r\n    \r\n    \r\n    &lt;tr&gt;\r\n      &lt;td&gt;&lt;div align=\"right\"&gt;Data de Levantamento:&lt;/div&gt;&lt;/td&gt;\r\n      &lt;td&gt;&lt;encounterDate id=\"dataConsulta\"/&gt;&lt;/td&gt;\r\n    &lt;/tr&gt;\r\n    &lt;tr&gt;\r\n      &lt;td&gt;&lt;div align=\"right\"&gt;Provedor:&lt;/div&gt;&lt;/td&gt;\r\n      &lt;td&gt;&lt;encounterProvider role=\"Provider\" type=\"autocomplete\"/&gt;&lt;/td&gt;\r\n    &lt;/tr&gt;\r\n    &lt;tr&gt;\r\n      &lt;td&gt;&lt;div align=\"right\"&gt;Unidade Sanitária:&lt;/div&gt;&lt;/td&gt;\r\n      &lt;td&gt;\r\n   &lt;encounterLocation id=\"localConsulta\" default=\"GlobalProperty:default_location\" type=\"autocomplete\"/&gt;\r\n   &lt;/td&gt;\r\n    &lt;/tr&gt;\r\n    &lt;tr&gt;\r\n      &lt;td width=\"40%\"&gt;&lt;div align=\"right\"&gt;Medicamentos ARVs:&lt;/div&gt;&lt;/td&gt;\r\n      &lt;td width=\"60%\"&gt;Ultimo Regime:\r\n        &lt;strong&gt;\r\n        &lt;lookup expression=\"fn.latestObs(1088).getValueAsString($!{locale})\"/&gt;&lt;/strong&gt;&lt;br /&gt;\r\n        \r\n     \r\n      &lt;obs id=\"regime\" conceptId=\"e1d83e4e-1d5f-11e0-b929-000c29ad1d07\" answerConceptIds=\"\r\n                                              e1de19fe-1d5f-11e0-b929-000c29ad1d07,\r\n                                              28b28521-b6cd-454e-9ec5-f2c6c9c58468,\r\n                                              e1dd2f44-1d5f-11e0-b929-000c29ad1d07,\r\n                                              9dc17c1b-7b6d-488e-a38d-505a7b65ec82,\r\n                                              2e44e77e-eac4-4f64-84d2-73d32abf94d5,\r\n                                              78419317-cdda-42e9-92a3-13cb0cbf0020,\r\n                                              e3f6bb60-e2cf-46cb-a9da-27d634ba8607,\r\n                                              af15246d-30b8-4aff-8391-ca2b58e2c88b,\r\n                                              3e7f46c7-a971-4c0c-82aa-a65589fd518e,\r\n                                              cf05347e-063c-4896-91a4-097741cf6be6,\r\n                                              e11be52e-0da1-4d32-ab5c-e0feb9b6abd6,\r\n                                              f8c5d365-7636-4449-9acd-c83c4fd2ea01,\r\n                                              d5f9d629-67bc-4f60-9e12-629e6d2c1d08,\r\n                                              7bf5a88d-6db6-4899-a01a-bfd14ce77b53,\r\n                                              e8b741b3-463c-46b1-8423-a16f736af8d4,\r\n                                              ba25f2b5-4216-4605-9e6b-1f591033dc3e,\r\n                                              7d18d08c-d1a8-4dc8-8d65-02197b42acf7,\r\n                                              c22c4431-a27e-4054-92bb-a1563482003e,\r\n                                              c4a56680-ac6e-4538-8126-e3097b7b4789,\r\n                                              8f9c4e58-0d70-4b09-a109-e776d325e9fd,\r\n                                              9cb63f72-4c08-4543-878a-537dcabe5670,\r\n                                              46b8a2ab-36a7-4072-ab62-0af9b3b58e72,\r\n                                              552dd71f-d1de-426a-a19c-49b8706a4a7f,\r\n                                              f32e013c-38c8-483a-8012-88596e8b13da,\r\n                                              c30f826d-9433-4e63-ac91-dbbc158686ff,\r\n                                              e1e59e0e-1d5f-11e0-b929-000c29ad1d07\" labelText=\"\" answerLabels=\"AZT+3TC+EFV,\r\n                                                                                                              AZT+3TC+LPV/r,\r\n                                                                                                              AZT+3TC+NVP,\r\n                                                                                                              TDF+3TC+EFV,\r\n                                                                                                              TDF+3TC+NVP,\r\n                                                                                                              ABC+3TC+EFV,\r\n                                                                                                              TDF+3TC+DTG,\r\n                                                                                                              ABC+3TC+DTG,\r\n                                                                                                              AZT+3TC+ABC,\r\n                                                                                                              ABC+3TC+LPV/r,\r\n                                                                                                              ABC+3TC+NVP,\r\n                                                                                                              TDF+3TC+LPV/r,\r\n                                                                                                              TDF+3TC+LPV/r+RTV,\r\n                                                                                                              TDF+3TC+ATV/r,\r\n                                                                                                              ABC+3TC+ATV/r,\r\n                                                                                                              AZT+3TC+ATV/r,\r\n                                                                                                              ABC+3TC+ATV/r+RAL,\r\n                                                                                                              TDF+3TC+ATV/r+RAL,\r\n                                                                                                              AZT+3TC+RAL,\r\n                                                                                                              AZT+3TC+DRV/r,\r\n                                                                                                              AZT+3TC+DTG,\r\n                                                                                                              TDF+3TC+RAL+DRV/r,\r\n                                                                                                              ABC+3TC++RAL+DRV/r,\r\n                                                                                                              3TC+RAL+DRV/r,\r\n                                                                                                              AZT+3TC+RAL+DRV/r,\r\n                                                                                                              OUTRO\" required=\"true\"/&gt;\r\n     \r\n      \r\n      &lt;/td&gt;\r\n    &lt;/tr&gt;  \r\n    &lt;tr&gt;\r\n      &lt;td&gt;&lt;div align=\"right\"&gt;Quantidade Aviada:&lt;/div&gt;&lt;/td&gt;\r\n      &lt;td&gt;&lt;obs id=\"quantidadeAviada\" conceptId=\"1715\" labelText=\"\" answers=\"15,30,45,60,90,120,180\" answerLabels=\"15,30,45,60,90,120,180\"/&gt; - &lt;obs conceptId=\"1715\" labelText=\"Outra:\"/&gt;&lt;/td&gt;\r\n    &lt;/tr&gt;\r\n    &lt;tr&gt;\r\n      &lt;td&gt;&lt;div align=\"right\"&gt;Dosagem:&lt;/div&gt;&lt;/td&gt;\r\n      &lt;td&gt;&lt;obs id=\"posologia\" conceptId=\"1711\" labelText=\"\" answers=\"1-0-1,0-0-1,1-0-0,2-0-2,3-0-3,0-0-3,1-0-2,1-0-1.5\" answerLabels=\"1-0-1,0-0-1,1-0-0,2-0-2,3-0-3,0-0-3,1-0-2,1-0-1.5\"/&gt; - &lt;obs conceptId=\"1711\" labelText=\"Outra:\" size=\"8\"/&gt;&lt;/td&gt;\r\n    &lt;/tr&gt;\r\n    &lt;tr&gt;\r\n      &lt;td&gt;&lt;div align=\"right\"&gt;Data do próximo Levantamento:&lt;/div&gt;&lt;/td&gt;\r\n      &lt;td&gt;&lt;obs id=\"dataProxima\" conceptId=\"5096\" labelText=\"\" allowFutureDates=\"true\" required=\"true\"/&gt;&lt;/td&gt;\r\n    &lt;/tr&gt;\r\n     &lt;tr&gt;\r\n      &lt;td&gt;&lt;div align=\"right\"&gt;Levantamento efectuado num campo de acomodação?&lt;/div&gt;&lt;/td&gt;\r\n      &lt;td&gt;&lt;obs id=\"levaCamp\" conceptId=\"23856\" labelText=\"\" answerConceptIds=\"1065,1066\" answerLabels=\"Sim, Não\"/&gt;&lt;/td&gt;\r\n    &lt;/tr&gt;\r\n    &lt;tr&gt;\r\n      &lt;td&gt;&lt;div align=\"right\"&gt;Qual é o número do campo?&lt;/div&gt;&lt;/td&gt;\r\n      &lt;td&gt;&lt;obs id=\"nomeCamp\" conceptId=\"23857\" labelText=\"\"/&gt;&lt;/td&gt;\r\n    &lt;/tr&gt;\r\n  &lt;tr&gt;\r\n      &lt;td&gt;&lt;div align=\"right\"&gt;Modo de Dispensa&lt;/div&gt;&lt;/td&gt;\r\n      &lt;td&gt;     \r\n        &lt;obs id=\"modoDeDispensa\" conceptId=\"40a9a12b-1205-4a55-bb93-caf15452bf61\" answerConceptIds=\"4b51ace2-f778-4f54-bdaa-be2b350b7499,\r\n        1309d08a-5c73-4429-8f4b-43a551952858,\r\n        d2eaec39-9c48-443b-a8d5-b2b163d42c53,\r\n        870e2d25-c5ef-4e36-89db-0a4a37af214e,\r\n        0843c71b-be47-4de2-ba16-a08db52c1136,\r\n        3ab58d0e-f831-4966-97bd-209738f5e4df,\r\n        d6ad74a1-ff67-4b81-afa1-a0d906462623,\r\n        467718bc-1756-4b3f-b1ee-98d01910153a,\r\n        091737af-d6bf-4830-8e87-82572ffac9ea\r\n        \" labelText=\"\" answerLabels=\"Horário Normal de Expediente,\r\n        Fora do Horário,\r\n        FARMAC/Farmácia privada,\r\n        Dispensa Comunitária via Provedor,\r\n        Dispensa Comunitária via APE,\r\n        Brigadas Móveis Diurnas,\r\n        Brigadas Móveis Nocturnas (Hotspots),\r\n        Clínicas Móveis Diurnas,\r\n        Clínicas Móveis Nocturnas (Hotspots)\" /&gt;&lt;/td&gt;\r\n    &lt;/tr&gt;\r\n    &lt;tr&gt;\r\n      &lt;td colspan=\"2\"&gt;&lt;div align=\"center\"&gt;\r\n     &lt;submit submitLabel=\"Submeter\"/&gt;\r\n    &lt;/div&gt;\r\n      &lt;/td&gt;\r\n    &lt;/tr&gt;\r\n    &lt;/tbody&gt;\r\n  &lt;/table&gt;\r\n  \r\n  &lt;/body&gt;\r\n  &lt;/html&gt;\r\n  &lt;/htmlform&gt;</t>
   </si>
   <si>
     <t>b30f1085-fc70-4258-aa5f-5c5f3bc2f3b1</t>
@@ -966,15 +966,13 @@
     <t>7d8a6c2e-6398-49ab-aa22-3125718013b8</t>
   </si>
   <si>
-    <t>&lt;htmlform&gt;\r\n\r\n        &lt;html xmlns=\"http://www.w3.org/1999/xhtml\"&gt;\r\n        &lt;head&gt;\r\n        &lt;meta http-equiv=\"Content-Type\" content=\"text/html; charset=utf-8\" /&gt;\r\n        &lt;title&gt;FILA&lt;/title&gt;\r\n            \r\n        &lt;style&gt;\r\n                h2 { border-bottom: 3px solid red; }\r\n                p { border: 1px solid black; }\r\n                \r\n                \r\n                table{\r\n                    border: 3px solid #1aac9b;\r\n                    border-collapse: collapse;\r\n                }\r\n    \r\n                tr:first-child {\r\n                    background-color: #1aac9b;\r\n                }\r\n    \r\n                tr:first-child label {\r\n                    padding: 4px !important;\r\n                    color: #fff;\r\n                    font-weight: bold;\r\n                    margin: 4px !important;\r\n                    text-shadow: 0 0 .3em black;\r\n                    font-size: 12pt;\r\n                }\r\n    \r\n                td {\r\n                    border: 1px solid #1aac9b;\r\n                }\r\n                    \r\n            .style1 {\r\n                font-size: 14px;\r\n                font-weight: bold;\r\n            }\r\n    \r\n            .obs{\r\n                font-size: 14px;\r\n                font-weight: bold;\r\n            }\r\n    \r\n            .submit-btn {\r\n                        flex: 1;\r\n                        margin: 10px 15px;\r\n                    }\r\n    \r\n            .submit-btn input{\r\n                color: #fff;\r\n                background: #1aac9b;\r\n                padding: 8px;\r\n                width: 12.8em;\r\n                font-weight: bold;\r\n                text-shadow: 0 0 .3em black;\r\n                font-size: 9pt;\r\n                border-radius: 5px 5px;\r\n            }\r\n        &lt;/style&gt;\r\n        &lt;script type=\"text/javascript\"&gt;\r\n            function findAutoCompleteErrors() {\r\n                /* see if there are  errors in option fields */\r\n                var containError = false;\r\n                var ary = $j(\".optionAutoCompleteHidden\");\r\n                $j.each(ary,function(index, value){\r\n                    if(value.value == \"ERROR\"){\r\n                        containError=true;\r\n                    }\r\n                });\r\n                return containError;\r\n            }\r\n            $j(function() {\r\n                $j(\'.submitButton\').click(function(event) {\r\n                    if(!findAutoCompleteErrors()){\r\n                        $j(\'.submitButton\').prop(\'disabled\', true);\r\n                    }\r\n                });\r\n            });\r\n        &lt;/script&gt;\r\n        &lt;/head&gt;\r\n        &lt;body&gt;\r\n        &lt;table width=\"900\" border=\"1\" align=\"center\"&gt;\r\n          &lt;tbody align=\"left\" style=\"font-family:verdana; font-size:12px\"&gt;\r\n          &lt;tr&gt;\r\n            &lt;td width=\"285\" rowspan=\"4\" align=\"center\"&gt;REPÚBLICA DE MOÇAMBIQUE&lt;br/&gt;Serviço Nacional de Saúde &lt;br/&gt;&lt;br/&gt; NID: &lt;lookup expression=\"patient.getPatientIdentifier(2)\"/&gt;&lt;/td&gt;\r\n            &lt;td colspan=\"2\"  height=\"30\" &gt;&lt;div align=\"center\" class=\"style1\"&gt;&lt;label&gt;Registo de Levantamento de ARVs Master Card&lt;/label&gt;&lt;/div&gt;&lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          \r\n          &lt;tr&gt;\r\n            &lt;td width=\"245\"&gt;&lt;div align=\"right\"&gt;Nome:&lt;/div&gt;&lt;/td&gt;\r\n            &lt;td width=\"348\"&gt;&lt;lookup expression=\"patient.personName\"/&gt;&lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;&lt;div align=\"right\"&gt;Contacto:&lt;/div&gt;&lt;/td&gt;\r\n            &lt;td&gt;&lt;lookup expression=\"patient.getAttribute(9)\"/&gt;&lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;&lt;div align=\"right\"&gt;Endereço:&lt;/div&gt;&lt;/td&gt;\r\n            &lt;td&gt;&lt;lookup complexExpression=\"#foreach( $addr in $patient.addresses ) $!addr.subregion #end\"/&gt;&lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          \r\n          &lt;/tbody&gt;\r\n        &lt;/table&gt;\r\n        \r\n        &lt;br/&gt;\r\n        \r\n        &lt;table width=\"900\" border=\"1\" align=\"center\"&gt;\r\n          &lt;tbody align=\"left\" style=\"font-family:verdana; font-size:12px\"&gt;\r\n          \r\n          &lt;tr&gt;\r\n            &lt;td&gt;&lt;div align=\"right\"&gt;Unidade Sanitária:&lt;/div&gt;&lt;/td&gt;\r\n            &lt;td&gt;\r\n        &lt;encounterLocation id=\"localConsulta\" default=\"GlobalProperty:default_location\" type=\"autocomplete\"/&gt; \r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;  \r\n            \r\n          &lt;tr style=\"display: none;\"&gt;\r\n            &lt;td&gt;&lt;div align=\"right\"&gt;Recepcionista:&lt;/div&gt;&lt;/td&gt;\r\n            &lt;td&gt;&lt;encounterProvider role=\"Provider\" default=\"generic.provider\" widget=\"hidden\"/&gt;&lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          \r\n          &lt;tr&gt;\r\n            &lt;td&gt;&lt;div align=\"right\"&gt;Data de Registo:&lt;/div&gt;&lt;/td&gt;\r\n            &lt;td&gt;&lt;encounterDate id=\"encounterDate\"  widget=\"hidden\" default=\"today\"/&gt;&lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          \r\n          \r\n          &lt;tr&gt;\r\n            &lt;td&gt;&lt;div align=\"right\"&gt;Levantou ARV:&lt;/div&gt;&lt;/td&gt;\r\n            &lt;td&gt;\r\n                &lt;obs conceptId=\"e07fb227-7a5a-4edf-93e8-7633c9fd1ea0\" labelText=\"\" answerConceptIds=\"e1d81b62-1d5f-11e0-b929-000c29ad1d07,e1d81c70-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"S, N\" style=\"radio\" required=\"true\"/&gt;\r\n                \r\n            &lt;/td&gt;\r\n          &lt;/tr&gt; \r\n          &lt;tr&gt;\r\n            &lt;td&gt;&lt;div align=\"right\"&gt;Data do Levantamento:&lt;/div&gt;&lt;/td&gt;\r\n            &lt;td&gt;  \r\n                &lt;obs id=\"dataLevantamento\" conceptId=\"74f6c17f-9819-41da-ba34-5910f67d24d0\" labelText=\"\" allowFutureDates=\"true\" required=\"true\"/&gt;  \r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td colspan=\"2\"&gt;&lt;div align=\"center\"&gt;\r\n                &lt;div class=\"submit-btn\"&gt;&lt;submit submitLabel=\"Submeter\"/&gt;&lt;/div&gt;\r\n            &lt;/div&gt;&lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;/tbody&gt;\r\n        &lt;/table&gt;\r\n        \r\n        &lt;/body&gt;\r\n        &lt;/html&gt;\r\n        &lt;/htmlform&gt;</t>
+    <t>&lt;htmlform&gt;\r\n\r\n        &lt;html xmlns=\"http://www.w3.org/1999/xhtml\"&gt;\r\n        &lt;head&gt;\r\n        &lt;meta http-equiv=\"Content-Type\" content=\"text/html; charset=utf-8\" /&gt;\r\n        &lt;title&gt;FILA&lt;/title&gt;\r\n            \r\n        &lt;style&gt;\r\n                h2 { border-bottom: 3px solid red; }\r\n                p { border: 1px solid black; }\r\n                \r\n                \r\n                table{\r\n                    border: 3px solid #1aac9b;\r\n                    border-collapse: collapse;\r\n                }\r\n    \r\n                tr:first-child {\r\n                    background-color: #1aac9b;\r\n                }\r\n    \r\n                tr:first-child label {\r\n                    padding: 4px !important;\r\n                    color: #fff;\r\n                    font-weight: bold;\r\n                    margin: 4px !important;\r\n                    text-shadow: 0 0 .3em black;\r\n                    font-size: 12pt;\r\n                }\r\n    \r\n                td {\r\n                    border: 1px solid #1aac9b;\r\n                }\r\n                    \r\n            .style1 {\r\n                font-size: 14px;\r\n                font-weight: bold;\r\n            }\r\n    \r\n            .obs{\r\n                font-size: 14px;\r\n                font-weight: bold;\r\n            }\r\n    \r\n            .submit-btn {\r\n                        flex: 1;\r\n                        margin: 10px 15px;\r\n                    }\r\n    \r\n            .submit-btn input{\r\n                color: #fff;\r\n                background: #1aac9b;\r\n                padding: 8px;\r\n                width: 12.8em;\r\n                font-weight: bold;\r\n                text-shadow: 0 0 .3em black;\r\n                font-size: 9pt;\r\n                border-radius: 5px 5px;\r\n            }\r\n        &lt;/style&gt;\r\n        &lt;script type=\"text/javascript\"&gt;\r\n            function findAutoCompleteErrors() {\r\n                /* see if there are  errors in option fields */\r\n                var containError = false;\r\n                var ary = $j(\".optionAutoCompleteHidden\");\r\n                $j.each(ary,function(index, value){\r\n                    if(value.value == \"ERROR\"){\r\n                        containError=true;\r\n                    }\r\n                });\r\n                return containError;\r\n            }\r\n            $j(function() {\r\n                $j(\'.submitButton\').click(function(event) {\r\n                    if(!findAutoCompleteErrors()){\r\n                        $j(\'.submitButton\').prop(\'disabled\', true);\r\n                    }\r\n                });\r\n            });\r\n\r\n            beforeSubmit.push(function() {\r\n                //Variaveis para lidar com a secção de TARV\r\n                \r\n                var dataLevan = new Date(getValue(\'dataLevantamento.value\'));\r\n                var dataBase = new Date(Date.parse(\'1985-12-31\'));\r\n                \r\n                if(dataLevan == null || dataLevan == \'\'){                       \r\n                        getField(\'dataLevantamento.error\').html(\'Deve indicar a data de Levantamento\').show();\r\n                        $j(\'.submitButton\').prop(\'disabled\', false);\r\n                        \r\n                        return false;\r\n                }\r\n                        \r\n                //Compara se a data da consulta é menor que a data de nascimento        \r\n                if (dataLevan &amp;lt;= dataBase) {                                  \r\n                        getField(\'dataLevantamento.error\').html(\'A data de levantamento deve ser superior a 31 de Dezembro de 1985\').show();\r\n                        $j(\'.submitButton\').prop(\'disabled\', false);\r\n                        \r\n                        return false;                  \r\n                }          \r\n                return true;\r\n        });\r\n\r\n        &lt;/script&gt;\r\n        &lt;/head&gt;\r\n        &lt;body&gt;\r\n        &lt;table width=\"900\" border=\"1\" align=\"center\"&gt;\r\n          &lt;tbody align=\"left\" style=\"font-family:verdana; font-size:12px\"&gt;\r\n          &lt;tr&gt;\r\n            &lt;td width=\"285\" rowspan=\"4\" align=\"center\"&gt;REPÚBLICA DE MOÇAMBIQUE&lt;br/&gt;Serviço Nacional de Saúde &lt;br/&gt;&lt;br/&gt; NID: &lt;lookup expression=\"patient.getPatientIdentifier(2)\"/&gt;&lt;/td&gt;\r\n            &lt;td colspan=\"2\"  height=\"30\" &gt;&lt;div align=\"center\" class=\"style1\"&gt;&lt;label&gt;Registo de Levantamento de ARVs Master Card&lt;/label&gt;&lt;/div&gt;&lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          \r\n          &lt;tr&gt;\r\n            &lt;td width=\"245\"&gt;&lt;div align=\"right\"&gt;Nome:&lt;/div&gt;&lt;/td&gt;\r\n            &lt;td width=\"348\"&gt;&lt;lookup expression=\"patient.personName\"/&gt;&lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;&lt;div align=\"right\"&gt;Contacto:&lt;/div&gt;&lt;/td&gt;\r\n            &lt;td&gt;&lt;lookup expression=\"patient.getAttribute(9)\"/&gt;&lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td&gt;&lt;div align=\"right\"&gt;Endereço:&lt;/div&gt;&lt;/td&gt;\r\n            &lt;td&gt;&lt;lookup complexExpression=\"#foreach( $addr in $patient.addresses ) $!addr.subregion #end\"/&gt;&lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          \r\n          &lt;/tbody&gt;\r\n        &lt;/table&gt;\r\n        \r\n        &lt;br/&gt;\r\n        \r\n        &lt;table width=\"900\" border=\"1\" align=\"center\"&gt;\r\n          &lt;tbody align=\"left\" style=\"font-family:verdana; font-size:12px\"&gt;\r\n          \r\n          &lt;tr&gt;\r\n            &lt;td&gt;&lt;div align=\"right\"&gt;Unidade Sanitária:&lt;/div&gt;&lt;/td&gt;\r\n            &lt;td&gt;\r\n        &lt;encounterLocation id=\"localConsulta\" default=\"GlobalProperty:default_location\" type=\"autocomplete\"/&gt; \r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;  \r\n            \r\n          &lt;tr style=\"display: none;\"&gt;\r\n            &lt;td&gt;&lt;div align=\"right\"&gt;Recepcionista:&lt;/div&gt;&lt;/td&gt;\r\n            &lt;td&gt;&lt;encounterProvider role=\"Provider\" default=\"generic.provider\" widget=\"hidden\"/&gt;&lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          \r\n          &lt;tr&gt;\r\n            &lt;td&gt;&lt;div align=\"right\"&gt;Data de Registo:&lt;/div&gt;&lt;/td&gt;\r\n            &lt;td&gt;&lt;encounterDate id=\"encounterDate\"  widget=\"hidden\" default=\"today\"/&gt;&lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          \r\n          \r\n          &lt;tr&gt;\r\n            &lt;td&gt;&lt;div align=\"right\"&gt;Levantou ARV:&lt;/div&gt;&lt;/td&gt;\r\n            &lt;td&gt;\r\n                &lt;obs conceptId=\"e07fb227-7a5a-4edf-93e8-7633c9fd1ea0\" labelText=\"\" answerConceptIds=\"e1d81b62-1d5f-11e0-b929-000c29ad1d07,e1d81c70-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"S, N\" style=\"radio\" required=\"true\"/&gt;\r\n                \r\n            &lt;/td&gt;\r\n          &lt;/tr&gt; \r\n          &lt;tr&gt;\r\n            &lt;td&gt;&lt;div align=\"right\"&gt;Data do Levantamento:&lt;/div&gt;&lt;/td&gt;\r\n            &lt;td&gt;  \r\n                &lt;obs id=\"dataLevantamento\" conceptId=\"74f6c17f-9819-41da-ba34-5910f67d24d0\" labelText=\"\" allowFutureDates=\"true\" required=\"true\"/&gt;  \r\n            &lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;tr&gt;\r\n            &lt;td colspan=\"2\"&gt;&lt;div align=\"center\"&gt;\r\n                &lt;div class=\"submit-btn\"&gt;&lt;submit submitLabel=\"Submeter\"/&gt;&lt;/div&gt;\r\n            &lt;/div&gt;&lt;/td&gt;\r\n          &lt;/tr&gt;\r\n          &lt;/tbody&gt;\r\n        &lt;/table&gt;\r\n        \r\n        &lt;/body&gt;\r\n        &lt;/html&gt;\r\n        &lt;/htmlform&gt;</t>
   </si>
   <si>
     <t>597a00b1-ae77-4f40-b8c7-fb79783e8e56</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;htmlform&gt;\r\n        &lt;html xmlns=\"http://www.w3.org/1999/xhtml\"&gt;\r\n        &lt;head&gt;\r\n        &lt;meta http-equiv=\"Content-Type\" content=\"text/html; charset=utf-8\" /&gt;\r\n        &lt;title&gt;FICHA RESUMO&lt;/title&gt;\r\n          \r\n          &lt;style&gt;\r\n    \r\n            .main{\r\n                display: flex;\r\n                align-items: center;\r\n                flex-direction: column;\r\n                font-size: .9em;\r\n                width: 100%;\r\n            }\r\n    \r\n            .header-box{\r\n                width: 80%;\r\n                background: #1aac9b;\r\n                padding: 1px !important;\r\n                color: #fff;\r\n                box-shadow: 0 0 .3em #000;\r\n                margin-bottom: 10px;\r\n            }\r\n            \r\n            .content {\r\n                display: flex;\r\n                flex-flow: row wrap;\r\n                width: 80%;\r\n                border: 1px solid #1aac9b;\r\n                box-shadow: 0 0 .3em #000;\r\n            }\r\n    \r\n            .line-break {\r\n                width: 100%;\r\n            }\r\n    \r\n            .header, .space-between{\r\n                display: flex;\r\n                flex-flow: row wrap;\r\n                justify-content: space-between;\r\n                align-content: space-between;\r\n                width: 100%\r\n            }\r\n    \r\n            .header-data{\r\n              border: 1px solid #1aac9b;\r\n              margin-bottom: 10px !important;\r\n              padding: 0px 10px 0px 10px;\r\n              box-shadow: 0 0 .1em #000;\r\n              margin: 10px 10px;\r\n              background: #dedede\r\n            }\r\n    \r\n            .header-info{\r\n              border: 1px solid #1aac9b;\r\n              padding: 0px 10px 0px 10px;\r\n              box-shadow: 0 0 .1em #000;\r\n              margin: 10px 10px;\r\n              background: #dedede\r\n            }\r\n    \r\n            .header-box h2{\r\n               padding-left: 10px;\r\n               text-shadow: 0 0 .3em #000;\r\n            }\r\n    \r\n    \r\n            .header-info h3{\r\n              text-align: center;\r\n            }\r\n    \r\n            input[type=\"text\"]{\r\n                width: 150px;\r\n                margin-bottom: 4px;\r\n            }\r\n    \r\n            .input-size input[type=\"text\"]{\r\n                width: 50px !important;\r\n            }\r\n    \r\n            .input-size-2 input[type=\"text\"]{\r\n                width: 70px !important;\r\n            }\r\n    \r\n            p select {\r\n                width: 150px;\r\n                margin-bottom: 4px;\r\n            }\r\n    \r\n            .base-margin {\r\n                margin-left: 15px;\r\n            }\r\n    \r\n            .submit-btn {\r\n                flex: 1;\r\n                margin: 10px 15px;\r\n            }\r\n    \r\n             .submit-btn input{\r\n               color: #fff;\r\n               background: #1aac9b;\r\n               padding: 8px;\r\n               width: 12.8em;\r\n               font-weight: bold;\r\n               text-shadow: 0 0 .3em black;\r\n               font-size: 9pt;\r\n               border-radius: 5px 5px;\r\n            }\r\n    \r\n            .label-tag {\r\n               color: #fff;\r\n               background: #1aac9b;\r\n               padding: 7px;\r\n               font-weight: bold;\r\n               text-shadow: 0 0 .3em black;\r\n               font-size: 9pt;\r\n               border-radius: 5px 5px;\r\n               width: 100%;\r\n               display: inline-block;\r\n            }\r\n    \r\n            .input-with-size input[type=\"text\"]{\r\n                width : 50px !important;\r\n            }\r\n    \r\n            .input-with-size-lg input[type=\"text\"]{\r\n                width : 400px !important;\r\n            }\r\n    \r\n            .hasDatepicker{\r\n                width : 80px !important;\r\n            }\r\n\r\n            .boder-in {\r\n                margin-top: -14px;\r\n                margin-bottom: -22px;\r\n            }\r\n\r\n           .space-justify {\r\n                display: flex;\r\n                flex-flow: row wrap;\r\n                justify-content:baseline;;\r\n                align-content: flex-start;\r\n                width: 100%\r\n            }\r\n\r\n            .base-width {\r\n                width: 152px;\r\n            }\r\n\r\n            .space-justify label {\r\n                font-weight: bold;\r\n            }\r\n\r\n            #sociais select {\r\n                width: 289px;\r\n            }\r\n    \r\n            &lt;/style&gt;\r\n            &lt;script type=\"text/javascript\"&gt;\r\n                    function findAutoCompleteErrors() {\r\n                        /* see if there are  errors in option fields */\r\n                        var containError = false;\r\n                        var ary = $j(\".optionAutoCompleteHidden\");\r\n                        $j.each(ary,function(index, value){\r\n                            if(value.value == \"ERROR\"){\r\n                                containError=true;\r\n                            }\r\n                        });\r\n                        return containError;\r\n                    }\r\n                    $j(function() {\r\n                        $j(\'.submitButton\').click(function(event) {\r\n                            if(!findAutoCompleteErrors()){\r\n                                $j(\'.submitButton\').prop(\'disabled\', true);\r\n                            }\r\n                        });\r\n                    });\r\n            &lt;/script&gt;            \r\n            \r\n        &lt;/head&gt;\r\n        &lt;body&gt;\r\n            \r\n        &lt;div class=\"main\"&gt;\r\n            \r\n            &lt;div class=\"header-box\"&gt;\r\n                &lt;h2&gt;FICHA RESUMO&lt;/h2&gt;\r\n            &lt;/div&gt;\r\n    \r\n            &lt;div class=\"content\"&gt;\r\n    \r\n                    &lt;div class=\"header\"&gt;\r\n    \r\n                        &lt;div class=\"header-data\"&gt;\r\n                                &lt;p&gt;\r\n                                &lt;label&gt;Nome:&lt;/label&gt;\r\n                                &lt;lookup expression=\"patient.personName\"/&gt;\r\n                            &lt;/p&gt;\r\n    \r\n                            &lt;p&gt;\r\n                                &lt;label&gt;Género/Data de Nasc./Idade:&lt;/label&gt;\r\n                                &lt;lookup expression=\"patient.gender\"/&gt; - &lt;lookup expression=\"patient.birthdate\"/&gt; - &lt;lookup expression=\"patient.age\"/&gt;\r\n                            &lt;/p&gt;\r\n                        &lt;/div&gt;\r\n    \r\n                        &lt;div class=\"header-info\"&gt;\r\n                            &lt;h3&gt;REPÚBLICA DE MOÇAMBIQUE&lt;/h3&gt;\r\n                            &lt;h3&gt;SERVIÇO NACIONAL DE SAÚDE&lt;/h3&gt;\r\n                            &lt;p&gt;\r\n                                &lt;label&gt;NID:&lt;lookup expression=\"patient.getPatientIdentifier(2)\"/&gt;&lt;/label&gt;\r\n                            &lt;/p&gt;\r\n                        &lt;/div&gt;\r\n    \r\n                    &lt;/div&gt;\r\n                    \r\n                    &lt;div class=\"line-break\"&gt;&lt;/div&gt;\r\n    \r\n                    &lt;div class=\"base-margin\"&gt;\r\n    \r\n                        &lt;label class=\"label-tag\"&gt;Livros: Pré-TARV&lt;/label&gt;   \r\n    \r\n                        &lt;p class=\"input-size-2\"&gt;\r\n                            &lt;obs conceptId=\"d8ec9c7c-6b46-435b-8c80-3967f396bd71\" labelText=\"Nr. do Livro:\" /&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"c02181e6-8f9f-4387-9cf6-9a3d0f45b7fc\" labelText=\"Página:\" /&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"bf958c27-fa29-4b95-a055-a9d2d162ef76\" labelText=\"Linha:\" /&gt;\r\n                        &lt;/p&gt;\r\n    \r\n                    &lt;/div&gt;\r\n    \r\n                    &lt;div class=\"base-margin\"&gt;\r\n                        &lt;label class=\"label-tag\"&gt;Livros: TARV&lt;/label&gt;   \r\n    \r\n                        &lt;p class=\"input-size-2\"&gt;\r\n                            &lt;obs conceptId=\"39a21629-cf4e-45f3-be2e-287cce2d5d4c\" labelText=\"Nr. do Livro:\" /&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"9a9b36c9-ace0-40e9-a296-e547197358df\" labelText=\"Página:\" /&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"65be2cd1-8c97-41f8-9ff9-665d54479943\" labelText=\"Linha:\" /&gt;\r\n                        &lt;/p&gt;\r\n                    &lt;/div&gt;\r\n    \r\n                    &lt;div class=\"line-break\"&gt;&lt;/div&gt;\r\n    \r\n                    &lt;div class=\"base-margin\"&gt;\r\n    \r\n                        &lt;p&gt;\r\n                            &lt;label&gt;Unidade Sanitária:&lt;/label&gt;\r\n                            &lt;encounterLocation id=\"localConsulta\" default=\"GlobalProperty:default_location\" type=\"autocomplete\"/&gt;\r\n                        &lt;/p&gt;\r\n    \r\n                    &lt;/div&gt;\r\n    \r\n                    &lt;div class=\"line-break\"&gt;&lt;/div&gt;\r\n    \r\n                    &lt;div class=\"base-margin\"&gt;\r\n    \r\n                        &lt;p&gt;\r\n                            &lt;label&gt;Data Abertura da Ficha:&lt;/label&gt;                                \r\n                            &lt;obs conceptId=\"68d65d0c-8fee-456b-8e95-caed990351e1\" required=\"true\" /&gt;\r\n                        &lt;/p&gt;\r\n    \r\n                    &lt;/div&gt;\r\n    \r\n                    &lt;div class=\"base-margin\"&gt;\r\n    \r\n                        &lt;p&gt;\r\n                            &lt;label&gt;Profissão:&lt;/label&gt;\r\n                            &lt;obs conceptId=\"e1dc07c2-1d5f-11e0-b929-000c29ad1d07\" /&gt;\r\n                        &lt;/p&gt; \r\n    \r\n                    &lt;/div&gt;\r\n    \r\n                    &lt;div class=\"base-margin\"&gt;\r\n    \r\n                        &lt;p&gt;\r\n                            &lt;label&gt;Nível de Escolaridade:&lt;/label&gt;\r\n                            &lt;obs conceptId=\"e1db0700-1d5f-11e0-b929-000c29ad1d07\" answerConceptIds=\"e1db08fe-1d5f-11e0-b929-000c29ad1d07, e1db09f8-1d5f-11e0-b929-000c29ad1d07, e1db0af2-1d5f-11e0-b929-000c29ad1d07, e1db0bf6-1d5f-11e0-b929-000c29ad1d07\" /&gt;\r\n                        &lt;/p&gt;  \r\n    \r\n                    &lt;/div&gt;\r\n    \r\n                    &lt;div class=\"line-break\"&gt;&lt;/div&gt;\r\n    \r\n                    &lt;div class=\"base-margin\"&gt;\r\n                            &lt;label class=\"label-tag\"&gt;Confidente:&lt;/label&gt;   \r\n    \r\n                        &lt;p&gt;\r\n                            &lt;obs conceptId=\"e1de46a4-1d5f-11e0-b929-000c29ad1d07\" labelText=\"Nome:\" /&gt;\r\n                            &lt;obs conceptId=\"dbf852ab-697f-4c92-a546-74e5301de419\" labelText=\"Parentesco:\" /&gt; &lt;br/&gt;\r\n                            &lt;obs conceptId=\"eb23c94a-2c2e-40fa-ab82-22308b1c5f27\" labelText=\"Telefone Celular (1):\" /&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"eb23c94a-2c2e-40fa-ab82-22308b1c5f27\" labelText=\"Telefone Celular (2):\" /&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"e1e0c208-1d5f-11e0-b929-000c29ad1d07\" labelText=\"Endereço:\" class=\"input-with-size-lg\"/&gt;\r\n                        &lt;/p&gt;\r\n    \r\n                    &lt;/div&gt;\r\n    \r\n                    &lt;div class=\"line-break\"&gt;&lt;/div&gt;\r\n    \r\n                    &lt;div class=\"base-margin\"&gt;\r\n    \r\n                        &lt;label class=\"label-tag\" style=\"margin-bottom: 6px;\"&gt;Situação da família:&lt;/label&gt;\r\n\r\n                        &lt;div class=\"space-justify\"&gt;\r\n                            \r\n                            &lt;div class=\"base-width\"&gt;\r\n                                &lt;label&gt;Nome:&lt;/label&gt;\r\n                            &lt;/div&gt;\r\n\r\n                            &lt;div class=\"base-width base-margin\"&gt;\r\n                                &lt;label&gt;Parentesco:&lt;/label&gt;\r\n                            &lt;/div&gt;\r\n\r\n                            &lt;div class=\"base-width base-margin\"&gt;\r\n                                &lt;label&gt;Outro(Especifique):&lt;/label&gt;\r\n                             &lt;/div&gt;\r\n\r\n                            &lt;div class=\"base-margin\" style=\"width: 75px;\"&gt;\r\n                                &lt;label&gt;Idade:&lt;/label&gt;\r\n                            &lt;/div&gt;\r\n\r\n                            &lt;div class=\"base-width base-margin\"&gt;\r\n                                &lt;label&gt;Teste de HIV:&lt;/label&gt;\r\n                            &lt;/div&gt;\r\n\r\n                            &lt;div class=\"base-width base-margin\"&gt;\r\n                                &lt;label&gt;Cuidades de HIV:&lt;/label&gt;\r\n                            &lt;/div&gt;\r\n\r\n                            &lt;div class=\"base-width base-margin\"&gt;\r\n                                &lt;label&gt;Em CCR:&lt;/label&gt;\r\n                            &lt;/div&gt;\r\n\r\n                            &lt;div class=\"base-margin\"&gt;\r\n                                &lt;label&gt;NID:&lt;/label&gt;\r\n                            &lt;/div&gt;\r\n\r\n                        &lt;/div&gt;\r\n\r\n                        &lt;repeat&gt;\r\n                            &lt;template&gt;\r\n                                &lt;obsgroup groupingConceptId=\"b1dec8a4-c8a8-4d93-81b9-fd23d9c835fd\"&gt;\r\n    \r\n                                    &lt;div class=\"space-between boder-in\"&gt;\r\n            \r\n                                        &lt;div&gt;\r\n                                            &lt;p&gt;\r\n                                                &lt;obs conceptId=\"58849bca-141e-4f6c-aaff-509b1efa99ec\" /&gt;\r\n                                            &lt;/p&gt;\r\n                                        &lt;/div&gt;\r\n            \r\n                                        &lt;div class=\"base-margin\"&gt;\r\n                                            &lt;p&gt;\r\n                                                &lt;obs conceptId=\"dbf852ab-697f-4c92-a546-74e5301de419\" /&gt;\r\n                                            &lt;/p&gt;\r\n                                        &lt;/div&gt;\r\n\r\n                                        &lt;div class=\"base-margin\"&gt;\r\n                                            &lt;p&gt;\r\n                                                &lt;obs conceptId=\"e1e783ea-1d5f-11e0-b929-000c29ad1d07\" /&gt;\r\n                                            &lt;/p&gt;\r\n                                        &lt;/div&gt;\r\n            \r\n                                        &lt;div class=\"base-margin\"&gt;\r\n                                            &lt;p class=\"input-size-2\"&gt;\r\n                                                &lt;obs conceptId=\"695d79ba-97d1-4d6d-bfe7-25dcb650a568\" /&gt;\r\n                                            &lt;/p&gt;\r\n                                        &lt;/div&gt;\r\n            \r\n                                        &lt;div class=\"base-margin\"&gt;\r\n                                            &lt;p&gt;\r\n                                                &lt;obs conceptId=\"42a90771-4d00-44ec-b637-d704025855ba\" answerConceptIds=\"e1d47386-1d5f-11e0-b929-000c29ad1d07, e1d446cc-1d5f-11e0-b929-000c29ad1d07, e1d81d7e-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"Positivo (P),Negativo (N),Desconhecido (D)\" /&gt;\r\n                                            &lt;/p&gt;\r\n                                        &lt;/div&gt;\r\n            \r\n                                        &lt;div class=\"base-margin\"&gt;\r\n                                            &lt;p&gt;\r\n                                                &lt;obs conceptId=\"541d20ec-96d8-4705-ba7d-2df81cfff751\" answerConceptIds=\"e1d81b62-1d5f-11e0-b929-000c29ad1d07, e1d81c70-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"Sim,Não\"  /&gt;\r\n                                            &lt;/p&gt;\r\n                                        &lt;/div&gt;\r\n            \r\n                                        &lt;div class=\"base-margin\"&gt;\r\n                                            &lt;p&gt;\r\n                                                &lt;obs conceptId=\"e1def0cc-1d5f-11e0-b929-000c29ad1d07\" answerConceptIds=\"e1d81b62-1d5f-11e0-b929-000c29ad1d07,e1d81c70-1d5f-11e0-b929-000c29ad1d07,f3c00a5c-d251-43d0-864e-8897f5556417\" answerLabels=\"Sim (S),Não (N),Alta (A)\" /&gt;\r\n                                            &lt;/p&gt;\r\n                                        &lt;/div&gt;\r\n            \r\n                                        &lt;div class=\"base-margin\"&gt;\r\n                                            &lt;p&gt;\r\n                                                &lt;obs conceptId=\"59177ab6-a2db-4c20-a1c6-bb5c7c13cad4\" /&gt;\r\n                                            &lt;/p&gt;\r\n                                            \r\n                                        
-/div&gt;\r\n            \r\n                                    &lt;/div&gt;\r\n            \r\n                                &lt;/obsgroup&gt;\r\n                            &lt;/template&gt;\r\n                            &lt;render/&gt;\r\n                            &lt;render/&gt;\r\n                            &lt;render/&gt;\r\n                            &lt;render/&gt;\r\n                            &lt;render/&gt;\r\n                            &lt;render/&gt;\r\n                        &lt;/repeat&gt;\r\n    \r\n                    &lt;/div&gt;\r\n\r\n                    &lt;div class=\"line-break\"&gt;&lt;/div&gt;\r\n    \r\n                    &lt;div class=\"base-margin\"&gt;\r\n                \r\n                        &lt;label class=\"label-tag\" style=\"margin-top: 14px;\"&gt;Cuidados de HIV&lt;/label&gt;\r\n    \r\n                        &lt;div class=\"space-between\"&gt;\r\n    \r\n                            &lt;div&gt;\r\n                                &lt;p class=\"input-size-2\"&gt;\r\n                                    &lt;obs conceptId=\"c7ac119c-d59d-474d-8334-0c5bdd2e9863\" labelText=\"Teste HIV+:\" style=\"radio\" answerConceptIds=\"e1d800dc-1d5f-11e0-b929-000c29ad1d07, e1d7f61e-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"TR, PCR\" dateLabel=\"| Data:\"/&gt;&lt;br/&gt;&lt;br/&gt;\r\n                                    &lt;obs conceptId=\"b792c72c-eaf4-4386-b4a5-8f79c9a83746\" style=\"checkbox\" answerLabel=\"Diagnóstico presuntivo em crianças menores de 18 meses:\" answerConceptId=\"e1d81b62-1d5f-11e0-b929-000c29ad1d07\" dateLabel=\"| Data:\"/&gt;&lt;br/&gt;&lt;br/&gt;\r\n                                    &lt;obs conceptId=\"f69b1fe0-a657-4225-a996-20b599132508\" labelText=\"Data Inicio Pré-TARV:\" commentFieldLabel=\" Unidade Sanitária: \" /&gt;&lt;br/&gt;&lt;br/&gt;\r\n                                    &lt;obs conceptId=\"e1da7d3a-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1d81b62-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"Transferido de outra US\" dateLabel=\"| Data:\" commentFieldLabel=\" Unidade Sanitária: \"/&gt;\r\n                                &lt;/p&gt;\r\n        \r\n                            &lt;/div&gt;\r\n    \r\n                            &lt;div  class=\"base-margin\"&gt;\r\n                                &lt;p&gt;\r\n                                    &lt;obs conceptId=\"602d1865-4689-4b5b-84ff-092b51e7840c\" style=\"radio\" answerConceptIds=\"bdca9223-527b-46f7-8fb8-0288a58c83f1, cf6e0b75-d0b4-403a-a886-0c06e1e9ea77\" answerLabels=\"Unidade Sanitária, ATSC\" commentFieldLabel=\" Designação: \"/&gt;\r\n                                    &lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;\r\n                                    \r\n                                    \r\n                                    &lt;obs conceptId=\"beb9f5d1-3365-4574-894e-445b82a81087\" labelText=\"Sector:\" answerConceptIds=\"e1daea2c-1d5f-11e0-b929-000c29ad1d07, e1e05bc4-1d5f-11e0-b929-000c29ad1d07, e1e0599e-1d5f-11e0-b929-000c29ad1d07, e1dee38e-1d5f-11e0-b929-000c29ad1d07, d6b884fc-c799-4c23-844a-5eb1c470ab62\" answerLabels=\"TB, SAAJ, CPN/G, CCR/L, Clínica\" /&gt;&lt;br/&gt;&lt;br/&gt;\r\n                                    \r\n                                    &lt;obs conceptId=\"4f139c0a-9843-4dc4-b3e5-5aa00812e605\" style=\"radio\" answerConceptIds=\"44f812e8-c4c0-40cd-aef3-6b1ef76d43e1, 7f3af436-5c3a-447c-9012-42bb314e03db\" answerLabels=\"Em Pré-TARV, Em TARV\"/&gt;\r\n                                &lt;/p&gt;\r\n                            &lt;/div&gt;\r\n    \r\n                        &lt;/div&gt;\r\n    \r\n                    &lt;/div&gt;\r\n    \r\n                    &lt;div class=\"line-break\"&gt;&lt;/div&gt;\r\n    \r\n                    &lt;div class=\"base-margin\"&gt;\r\n                        \r\n                        &lt;label class=\"label-tag\" style=\"margin-bottom: 14px;\"&gt;Alergia a Medicamentos&lt;/label&gt;\r\n                        \r\n                        &lt;div class=\"box-inline\"&gt;\r\n                            &lt;repeat&gt;\r\n                                    &lt;template&gt;                  \r\n                                        &lt;obsgroup groupingConceptId=\"4b6e0e40-0d93-4112-95fe-38c01ceee2d6\"&gt;\r\n                                            &lt;label&gt;Alergia:&lt;/label&gt;\r\n                                            &lt;obs conceptId=\"e1dcadf8-1d5f-11e0-b929-000c29ad1d07\"  dateLabel=\"| Data:\"/&gt;\r\n                                            &lt;label&gt;Outra (Especifique):&lt;/label&gt;\r\n                                            &lt;obs conceptId=\"e1dc4af2-1d5f-11e0-b929-000c29ad1d07\"/&gt;&lt;br/&gt;\r\n                                        &lt;/obsgroup&gt;\r\n                                    &lt;/template&gt;\r\n                                    &lt;render/&gt;\r\n                                    &lt;render/&gt;\r\n                                    &lt;render/&gt;\r\n                            &lt;/repeat&gt;\r\n                        &lt;/div&gt;\r\n                        \r\n                    &lt;/div&gt;\r\n    \r\n                    &lt;div class=\"base-margin\"&gt;\r\n                        \r\n                        &lt;label class=\"label-tag\"&gt;Condições Medicas Importantes&lt;/label&gt;\r\n                        \r\n                        &lt;div class=\"space-between\"&gt;\r\n    \r\n                            &lt;div&gt;\r\n                                &lt;p class=\"input-size-2\"&gt;\r\n                                    &lt;obs conceptId=\"e1dae234-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1cdc68a-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"Hepatite\" dateLabel=\" | Data:\"/&gt;&lt;br/&gt;\r\n                                    &lt;obs conceptId=\"e1dae234-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1cfe2ee-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"Diabetes\" dateLabel=\" | Data:\"/&gt;&lt;br/&gt;\r\n                                    &lt;obs conceptId=\"e1dae234-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1cdd38c-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"TB\" dateLabel=\" | Data:\"/&gt;&lt;br/&gt;\r\n&lt;obs conceptId=\"e1e0dcde-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1d47386-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"Via Positivo\" dateLabel=\" | Data:\"/&gt;&lt;br/&gt;\r\n                                    \r\n                                &lt;/p&gt;\r\n                            &lt;/div&gt;\r\n    \r\n                            &lt;div  class=\"base-margin\"&gt;\r\n                                &lt;p class=\"input-size-2\"&gt;\r\n                                    &lt;obs conceptId=\"e1dae234-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"5a5619d5-89df-4acb-b0eb-c5e3c88235b8\" answerLabel=\"HTA\" dateLabel=\" | Data:\"/&gt;&lt;br/&gt;\r\n                                    &lt;obs conceptId=\"e1dae234-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"d4d5e9e8-9082-11e6-a98e-000c29db4475\" answerLabel=\"Criptococose\" dateLabel=\" | Data:\"/&gt;&lt;br/&gt;\r\n                                    &lt;obs conceptId=\"e1dae234-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1d2984a-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"S. Kaposi\" dateLabel=\" | Data:\"/&gt;&lt;br/&gt;\r\n&lt;label&gt;Outra:&lt;/label&gt;&lt;obs conceptId=\"e1dd2d50-1d5f-11e0-b929-000c29ad1d07\"  dateLabel=\"Data:\"/&gt;\r\n                                &lt;/p&gt;\r\n                            &lt;/div&gt;\r\n                            \r\n                        &lt;/div&gt;\r\n                        \r\n                    &lt;/div&gt;\r\n    \r\n                    &lt;div class=\"line-break\"&gt;&lt;/div&gt;\r\n    \r\n                    &lt;div class=\"base-margin\"&gt;\r\n                        &lt;label&gt;Último CD4:&lt;/label&gt;\r\n                        &lt;obs conceptId=\"e1dd5ab4-1d5f-11e0-b929-000c29ad1d07\" dateLabel=\"Data:\"/&gt;&lt;br/&gt;\r\n                    &lt;/div&gt;\r\n    \r\n                    &lt;div class=\"base-margin\"&gt;\r\n                        &lt;label&gt;Última Carga Viral:&lt;/label&gt;\r\n                        &lt;obs conceptId=\"e1d6247e-1d5f-11e0-b929-000c29ad1d07\" dateLabel=\"Data:\"/&gt;&lt;br/&gt;\r\n                    &lt;/div&gt;\r\n    \r\n                    &lt;div class=\"base-margin\"&gt;\r\n                        &lt;label&gt;Ùltima profilaxia Isoniazida (Data Inicio):&lt;/label&gt;\r\n                        &lt;obs conceptId=\"6fa92ac9-0a96-4372-9e10-dd9683c19135\" /&gt;\r\n                        &lt;label&gt;Ùltima profilaxia Isoniazida (Data Fim):&lt;/label&gt;\r\n                        &lt;obs conceptId=\"9e555978-3a02-4da4-855e-7b1bfc807347\" /&gt;\r\n                    &lt;/div&gt;\r\n                    \r\n                    &lt;div class=\"base-margin\"&gt;\r\n                        &lt;label&gt;ARVs tomados anteriormente, antes do TARV Actual:&lt;/label&gt;\r\n                        &lt;obs conceptId=\"e1e8d876-1d5f-11e0-b929-000c29ad1d07\" style=\"radio\" answerConceptIds=\"e1d81b62-1d5f-11e0-b929-000c29ad1d07, e1d81c70-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"Sim, Não\"/&gt;\r\n                    &lt;/div&gt;\r\n                    &lt;div class=\"line-break\"&gt;&lt;/div&gt;\r\n                    &lt;div class=\"base-margin\"&gt;\r\n                        &lt;label&gt;Se SIM:&lt;/label&gt;\r\n                        &lt;obs conceptId=\"16f3d28e-03d5-467f-841c-ad678e9a4c19\" answerConceptId=\"e1dc0eca-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"PTV\" dateLabel=\"Data:\" commentFieldLabel=\"Onde?\" /&gt;&lt;br/&gt;\r\n                        &lt;obs conceptId=\"16f3d28e-03d5-467f-841c-ad678e9a4c19\" answerConceptId=\"cdcf3400-f17b-400b-82be-b22cb4f0ebb7\" answerLabel=\"PPE\" dateLabel=\"Data:\" commentFieldLabel=\"Onde?\" /&gt;&lt;br/&gt;\r\n                        &lt;obs conceptId=\"16f3d28e-03d5-467f-841c-ad678e9a4c19\" answerConceptId=\"c29e5740-8ea5-409e-b322-7414f36e2739\" answerLabel=\"PrEP\" dateLabel=\"Data:\" commentFieldLabel=\"Onde?\" /&gt;&lt;br/&gt;\r\n                        &lt;obs conceptId=\"16f3d28e-03d5-467f-841c-ad678e9a4c19\" answerConceptId=\"39cab1ff-93e7-4a5e-bd42-6f8e6cb39359\" answerLabel=\"Outro\" dateLabel=\"Data:\" commentFieldLabel=\"Onde?\" /&gt;\r\n                        &lt;obs conceptId=\"39cab1ff-93e7-4a5e-bd42-6f8e6cb39359\" labelText=\"Especifique:\"/&gt;\r\n                        &lt;obs conceptId=\"e1dc3e04-1d5f-11e0-b929-000c29ad1d07\" answerConceptIds=\"e1d3d5de-1d5f-11e0-b929-000c29ad1d07, e1d5d988-1d5f-11e0-b929-000c29ad1d07,e1d5d438-1d5f-11e0-b929-000c29ad1d07,\r\n                        e1d3d2c8-1d5f-11e0-b929-000c29ad1d07,e1de9046-1d5f-11e0-b929-000c29ad1d07,e1de9140-1d5f-11e0-b929-000c29ad1d07,e1d3d4da-1d5f-11e0-b929-000c29ad1d07\" labelText=\"ARVs:\"/&gt;&lt;br/&gt;\r\n                    &lt;/div&gt;\r\n    \r\n                    &lt;div class=\"line-break\" style=\"margin-top: 14px;\"&gt;&lt;/div&gt;\r\n                    \r\n                    \r\n                    &lt;div class=\"line-break\"&gt;&lt;/div&gt;\r\n    \r\n                    &lt;div class=\"base-margin\"&gt;\r\n                        \r\n                        &lt;label class=\"label-tag\"&gt;No início do TARV&lt;/label&gt;\r\n                        \r\n                        &lt;div class=\"space-between\"&gt;\r\n    \r\n                            &lt;div&gt;\r\n                                &lt;p&gt;\r\n                                    \r\n                                    &lt;label&gt;Data de inicio TARV:&lt;/label&gt;\r\n                                    &lt;obs conceptId=\"e1d8f690-1d5f-11e0-b929-000c29ad1d07\" /&gt;&lt;br/&gt;\r\n                                    &lt;label&gt;Regime ARV inicial de primeira linha:&lt;/label&gt;\r\n                                    &lt;obs conceptId=\"62cd383d-165d-4b2a-96c1-a557d5c2bb6f\"/&gt;\r\n                                &lt;/p&gt;\r\n                            &lt;/div&gt;\r\n    \r\n                            &lt;div class=\"base-margin\"&gt;\r\n                                &lt;p&gt;\r\n                                    &lt;label&gt;Unidade Sanitária:&lt;/label&gt;\r\n                                    &lt;obs conceptId=\"760180a9-bcf0-4820-8771-d57d73d1f68d\"/&gt;&lt;br/&gt;\r\n                                    &lt;label&gt;Gravidez:&lt;/label&gt;\r\n                                    &lt;obs conceptId=\"e1e056a6-1d5f-11e0-b929-000c29ad1d07\" style=\"radio\" answerConceptIds=\"e1d81b62-1d5f-11e0-b929-000c29ad1d07, e1d81c70-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"Sim, Não\"/&gt;\r\n                                    &lt;label&gt; | Lactante:&lt;/label&gt;\r\n                                    &lt;obs conceptId=\"bc4fe755-fc8f-49b8-9956-baf2477e8313\" style=\"radio\" answerConceptIds=\"e1d81b62-1d5f-11e0-b929-000c29ad1d07, e1d81c70-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"Sim, Não\"/&gt;&lt;br/&gt;\r\n                                    &lt;label&gt;Estadio OMS:&lt;/label&gt;\r\n                                    &lt;obs conceptId=\"e1e53c02-1d5f-11e0-b929-000c29ad1d07\" answerConceptIds=\"e1d9055e-1d5f-11e0-b929-000c29ad1d07,e1d9066c-1d5f-11e0-b929-000c29ad1d07,e1d9077a-1d5f-11e0-b929-000c29ad1d07,e1d90888-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"I,II,III,IV\"/&gt;\r\n                                    &lt;label&gt;CD4(Nr.| %):&lt;/label&gt;\r\n                                    &lt;obs conceptId=\"596e9d7c-1a17-4177-b4fb-76341dbee9dd\" class=\"input-with-size\"/&gt; |  &lt;obs conceptId=\"e1d48fba-1d5f-11e0-b929-000c29ad1d07\" class=\"input-with-size\"/&gt;\r\n                                &lt;/p&gt;\r\n                            &lt;/div&gt;\r\n    \r\n                        &lt;/div&gt;\r\n                        \r\n                    &lt;/div&gt;\r\n    \r\n                    &lt;div class=\"line-break\"&gt;&lt;/div&gt;\r\n    \r\n                    &lt;div class=\"base-margin\"&gt;\r\n                            \r\n                        &lt;label class=\"label-tag\" style=\"margin-bottom: 14px;\"&gt;Alternativas à Linha - Primeira Linha&lt;/label&gt;\r\n                        &lt;repeat&gt;\r\n                            &lt;template&gt;\r\n                                &lt;obsgroup groupingConceptId=\"c95bf5fa-a04f-48d9-8504-f0575c2e255f\"&gt;\r\n                                        Novo Regime:\r\n                                        &lt;obs id=\"regime\" conceptId=\"618650c6-90c3-4acd-ae4d-ffb2f6452a5b\" answerConceptIds=\"\r\n                                            e1de19fe-1d5f-11e0-b929-000c29ad1d07,\r\n                                            28b28521-b6cd-454e-9ec5-f2c6c9c58468,\r\n                                            e1dd2f44-1d5f-11e0-b929-000c29ad1d07,\r\n                                            9dc17c1b-7b6d-488e-a38d-505a7b65ec82,\r\n                                            2e44e77e-eac4-4f64-84d2-73d32abf94d5,\r\n                                            78419317-cdda-42e9-92a3-13cb0cbf0020,\r\n                                            e3f6bb60-e2cf-46cb-a9da-27d634ba8607,\r\n                                            af15246d-30b8-4aff-8391-ca2b58e2c88b,\r\n                                            3e7f46c7-a971-4c0c-82aa-a65589fd518e,\r\n                                            cf05347e-063c-4896-91a4-097741cf6be6,\r\n                                            e11be52e-0da1-4d32-ab5c-e0feb9b6abd6,\r\n                                            f8c5d365-7636-4449-9acd-c83c4fd2ea01,\r\n                                            d5f9d629-67bc-4f60-9e12-629e6d2c1d08,\r\n                                            7bf5a88d-6db6-4899-a01a-bfd14ce77b53,\r\n                                            e8b741b3-463c-46b1-8423-a16f736af8d4,\r\n                                            ba25f2b5-4216-4605-9e6b-1f591033dc3e,\r\n                                            7d18d08c-d1a8-4dc8-8d65-02197b42acf7,\r\n                                            c22c4431-a27e-4054-92bb-a1563482003e,\r\n                                            c4a56680-ac6e-4538-8126-e3097b7b4789,\r\n                                            8f9c4e58-0d70-4b09-a109-e776d325e9fd,\r\n                                            9cb63f72-4c08-4543-878a-537dcabe5670,\r\n                                            46b8a2ab-36a7-4072-ab62-0af9b3b58e72,\r\n                                            552dd71f-d1de-426a-a19c-49b8706a4a7f,\r\n                                            f32e013c-38c8-483a-8012-88596e8b13da,\r\n                                            c30f826d-9433-4e63-ac91-dbbc158686ff,\r\n                                            e1e59e0e-1d5f-11e0-b929-000c29ad1d07\" labelText=\"\" answerLabels=\"AZT+3TC+EFV,\r\n                                                                                                            AZT+3TC+LPV/r,\r\n                                                                                                            AZT+3TC+NVP,\r\n                                                                                                            TDF+3TC+EFV,\r\n                                                                                                            TDF+3TC+NVP,\r\n                                                                                                            ABC+3TC+EFV,\r\n                                  
-                               </t>
+    <t xml:space="preserve">     &lt;htmlform&gt;\r\n        &lt;html xmlns=\"http://www.w3.org/1999/xhtml\"&gt;\r\n        &lt;head&gt;\r\n        &lt;meta http-equiv=\"Content-Type\" content=\"text/html; charset=utf-8\" /&gt;\r\n        &lt;title&gt;FICHA RESUMO&lt;/title&gt;\r\n          \r\n          &lt;style&gt;\r\n    \r\n            .main{\r\n                display: flex;\r\n                align-items: center;\r\n                flex-direction: column;\r\n                font-size: .9em;\r\n                width: 100%;\r\n            }\r\n    \r\n            .header-box{\r\n                width: 80%;\r\n                background: #1aac9b;\r\n                padding: 1px !important;\r\n                color: #fff;\r\n                box-shadow: 0 0 .3em #000;\r\n                margin-bottom: 10px;\r\n            }\r\n            \r\n            .content {\r\n                display: flex;\r\n                flex-flow: row wrap;\r\n                width: 80%;\r\n                border: 1px solid #1aac9b;\r\n                box-shadow: 0 0 .3em #000;\r\n            }\r\n    \r\n            .line-break {\r\n                width: 100%;\r\n            }\r\n    \r\n            .header, .space-between{\r\n                display: flex;\r\n                flex-flow: row wrap;\r\n                justify-content: space-between;\r\n                align-content: space-between;\r\n                width: 100%\r\n            }\r\n    \r\n            .header-data{\r\n              border: 1px solid #1aac9b;\r\n              margin-bottom: 10px !important;\r\n              padding: 0px 10px 0px 10px;\r\n              box-shadow: 0 0 .1em #000;\r\n              margin: 10px 10px;\r\n              background: #dedede\r\n            }\r\n    \r\n            .header-info{\r\n              border: 1px solid #1aac9b;\r\n              padding: 0px 10px 0px 10px;\r\n              box-shadow: 0 0 .1em #000;\r\n              margin: 10px 10px;\r\n              background: #dedede\r\n            }\r\n    \r\n            .header-box h2{\r\n               padding-left: 10px;\r\n               text-shadow: 0 0 .3em #000;\r\n            }\r\n    \r\n    \r\n            .header-info h3{\r\n              text-align: center;\r\n            }\r\n    \r\n            input[type=\"text\"]{\r\n                width: 150px;\r\n                margin-bottom: 4px;\r\n            }\r\n    \r\n            .input-size input[type=\"text\"]{\r\n                width: 50px !important;\r\n            }\r\n    \r\n            .input-size-2 input[type=\"text\"]{\r\n                width: 70px !important;\r\n            }\r\n    \r\n            p select {\r\n                width: 150px;\r\n                margin-bottom: 4px;\r\n            }\r\n    \r\n            .base-margin {\r\n                margin-left: 15px;\r\n            }\r\n    \r\n            .submit-btn {\r\n                flex: 1;\r\n                margin: 10px 15px;\r\n            }\r\n    \r\n             .submit-btn input{\r\n               color: #fff;\r\n               background: #1aac9b;\r\n               padding: 8px;\r\n               width: 12.8em;\r\n               font-weight: bold;\r\n               text-shadow: 0 0 .3em black;\r\n               font-size: 9pt;\r\n               border-radius: 5px 5px;\r\n            }\r\n    \r\n            .label-tag {\r\n               color: #fff;\r\n               background: #1aac9b;\r\n               padding: 7px;\r\n               font-weight: bold;\r\n               text-shadow: 0 0 .3em black;\r\n               font-size: 9pt;\r\n               border-radius: 5px 5px;\r\n               width: 100%;\r\n               display: inline-block;\r\n            }\r\n    \r\n            .input-with-size input[type=\"text\"]{\r\n                width : 50px !important;\r\n            }\r\n    \r\n            .input-with-size-lg input[type=\"text\"]{\r\n                width : 400px !important;\r\n            }\r\n    \r\n            .hasDatepicker{\r\n                width : 80px !important;\r\n            }\r\n\r\n            .boder-in {\r\n                margin-top: -14px;\r\n                margin-bottom: -22px;\r\n            }\r\n\r\n           .space-justify {\r\n                display: flex;\r\n                flex-flow: row wrap;\r\n                justify-content:baseline;;\r\n                align-content: flex-start;\r\n                width: 100%\r\n            }\r\n\r\n            .base-width {\r\n                width: 152px;\r\n            }\r\n\r\n            .space-justify label {\r\n                font-weight: bold;\r\n            }\r\n\r\n            #sociais select {\r\n                width: 289px;\r\n            }\r\n    \r\n            &lt;/style&gt;\r\n            &lt;script type=\"text/javascript\"&gt;\r\n                    function findAutoCompleteErrors() {\r\n                        /* see if there are  errors in option fields */\r\n                        var containError = false;\r\n                        var ary = $j(\".optionAutoCompleteHidden\");\r\n                        $j.each(ary,function(index, value){\r\n                            if(value.value == \"ERROR\"){\r\n                                containError=true;\r\n                            }\r\n                        });\r\n                        return containError;\r\n                    }\r\n                    $j(function() {\r\n                        $j(\'.submitButton\').click(function(event) {\r\n                            if(!findAutoCompleteErrors()){\r\n                                $j(\'.submitButton\').prop(\'disabled\', true);\r\n                            }\r\n                        });\r\n                    });\r\n            &lt;/script&gt;            \r\n            \r\n        &lt;/head&gt;\r\n        &lt;body&gt;\r\n            \r\n        &lt;div class=\"main\"&gt;\r\n            \r\n            &lt;div class=\"header-box\"&gt;\r\n                &lt;h2&gt;FICHA RESUMO&lt;/h2&gt;\r\n            &lt;/div&gt;\r\n    \r\n            &lt;div class=\"content\"&gt;\r\n    \r\n                    &lt;div class=\"header\"&gt;\r\n    \r\n                        &lt;div class=\"header-data\"&gt;\r\n                                &lt;p&gt;\r\n                                &lt;label&gt;Nome:&lt;/label&gt;\r\n                                &lt;lookup expression=\"patient.personName\"/&gt;\r\n                               \r\n                            &lt;/p&gt;\r\n                            &lt;p&gt;\r\n                                &lt;label&gt;Género/Data de Nasc./Idade:&lt;/label&gt;\r\n                                &lt;lookup expression=\"patient.gender\"/&gt; - &lt;lookup expression=\"patient.birthdate\"/&gt; - &lt;lookup expression=\"patient.age\"/&gt;\r\n                            &lt;/p&gt;\r\n&lt;p&gt;\r\n  &lt;label&gt;Telefone celular: &lt;/label&gt;\r\n                          &lt;lookup expression=\"patient.getAttribute(9)\"/&gt;\r\n&lt;/p&gt;\r\n\r\n                        &lt;/div&gt;\r\n    \r\n                        &lt;div class=\"header-info\"&gt;\r\n                            &lt;h3&gt;REPÚBLICA DE MOÇAMBIQUE&lt;/h3&gt;\r\n                            &lt;h3&gt;SERVIÇO NACIONAL DE SAÚDE&lt;/h3&gt;\r\n                            &lt;p&gt;\r\n                                &lt;label&gt;NID:&lt;lookup expression=\"patient.getPatientIdentifier(2)\"/&gt;&lt;/label&gt;\r\n                            &lt;/p&gt;\r\n                        &lt;/div&gt;\r\n    \r\n                    &lt;/div&gt;\r\n                    \r\n                    &lt;div class=\"line-break\"&gt;&lt;/div&gt;\r\n    \r\n                    &lt;div class=\"base-margin\"&gt;\r\n    \r\n                        &lt;label class=\"label-tag\"&gt;Livros: Pré-TARV&lt;/label&gt;   \r\n    \r\n                        &lt;p class=\"input-size-2\"&gt;\r\n                            &lt;obs conceptId=\"d8ec9c7c-6b46-435b-8c80-3967f396bd71\" labelText=\"Nr. do Livro:\" /&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"c02181e6-8f9f-4387-9cf6-9a3d0f45b7fc\" labelText=\"Página:\" /&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"bf958c27-fa29-4b95-a055-a9d2d162ef76\" labelText=\"Linha:\" /&gt;\r\n                        &lt;/p&gt;\r\n    \r\n                    &lt;/div&gt;\r\n    \r\n                    &lt;div class=\"base-margin\"&gt;\r\n                        &lt;label class=\"label-tag\"&gt;Livros: TARV&lt;/label&gt;   \r\n    \r\n                        &lt;p class=\"input-size-2\"&gt;\r\n                            &lt;obs conceptId=\"39a21629-cf4e-45f3-be2e-287cce2d5d4c\" labelText=\"Nr. do Livro:\" /&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"9a9b36c9-ace0-40e9-a296-e547197358df\" labelText=\"Página:\" /&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"65be2cd1-8c97-41f8-9ff9-665d54479943\" labelText=\"Linha:\" /&gt;\r\n                        &lt;/p&gt;\r\n                    &lt;/div&gt;\r\n    \r\n                    &lt;div class=\"line-break\"&gt;&lt;/div&gt;\r\n    \r\n                    &lt;div class=\"base-margin\"&gt;\r\n    \r\n                        &lt;p&gt;\r\n                            &lt;label&gt;Unidade Sanitária:&lt;/label&gt;\r\n                            &lt;encounterLocation id=\"localConsulta\" default=\"GlobalProperty:default_location\" type=\"autocomplete\"/&gt;\r\n                        &lt;/p&gt;\r\n    \r\n                    &lt;/div&gt;\r\n    \r\n                    &lt;div class=\"line-break\"&gt;&lt;/div&gt;\r\n    \r\n                    &lt;div class=\"base-margin\"&gt;\r\n    \r\n                        &lt;p&gt;\r\n                            &lt;label&gt;Data Abertura da Ficha:&lt;/label&gt;                                \r\n                            &lt;obs conceptId=\"68d65d0c-8fee-456b-8e95-caed990351e1\" required=\"true\" /&gt;\r\n                        &lt;/p&gt;\r\n    \r\n                    &lt;/div&gt;\r\n    \r\n                    &lt;div class=\"base-margin\"&gt;\r\n    \r\n                        &lt;p&gt;\r\n                            &lt;label&gt;Profissão:&lt;/label&gt;\r\n                            &lt;obs conceptId=\"e1dc07c2-1d5f-11e0-b929-000c29ad1d07\" /&gt;\r\n                        &lt;/p&gt; \r\n    \r\n                    &lt;/div&gt;\r\n    \r\n                    &lt;div class=\"base-margin\"&gt;\r\n    \r\n                        &lt;p&gt;\r\n                            &lt;label&gt;Nível de Escolaridade:&lt;/label&gt;\r\n                            &lt;obs conceptId=\"e1db0700-1d5f-11e0-b929-000c29ad1d07\" answerConceptIds=\"e1db08fe-1d5f-11e0-b929-000c29ad1d07, e1db09f8-1d5f-11e0-b929-000c29ad1d07, e1db0af2-1d5f-11e0-b929-000c29ad1d07, e1db0bf6-1d5f-11e0-b929-000c29ad1d07\" /&gt;\r\n                        &lt;/p&gt;  \r\n    \r\n                    &lt;/div&gt;\r\n    \r\n                    &lt;div class=\"line-break\"&gt;&lt;/div&gt;\r\n    \r\n                    &lt;div class=\"base-margin\"&gt;\r\n                            &lt;label class=\"label-tag\"&gt;Confidente:&lt;/label&gt;   \r\n    \r\n                        &lt;p&gt;\r\n                            &lt;obs conceptId=\"e1de46a4-1d5f-11e0-b929-000c29ad1d07\" labelText=\"Nome:\" /&gt;\r\n                            &lt;obs conceptId=\"dbf852ab-697f-4c92-a546-74e5301de419\" labelText=\"Parentesco:\" /&gt; &lt;br/&gt;\r\n                            &lt;obs conceptId=\"eb23c94a-2c2e-40fa-ab82-22308b1c5f27\" labelText=\"Telefone Celular (1):\" /&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"eb23c94a-2c2e-40fa-ab82-22308b1c5f27\" labelText=\"Telefone Celular (2):\" /&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"e1e0c208-1d5f-11e0-b929-000c29ad1d07\" labelText=\"Endereço:\" class=\"input-with-size-lg\"/&gt;\r\n                        &lt;/p&gt;\r\n    \r\n                    &lt;/div&gt;\r\n    \r\n                    &lt;div class=\"line-break\"&gt;&lt;/div&gt;\r\n    \r\n                    &lt;div class=\"base-margin\"&gt;\r\n    \r\n                        &lt;label class=\"label-tag\" style=\"margin-bottom: 6px;\"&gt;Situação da família:&lt;/label&gt;\r\n\r\n                        &lt;div class=\"space-justify\"&gt;\r\n                            \r\n                            &lt;div class=\"base-width\"&gt;\r\n                                &lt;label&gt;Nome:&lt;/label&gt;\r\n                            &lt;/div&gt;\r\n\r\n                            &lt;div class=\"base-width base-margin\"&gt;\r\n                                &lt;label&gt;Parentesco:&lt;/label&gt;\r\n                            &lt;/div&gt;\r\n\r\n                            &lt;div class=\"base-width base-margin\"&gt;\r\n                                &lt;label&gt;Outro(Especifique):&lt;/label&gt;\r\n                             &lt;/div&gt;\r\n\r\n                            &lt;div class=\"base-margin\" style=\"width: 75px;\"&gt;\r\n                                &lt;label&gt;Idade:&lt;/label&gt;\r\n                            &lt;/div&gt;\r\n\r\n                            &lt;div class=\"base-width base-margin\"&gt;\r\n                                &lt;label&gt;Teste de HIV:&lt;/label&gt;\r\n                            &lt;/div&gt;\r\n\r\n                            &lt;div class=\"base-width base-margin\"&gt;\r\n                                &lt;label&gt;Cuidados de HIV:&lt;/label&gt;\r\n                            &lt;/div&gt;\r\n\r\n                            &lt;div class=\"base-width base-margin\"&gt;\r\n                                &lt;label&gt;Em CCR:&lt;/label&gt;\r\n                            &lt;/div&gt;\r\n\r\n                            &lt;div class=\"base-margin\"&gt;\r\n                                &lt;label&gt;NID:&lt;/label&gt;\r\n                            &lt;/div&gt;\r\n\r\n                        &lt;/div&gt;\r\n\r\n                        &lt;repeat&gt;\r\n                            &lt;template&gt;\r\n                                &lt;obsgroup groupingConceptId=\"b1dec8a4-c8a8-4d93-81b9-fd23d9c835fd\"&gt;\r\n    \r\n                                    &lt;div class=\"space-between boder-in\"&gt;\r\n            \r\n                                        &lt;div&gt;\r\n                                            &lt;p&gt;\r\n                                                &lt;obs conceptId=\"58849bca-141e-4f6c-aaff-509b1efa99ec\" /&gt;\r\n                                            &lt;/p&gt;\r\n                                        &lt;/div&gt;\r\n            \r\n                                        &lt;div class=\"base-margin\"&gt;\r\n                                            &lt;p&gt;\r\n                                                &lt;obs conceptId=\"dbf852ab-697f-4c92-a546-74e5301de419\" /&gt;\r\n                                            &lt;/p&gt;\r\n                                        &lt;/div&gt;\r\n\r\n                                        &lt;div class=\"base-margin\"&gt;\r\n                                            &lt;p&gt;\r\n                                                &lt;obs conceptId=\"e1e783ea-1d5f-11e0-b929-000c29ad1d07\" /&gt;\r\n                                            &lt;/p&gt;\r\n                                        &lt;/div&gt;\r\n            \r\n                                        &lt;div class=\"base-margin\"&gt;\r\n                                            &lt;p class=\"input-size-2\"&gt;\r\n                                                &lt;obs conceptId=\"695d79ba-97d1-4d6d-bfe7-25dcb650a568\" /&gt;\r\n                                            &lt;/p&gt;\r\n                                        &lt;/div&gt;\r\n            \r\n                                        &lt;div class=\"base-margin\"&gt;\r\n                                            &lt;p&gt;\r\n                                                &lt;obs conceptId=\"42a90771-4d00-44ec-b637-d704025855ba\" answerConceptIds=\"e1d47386-1d5f-11e0-b929-000c29ad1d07, e1d446cc-1d5f-11e0-b929-000c29ad1d07, e1d81d7e-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"Positivo (P),Negativo (N),Desconhecido (D)\" /&gt;\r\n                                            &lt;/p&gt;\r\n                                        &lt;/div&gt;\r\n            \r\n                                        &lt;div class=\"base-margin\"&gt;\r\n                                            &lt;p&gt;\r\n                                                &lt;obs conceptId=\"541d20ec-96d8-4705-ba7d-2df81cfff751\" answerConceptIds=\"e1d81b62-1d5f-11e0-b929-000c29ad1d07, e1d81c70-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"Sim,Não\"  /&gt;\r\n                                            &lt;/p&gt;\r\n                                        &lt;/div&gt;\r\n            \r\n                                        &lt;div class=\"base-margin\"&gt;\r\n                                            &lt;p&gt;\r\n                                                &lt;obs conceptId=\"e1def0cc-1d5f-11e0-b929-000c29ad1d07\" answerConceptIds=\"e1d81b62-1d5f-11e0-b929-000c29ad1d07,e1d81c70-1d5f-11e0-b929-000c29ad1d07,f3c00a5c-d251-43d0-864e-8897f5556417\" answerLabels=\"Sim (S),Não (N),Alta (A)\" /&gt;\r\n                                            &lt;/p&gt;\r\n                                        &lt;/div&gt;\r\n            \r\n                                        &lt;div class=\"base-margin\"&gt;\r\n                                            &lt;p&gt;\r\n                                                &lt;obs conceptId=\"59177ab6-a2db-4c20-a1c6-bb5c7c13cad4\" /&gt;\r\n                                            &lt;/p&gt;\r\n                                            \r\n                                        &lt;/div&gt;\r\n            \r\n                                    &lt;/div&gt;\r\n            \r\n                                &lt;/obsgroup&gt;\r\n                            &lt;/template&gt;\r\n                            &lt;render/&gt;\r\n                            &lt;render/&gt;\r\n                            &lt;render/&gt;\r\n                            &lt;render/&gt;\r\n                            &lt;render/&gt;\r\n                            &lt;render/&gt;\r\n                            &lt;render/&gt;\r\n                            &lt;render/&gt;\r\n                           &lt;render/&gt;\r\n                           &lt;render/&gt;\r\n                           &lt;render/&gt;\r\n                           &lt;render/&gt;\r\n                        &lt;/repeat&gt;\r\n    \r\n                    &lt;/div&gt;\r\n\r\n                    &lt;div class=\"line-break\"&gt;&lt;/div&gt;\r\n    \r\n                    &lt;div class=\"base-margin\"&gt;\r\n                \r\n                        &lt;label class=\"label-tag\" style=\"margin-top: 14px;\"&gt;Cuidados de HIV&lt;/label&gt;\r\n    \r\n                        &lt;div class=\"space-between\"&gt;\r\n    \r\n                            &lt;div&gt;\r\n                                &lt;p class=\"input-size-2\"&gt;\r\n                                    &lt;obs conceptId=\"c7ac119c-d59d-474d-8334-0c5bdd2e9863\" labelText=\"Teste HIV+:\" style=\"radio\" answerConceptIds=\"e1d800dc-1d5f-11e0-b929-000c29ad1d07, e1d7f61e-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"TR, PCR\" dateLabel=\"| Data:\"/&gt;&lt;br/&gt;&lt;br/&gt;\r\n                                    &lt;obs conceptId=\"b792c72c-eaf4-4386-b4a5-8f79c9a83746\" style=\"checkbox\" answerLabel=\"Diagnóstico presuntivo em crianças menores de 18 meses:\" answerConceptId=\"e1d81b62-1d5f-11e0-b929-000c29ad1d07\" dateLabel=\"| Data:\"/&gt;&lt;br/&gt;&lt;br/&gt;\r\n                                    &lt;obs conceptId=\"f69b1fe0-a657-4225-a996-20b599132508\" labelText=\"Data Inicio Pré-TARV:\" commentFieldLabel=\" Unidade Sanitária: \" /&gt;&lt;br/&gt;&lt;br/&gt;\r\n                                    &lt;obs conceptId=\"e1da7d3a-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1d81b62-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"Transferido de outra US\" dateLabel=\"| Data:\" commentFieldLabel=\" Unidade Sanitária: \"/&gt;\r\n                                &lt;/p&gt;\r\n        \r\n                            &lt;/div&gt;\r\n    \r\n                            &lt;div  class=\"base-margin\"&gt;\r\n                                &lt;p&gt;\r\n                                    &lt;obs conceptId=\"602d1865-4689-4b5b-84ff-092b51e7840c\" style=\"radio\" answerConceptIds=\"bdca9223-527b-46f7-8fb8-0288a58c83f1, cf6e0b75-d0b4-403a-a886-0c06e1e9ea77\" answerLabels=\"Unidade Sanitária, ATSC\" commentFieldLabel=\" Designação: \"/&gt;\r\n                                    &lt;br/&gt;&lt;br/&gt;&lt;br/&gt;&lt;br/&gt;\r\n                                    \r\n                                    \r\n                                    &lt;obs conceptId=\"beb9f5d1-3365-4574-894e-445b82a81087\" labelText=\"Sector:\" answerConceptIds=\"e1daea2c-1d5f-11e0-b929-000c29ad1d07, e1e05bc4-1d5f-11e0-b929-000c29ad1d07, e1e0599e-1d5f-11e0-b929-000c29ad1d07, e1dee38e-1d5f-11e0-b929-000c29ad1d07, d6b884fc-c799-4c23-844a-5eb1c470ab62\" answerLabels=\"TB, SAAJ, CPN/G, CCR/L, Clínica\" /&gt;&lt;br/&gt;&lt;br/&gt;\r\n                                    \r\n                                    &lt;obs conceptId=\"4f139c0a-9843-4dc4-b3e5-5aa00812e605\" style=\"radio\" answerConceptIds=\"44f812e8-c4c0-40cd-aef3-6b1ef76d43e1, 7f3af436-5c3a-447c-9012-42bb314e03db\" answerLabels=\"Em Pré-TARV, Em TARV\"/&gt;\r\n                                &lt;/p&gt;\r\n                            &lt;/div&gt;\r\n    \r\n                        &lt;/div&gt;\r\n    \r\n                    &lt;/div&gt;\r\n    \r\n                    &lt;div class=\"line-break\"&gt;&lt;/div&gt;\r\n    \r\n                    &lt;div class=\"base-margin\"&gt;\r\n                        \r\n                        &lt;label class=\"label-tag\" style=\"margin-bottom: 14px;\"&gt;Alergia a Medicamentos&lt;/label&gt;\r\n                        \r\n                        &lt;div class=\"box-inline\"&gt;\r\n                            &lt;repeat&gt;\r\n                                    &lt;template&gt;                  \r\n                                        &lt;obsgroup groupingConceptId=\"4b6e0e40-0d93-4112-95fe-38c01ceee2d6\"&gt;\r\n                                            &lt;label&gt;Alergia:&lt;/label&gt;\r\n                                            &lt;obs conceptId=\"e1dcadf8-1d5f-11e0-b929-000c29ad1d07\"  dateLabel=\"| Data:\"/&gt;\r\n                                            &lt;label&gt;Outra (Especifique):&lt;/label&gt;\r\n                                            &lt;obs conceptId=\"e1dc4af2-1d5f-11e0-b929-000c29ad1d07\"/&gt;&lt;br/&gt;\r\n                                        &lt;/obsgroup&gt;\r\n                                    &lt;/template&gt;\r\n                                    &lt;render/&gt;\r\n                                    &lt;render/&gt;\r\n                                    &lt;render/&gt;\r\n                            &lt;/repeat&gt;\r\n                        &lt;/div&gt;\r\n                        \r\n                    &lt;/div&gt;\r\n    \r\n                    &lt;div class=\"base-margin\"&gt;\r\n                        \r\n                        &lt;label class=\"label-tag\"&gt;Condições Medicas Importantes&lt;/label&gt;\r\n                        \r\n                        &lt;div class=\"space-between\"&gt;\r\n    \r\n                            &lt;div&gt;\r\n                                &lt;p class=\"input-size-2\"&gt;\r\n                                    &lt;obs conceptId=\"e1dae234-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1cdc68a-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"Hepatite\" dateLabel=\" | Data:\"/&gt;&lt;br/&gt;\r\n                                    &lt;obs conceptId=\"e1dae234-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1cfe2ee-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"Diabetes\" dateLabel=\" | Data:\"/&gt;&lt;br/&gt;\r\n                                    &lt;obs conceptId=\"e1dae234-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1cdd38c-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"TB\" dateLabel=\" | Data:\"/&gt;&lt;br/&gt;\r\n&lt;obs conceptId=\"e1e0dcde-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1d47386-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"Via Positivo\" dateLabel=\" | Data:\"/&gt;&lt;br/&gt;\r\n                                    \r\n                                &lt;/p&gt;\r\n                            &lt;/div&gt;\r\n    \r\n                            &lt;div  class=\"base-margin\"&gt;\r\n                                &lt;p class=\"input-size-2\"&gt;\r\n                                    &lt;obs conceptId=\"e1dae234-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"5a5619d5-89df-4acb-b0eb-c5e3c88235b8\" answerLabel=\"HTA\" dateLabel=\" | Data:\"/&gt;&lt;br/&gt;\r\n                                    &lt;obs conceptId=\"e1dae234-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"d4d5e9e8-9082-11e6-a98e-000c29db4475\" answerLabel=\"Criptococose\" dateLabel=\" | Data:\"/&gt;&lt;br/&gt;\r\n                                    &lt;obs conceptId=\"e1dae234-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1d2984a-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"S. Kaposi\" dateLabel=\" | Data:\"/&gt;&lt;br/&gt;\r\n&lt;label&gt;Outra:&lt;/label&gt;&lt;obs conceptId=\"e1dd2d50-1d5f-11e0-b929-000c29ad1d07\"  dateLabel=\"Data:\"/&gt;\r\n                                &lt;/p&gt;\r\n                            &lt;/div&gt;\r\n                            \r\n                        &lt;/div&gt;\r\n                        \r\n                    &lt;/div&gt;\r\n    \r\n                    &lt;div class=\"line-break\"&gt;&lt;/div&gt;\r\n    \r\n                    &lt;div class=\"base-margin\"&gt;\r\n                        &lt;label&gt;Último CD4:&lt;/label&gt;\r\n                        &lt;obs conceptId=\"e1dd5ab4-1d5f-11e0-b929-000c29ad1d07\" dateLabel=\"Data:\"/&gt;&lt;br/&gt;\r\n                    &lt;/div&gt;\r\n    \r\n                    &lt;div class=\"base-margin\"&gt;\r\n                        &lt;label&gt;Última Carga Viral:&lt;/label&gt;\r\n                        &lt;obs conceptId=\"e1d6247e-1d5f-11e0-b929-000c29ad1d07\" dateLabel=\"Data:\"/&gt;&lt;br/&gt;\r\n                    &lt;/div&gt;\r\n    \r\n                    &lt;div class=\"base-margin\"&gt;\r\n                        &lt;label&gt;Ùltima profilaxia Isoniazida (Data Inicio):&lt;/label&gt;\r\n                        &lt;obs conceptId=\"6fa92ac9-0a96-4372-9e10-dd9683c19135\" /&gt;\r\n                        &lt;label&gt;Ùltima profilaxia Isoniazida (Data Fim):&lt;/label&gt;\r\n                        &lt;obs conceptId=\"9e555978-3a02-4da4-855e-7b1bfc807347\" /&gt;\r\n                    &lt;/div&gt;\r\n                    \r\n                    &lt;div class=\"base-margin\"&gt;\r\n                        &lt;label&gt;ARVs tomados anteriormente, antes do TARV Actual:&lt;/label&gt;\r\n                        &lt;obs conceptId=\"e1e8d876-1d5f-11e0-b929-000c29ad1d07\" style=\"radio\" answerConceptIds=\"e1d81b62-1d5f-11e0-b929-000c29ad1d07, e1d81c70-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"Sim, Não\"/&gt;\r\n                    &lt;/div&gt;\r\n                    &lt;div class=\"line-break\"&gt;&lt;/div&gt;\r\n                    &lt;div class=\"base-margin\"&gt;\r\n                        &lt;label&gt;Se SIM:&lt;/label&gt;\r\n                        &lt;obs conceptId=\"16f3d28e-03d5-467f-841c-ad678e9a4c19\" answerConceptId=\"e1dc0eca-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"PTV\" dateLabel=\"Data:\" commentFieldLabel=\"Onde?\" /&gt;&lt;br/&gt;\r\n                        &lt;obs conceptId=\"16f3d28e-03d5-467f-841c-ad678e9a4c19\" answerConceptId=\"cdcf3400-f17b-400b-82be-b22cb4f0ebb7\" answerLabel=\"PPE\" dateLabel=\"Data:\" commentFieldLabel=\"Onde?\" /&gt;&lt;br/&gt;\r\n                        &lt;obs conceptId=\"16f3d28e-03d5-467f-841c-ad678e9a4c19\" answerConceptId=\"c29e5740-8ea5-409e-b322-7414f36e2739\" answerLabel=\"PrEP\" dateLabel=\"Data:\" commentFieldLabel=\"Onde?\" /&gt;&lt;br/&gt;\r\n                        &lt;obs conceptId=\"16f3d28e-03d5-467f-841c-ad678e9a4c19\" answerConceptId=\"39cab1ff-93e7-4a5e-bd42-6f8e6cb39359\" answerLabel=\"Outro\" dateLabel=\"Data:\" commentFieldLabel=\"Onde?\" /&gt;\r\n                        &lt;obs conceptId=\"39cab1ff-93e7-4a5e-bd42-6f8e6cb39359\" labelText=\"Especifique:\"/&gt;\r\n                        &lt;obs conceptId=\"e1dc3e04-1d5f-11e0-b929-000c29ad1d07\" answerConceptIds=\"e1d3d5de-1d5f-11e0-b929-000c29ad1d07, e1d5d988-1d5f-11e0-b929-000c29ad1d07,e1d5d438-1d5f-11e0-b929-000c29ad1d07,\r\n                        e1d3d2c8-1d5f-11e0-b929-000c29ad1d07,e1de9046-1d5f-11e0-b929-000c29ad1d07,e1de9140-1d5f-11e0-b929-000c29ad1d07,e1d3d4da-1d5f-11e0-b929-000c29ad1d07\" labelText=\"ARVs:\"/&gt;&lt;br/&gt;\r\n                    &lt;/div&gt;\r\n    \r\n                    &lt;div class=\"line-break\" style=\"margin-top: 14px;\"&gt;&lt;/div&gt;\r\n                    \r\n                    \r\n                    &lt;div class=\"line-break\"&gt;&lt;/div&gt;\r\n    \r\n                    &lt;div class=\"base-margin\"&gt;\r\n                        \r\n                        &lt;label class=\"label-tag\"&gt;No início do TARV&lt;/label&gt;\r\n                        \r\n                        &lt;div class=\"space-between\"&gt;\r\n    \r\n                            &lt;div&gt;\r\n                                &lt;p&gt;\r\n                                    \r\n                                    &lt;label&gt;Data de inicio TARV:&lt;/label&gt;\r\n                                    &lt;obs conceptId=\"e1d8f690-1d5f-11e0-b929-000c29ad1d07\" /&gt;&lt;br/&gt;\r\n                                    &lt;label&gt;Regime ARV inicial de primeira linha:&lt;/label&gt;\r\n                                    &lt;obs conceptId=\"62cd383d-165d-4b2a-96c1-a557d5c2bb6f\"/&gt;\r\n                                &lt;/p&gt;\r\n                            &lt;/div&gt;\r\n    \r\n                            &lt;div class=\"base-margin\"&gt;\r\n                                &lt;p&gt;\r\n                                    &lt;label&gt;Unidade Sanitária:&lt;/label&gt;\r\n                                    &lt;obs conceptId=\"760180a9-bcf0-4820-8771-d57d73d1f68d\"/&gt;&lt;br/&gt;\r\n                                    &lt;label&gt;Gravidez:&lt;/label&gt;\r\n                                    &lt;obs conceptId=\"e1e056a6-1d5f-11e0-b929-000c29ad1d07\" style=\"radio\" answerConceptIds=\"e1d81b62-1d5f-11e0-b929-000c29ad1d07, e1d81c70-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"Sim, Não\"/&gt;\r\n                                    &lt;label&gt; | Lactante:&lt;/label&gt;\r\n                                    &lt;obs conceptId=\"bc4fe755-fc8f-49b8-9956-baf2477e8313\" style=\"radio\" answerConceptIds=\"e1d81b62-1d5f-11e0-b929-000c29ad1d07, e1d81c70-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"Sim, Não\"/&gt;&lt;br/&gt;\r\n                                    &lt;label&gt;Estadio OMS:&lt;/label&gt;\r\n                                    &lt;obs conceptId=\"e1e53c02-1d5f-11e0-b929-000c29ad1d07\" answerConceptIds=\"e1d9055e-1d5f-11e0-b929-000c29ad1d07,e1d9066c-1d5f-11e0-b929-000c29ad1d07,e1d9077a-1d5f-11e0-b929-000c29ad1d07,e1d90888-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"I,II,III,IV\"/&gt;\r\n                                    &lt;label&gt;CD4(Nr.| %):&lt;/label&gt;\r\n                                    &lt;obs conceptId=\"596e9d7c-1a17-4177-b4fb-76341dbee9dd\" class=\"input-with-size\"/&gt; |  &lt;obs conceptId=\"e1d48fba-1d5f-11e0-b929-000c29ad1d07\" class=\"input-with-size\"/&gt;\r\n                                &lt;/p&gt;\r\n                            &lt;/div&gt;\r\n    \r\n                        &lt;/div&gt;\r\n                        \r\n                    &lt;/div&gt;\r\n    \r\n                    &lt;div class=\"line-break\"&gt;&lt;/div&gt;\r\n    \r\n                    &lt;div class=\"base-margin\"&gt;\r\n                            \r\n                        &lt;label class=\"label-tag\" style=\"margin-bottom: 14px;\"&gt;Alternativas à Linha - Primeira Linha&lt;/label&gt;\r\n                        &lt;repeat&gt;\r\n                            &lt;template&gt;\r\n                                &lt;obsgroup groupingConceptId=\"c95bf5fa-a04f-48d9-8504-f0575c2e255f\"&gt;\r\n                                        Novo Regime:\r\n                                        &lt;obs id=\"regime\" conceptId=\"618650c6-90c3-4acd-ae4d-ffb2f6452a5b\" answerConceptIds=\"\r\n                                            e1de19fe-1d5f-11e0-b929-000c29ad1d07,\r\n                                            28b28521-b6cd-454e-9ec5-f2c6c9c58468,\r\n                                            e1dd2f44-1d5f-11e0-b929-000c29ad1d07,\r\n                                            9dc17c1b-7b6d-488e-a38d-505a7b65ec82,\r\n                                            2e44e77e-eac4-4f64-84d2-73d32abf94d5,\r\n                                            78419317-cdda-42e9-92a3-13cb0cbf0020,\r\n                                            e3f6bb60-e2cf-46cb-a9da-27d634ba8607,\r\n                                            af15246d-30b8-4aff-8391-ca2b58e2c88b,\r\n                                            3e7f46c7-a971-4c0c-82aa-a65589fd518e,\r\n                                            cf05347e-063c-4896-91a4-097741cf6be6,\r\n                                            e11be52e-0da1-4d32-ab5c-e0feb9b6abd6,\r\n                                            f8c5d365-7636-4449-9acd-c83c4fd2ea01,\r\n                                            d5f9d629-67bc-4f60-9e12-629e6d2c1d08,\r\n                                            7bf5a88d-6db6-4899-a01a-bfd14ce77b53,\r\n                                            e8b741b3-463c-46b1-8423-a16f736af8d4,\r\n                                            ba25f2b5-4216-4605-9e6b-1f591033dc3e,\r\n                                            7d18d08c-d1a8-4dc8-8d65-02197b42acf7,\r\n                                            c22c4431-a27e-4054-92bb-a1563482003e,\r\n                                            c4a56680-ac6e-4538-8126-e3097b7b4789,\r\n                                            8f9c4e58-0d70-4b09-a109-e776d325e9fd,\r\n                                            9cb63f72-4c08-4543-878a-537dcabe5670,\r\n                                            46b8a2ab-36a7-4072-ab62-0af9b3b58e72,\r\n                                            552dd71f-d1de-426a-a19c-49b8706a4a7f,\r\n                                            f32e013c-38c8-483a-8012-88596e8b13da,\r\n                                            c30f826d-9433-4e63-ac91-dbbc158686ff,\r\n                                            e1e59e0e-1d5f-11e0-b929-000c29ad1d07\" labelText=\"\" answerLabels=\"AZT+3TC+EFV,\r\n                                                                                                            AZT+3TC+LPV/r,\r\n                                                                                                            AZT+3TC+NVP,\r\n                            </t>
   </si>
   <si>
     <t>dead3eec-60ab-46d2-9e63-e732a846c37c</t>
@@ -986,9 +984,7 @@
     <t>9ca0fd8d-1f62-4ca7-981d-ab5906f7755a</t>
   </si>
   <si>
-    <t>&lt;htmlform&gt;\r\n            &lt;html xmlns=\"http://www.w3.org/1999/xhtml\"&gt;\r\n            &lt;head&gt;\r\n            &lt;meta http-equiv=\"Content-Type\" content=\"text/html; charset=utf-8\" /&gt;\r\n            &lt;title&gt;FICHA CLÍNICA&lt;/title&gt;\r\n              \r\n              &lt;style&gt;\r\n\r\n                .main{\r\n                    display: flex;\r\n                    align-items: center;\r\n                    flex-direction: column;\r\n                    font-size: .9em;\r\n                    width: 100%;\r\n                }\r\n\r\n                .header-box{\r\n                    width: 85%;\r\n                    background: #1aac9b;\r\n                    padding: 1px !important;\r\n                    color: #fff;\r\n                    box-shadow: 0 0 .3em #000;\r\n                    margin-bottom: 10px;\r\n                }\r\n                \r\n                .content {\r\n                    display: flex;\r\n                    flex-flow: row wrap;\r\n                    width: 85%;\r\n                    border: 1px solid #1aac9b;\r\n                    box-shadow: 0 0 .3em #000;\r\n                }\r\n\r\n                .line-break {\r\n                    width: 100%;\r\n                }\r\n\r\n                .header, .space-between{\r\n                    display: flex;\r\n                    flex-flow: row wrap;\r\n                    justify-content: space-between;\r\n                    align-content: space-between;\r\n                    width: 100%;\r\n                }\r\n\r\n                .header-data{\r\n                  border: 1px solid #1aac9b;\r\n                  margin-bottom: 10px !important;\r\n                  padding: 0px 10px 0px 10px;\r\n                  box-shadow: 0 0 .1em #000;\r\n                  margin: 10px 10px;\r\n                  background: #dedede\r\n                }\r\n\r\n                .header-info{\r\n                  border: 1px solid #1aac9b;\r\n                  padding: 0px 10px 0px 10px;\r\n                  box-shadow: 0 0 .1em #000;\r\n                  margin: 10px 10px;\r\n                  background: #dedede\r\n                }\r\n\r\n                .header-box h2{\r\n                   padding-left: 10px;\r\n                   text-shadow: 0 0 .3em #000;\r\n                }\r\n\r\n\r\n                .header-info h3{\r\n                  text-align: center;\r\n                }\r\n\r\n                input[type=\"text\"]{\r\n                    width: 160px;\r\n                    margin-bottom: 4px;\r\n                }\r\n\r\n                .input-size input[type=\"text\"]{\r\n                    width: 50px !important;\r\n                }\r\n\r\n                .input-size-2 input[type=\"text\"]{\r\n                    width: 70px !important;\r\n                }\r\n\r\n                p select {\r\n                    width: 160px;\r\n                    margin-bottom: 4px;\r\n                }\r\n\r\n                .base-margin {\r\n                    margin-left: 15px;\r\n                }\r\n\r\n                .submit-btn {\r\n                    flex: 1;\r\n                    margin: 10px 15px;\r\n                }\r\n\r\n                 .submit-btn input{\r\n                   color: #fff;\r\n                   background: #1aac9b;\r\n                   padding: 8px;\r\n                   width: 12.8em;\r\n                   font-weight: bold;\r\n                   text-shadow: 0 0 .3em black;\r\n                   font-size: 9pt;\r\n                   border-radius: 5px 5px;\r\n                }\r\n\r\n                .label-tag {\r\n                   color: #fff;\r\n                   background: #1aac9b;\r\n                   padding: 7px;\r\n                   font-weight: bold;\r\n                   text-shadow: 0 0 .3em black;\r\n                   border-radius: 5px 5px;\r\n                   width: 95%;\r\n                   display: inline-block;\r\n                }\r\n\r\n                &lt;/style&gt;\r\n                &lt;script type=\"text/javascript\"&gt;\r\n                    function findAutoCompleteErrors() {\r\n                        /* see if there are  errors in option fields */\r\n                        var containError = false;\r\n                        var ary = $j(\".optionAutoCompleteHidden\");\r\n                        $j.each(ary,function(index, value){\r\n                            if(value.value == \"ERROR\"){\r\n                                containError=true;\r\n                            }\r\n                        });\r\n                        return containError;\r\n                    }\r\n                    $j(function() {\r\n                        $j(\'.submitButton\').click(function(event) {\r\n                            if(!findAutoCompleteErrors()){\r\n                                $j(\'.submitButton\').prop(\'disabled\', true);\r\n                            }\r\n                        });\r\n                    });\r\n                &lt;/script&gt;\r\n            &lt;/head&gt;\r\n            &lt;body&gt;\r\n                \r\n            &lt;div class=\"main\"&gt;\r\n                \r\n                &lt;div class=\"header-box\"&gt;\r\n                    &lt;h2&gt;FICHA CLÍNICA&lt;/h2&gt;\r\n                &lt;/div&gt;\r\n\r\n                &lt;div class=\"content\"&gt;\r\n\r\n                    &lt;div class=\"header\"&gt;\r\n\r\n                        &lt;div class=\"header-data\"&gt;\r\n                                &lt;p&gt;\r\n                                &lt;label&gt;Nome:&lt;/label&gt;\r\n                                &lt;lookup expression=\"patient.personName\"/&gt;\r\n                            &lt;/p&gt;\r\n    \r\n                            &lt;p&gt;\r\n                                &lt;label&gt;Género/Data de Nasc./Idade:&lt;/label&gt;\r\n                                &lt;lookup expression=\"patient.gender\"/&gt; - &lt;lookup expression=\"patient.birthdate\"/&gt; - &lt;lookup expression=\"patient.age\"/&gt;\r\n                            &lt;/p&gt;\r\n                        &lt;/div&gt;\r\n    \r\n                        &lt;div class=\"header-info\"&gt;\r\n                            &lt;h3&gt;REPÚBLICA DE MOÇAMBIQUE&lt;/h3&gt;\r\n                            &lt;h3&gt;SERVIÇO NACIONAL DE SAÚDE&lt;/h3&gt;\r\n                            &lt;p&gt;\r\n                                &lt;label&gt;NID/US: &lt;lookup expression=\"patient.getPatientIdentifier(2)\"/&gt;&lt;/label&gt;\r\n                            &lt;/p&gt;\r\n                        &lt;/div&gt;\r\n                    &lt;/div&gt;\r\n                    \r\n                    &lt;div class=\"line-break\"&gt;&lt;/div&gt;\r\n\r\n                    &lt;div class=\"base-margin\"&gt;\r\n                        &lt;p&gt;\r\n                            &lt;label&gt;Unidade Sanitária:&lt;/label&gt;\r\n                            &lt;encounterLocation id=\"localConsulta\" default=\"GlobalProperty:default_location\" type=\"autocomplete\"/&gt;\r\n                        &lt;/p&gt;\r\n\r\n                        &lt;p&gt;\r\n                            &lt;obs conceptId=\"c7c0b430-bbc1-4042-a365-ad78a13aef56\" labelText=\"População Chave:\" answerConceptIds=\"e1daa454-1d5f-11e0-b929-000c29ad1d07, 5bdb7ec1-908a-11e6-a98e-000c29db4475, 58021703-908a-11e6-a98e-000c29db4475, e1df1296-1d5f-11e0-b929-000c29ad1d07, e1e783ea-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"HSH, PID, REC, MTS, Outro\"/&gt;\r\n                            &lt;obs conceptId=\"e1e783ea-1d5f-11e0-b929-000c29ad1d07\" labelText=\"Outra (Especifique):\"/&gt;\r\n                        &lt;/p&gt;\r\n                        \r\n                        &lt;p&gt;\r\n                            &lt;obs labelText=\"População Vulnerável:\" conceptId=\"814a2be7-43db-49e5-a870-2ca1fedacb69\" answerConceptIds=\"95f393be-3853-4d63-8640-4a505f9ea81b, 2ccb7192-7321-4156-b25a-f656e065dcbc, e1e06ac4-1d5f-11e0-b929-000c29ad1d07, e1e051a6-1d5f-11e0-b929-000c29ad1d07, e1d8dffc-1d5f-11e0-b929-000c29ad1d07, cbb0baba-688d-4c7b-afb1-7d5be5d9a084, e1df3a8c-1d5f-11e0-b929-000c29ad1d07, e1df209c-1d5f-11e0-b929-000c29ad1d07, e1df2204-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"Rapariga entre os 10-14 anos, Mulher jovem entre 15-24, Casais serodiscordantes, Pessoas vivendo com HIV Sida (PVHS), Crianças órfãos e vulneráveis, Pessoa com deficiência, Mineiro, Camionista, Trabalhador sazonal\" /&gt;&lt;br/&gt;\r\n                        &lt;/p&gt;\r\n                    \r\n                    &lt;/div&gt;\r\n\r\n                    &lt;div class=\"line-break\"&gt;&lt;/div&gt;\r\n\r\n                    &lt;div class=\"base-margin\"&gt;\r\n                        &lt;p&gt;\r\n                            &lt;label&gt;Consulta Actual / Outros:&lt;/label&gt;&lt;br/&gt;\r\n                            &lt;encounterDate id=\"dataConsulta\" required=\"true\" /&gt;\r\n                        &lt;/p&gt;  \r\n                        \r\n                        &lt;p&gt;\r\n                            &lt;label&gt;Proxima Consulta:&lt;/label&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"e1dae630-1d5f-11e0-b929-000c29ad1d07\" allowFutureDates=\"true\" /&gt;\r\n                        &lt;/p&gt;     \r\n                    &lt;/div&gt;\r\n\r\n                    &lt;div class=\"base-margin\"&gt;                    \r\n                        &lt;p class=\"input-size\" &gt;\r\n                            &lt;label&gt;Tensão Arterial:&lt;/label&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"e1e2e3d0-1d5f-11e0-b929-000c29ad1d07\"/&gt; / &lt;obs conceptId=\"e1e2e4e8-1d5f-11e0-b929-000c29ad1d07\"/&gt;\r\n                        &lt;/p&gt;     \r\n\r\n                        &lt;p&gt;\r\n                            &lt;label&gt;&lt;/label&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"e1e056a6-1d5f-11e0-b929-000c29ad1d07\" style=\"checkbox\" answerConceptId=\"e1d81b62-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"Gravidez\"/&gt;\r\n                        &lt;/p&gt;  \r\n                    &lt;/div&gt; \r\n\r\n                    &lt;div class=\"base-margin\"&gt;                    \r\n\r\n                        &lt;p&gt;\r\n                            &lt;label&gt;Data. última mestruação:&lt;/label&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"e1dc0dd0-1d5f-11e0-b929-000c29ad1d07\" /&gt;\r\n                        &lt;/p&gt;\r\n\r\n                        &lt;p&gt;\r\n                            &lt;label&gt;&lt;/label&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"bc4fe755-fc8f-49b8-9956-baf2477e8313\" style=\"checkbox\" answerConceptId=\"e1d81b62-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"Lactante\"/&gt;\r\n                        &lt;/p&gt;   \r\n                    &lt;/div&gt; \r\n\r\n                    &lt;div class=\"base-margin\"&gt;\r\n                            \r\n                        &lt;label class=\"label-tag\"&gt;Planeamento Familiar:&lt;/label&gt;\r\n\r\n                        &lt;div class=\"space-between\"&gt;\r\n\r\n                            &lt;div&gt;\r\n                                &lt;p&gt;\r\n &lt;obs conceptId=\"e1d1a6d8-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1d85294-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"Não\" /&gt;&lt;br/&gt;                                   \r\n&lt;obs conceptId=\"e1d1a6d8-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1cff2ac-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"Preservativo (PRESS)\" /&gt;&lt;br/&gt;\r\n                                    &lt;obs conceptId=\"e1d1a6d8-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1d5c786-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"Contraceptivo Oral (PIL)\" /&gt;&lt;br/&gt;\r\n                                    &lt;obs conceptId=\"e1d1a6d8-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1e492ca-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"Injectável (INJ)\" /&gt;&lt;br/&gt;\r\n                                    &lt;obs conceptId=\"e1d1a6d8-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"b69a31ae-ef74-4daa-b7fe-5a153948a2cd\" answerLabel=\"Implante (IMP)\" /&gt;&lt;br/&gt;\r\n                                &lt;/p&gt;\r\n                            &lt;/div&gt;\r\n\r\n                            &lt;div class=\"base-margin\"&gt;\r\n                                &lt;p&gt;\r\n                                    &lt;obs conceptId=\"e1d1a6d8-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1e485fa-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"Dispositivo Intra-uterino (DIU)\" /&gt;&lt;br/&gt;\r\n                                    &lt;obs conceptId=\"e1d1a6d8-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1e486f4-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"Laqueação das Trompas (LT)\" /&gt;&lt;br/&gt;\r\n                                    &lt;obs conceptId=\"e1d1a6d8-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"0b9a8904-3c82-4b9a-9f15-50a2509cacf9\" answerLabel=\"Vasectomia (VAS)\" /&gt;&lt;br/&gt;\r\n                                    &lt;obs conceptId=\"e1d1a6d8-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"908967c6-57be-4fa8-859c-51ad614e4307\" answerLabel=\"Método Amenorreia Lactacional (MAL)\"/&gt;&lt;br/&gt;\r\n                                    \r\n                                    &lt;label&gt;Outro:&lt;/label&gt;\r\n                                    &lt;obs conceptId=\"20ba316b-ef66-4f39-a1af-1e978aa02d18\"/&gt;\r\n                                &lt;/p&gt;\r\n                            &lt;/div&gt;\r\n\r\n                        &lt;/div&gt;\r\n                    &lt;/div&gt;\r\n\r\n                    &lt;div class=\"base-margin\"&gt;                    \r\n                        &lt;p&gt;\r\n                            &lt;label&gt;Estadio OMS:&lt;/label&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"e1e53c02-1d5f-11e0-b929-000c29ad1d07\" answerConceptIds=\"e1d9055e-1d5f-11e0-b929-000c29ad1d07, e1d9066c-1d5f-11e0-b929-000c29ad1d07, e1d9077a-1d5f-11e0-b929-000c29ad1d07, e1d90888-1d5f-11e0-b929-000c29ad1d07\" /&gt;\r\n                        &lt;/p&gt;\r\n\r\n                        &lt;p&gt;\r\n                            &lt;label&gt;Criança Edemas:&lt;/label&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"4de87b19-68b3-4efb-b591-769f11611247\" answerConceptIds=\"fa1768bf-0d59-45f6-8673-187e45f68bbc, 6e5f36df-42c0-42d5-aeb5-f447e76288c4, dc3faae7-be20-4919-b51f-3643650d49f9, 68c97735-5a99-4c0f-8ffc-d19674a39146\" /&gt;\r\n                        &lt;/p&gt;   \r\n                    &lt;/div&gt;\r\n\r\n                    &lt;div class=\"base-margin\"&gt;                \r\n                        \r\n                        &lt;p class=\"input-size-2\"&gt;\r\n                            &lt;label&gt;Peso (Kg):&lt;/label&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"e1e2e826-1d5f-11e0-b929-000c29ad1d07\" /&gt;\r\n                        &lt;/p&gt;\r\n\r\n                        &lt;p class=\"input-size-2\"&gt;\r\n                            &lt;label&gt;Comprimento &lt;br/&gt; ou Altura (cm):&lt;/label&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"e1e2e934-1d5f-11e0-b929-000c29ad1d07\" /&gt;\r\n                        &lt;/p&gt;   \r\n                    &lt;/div&gt; \r\n\r\n                    &lt;div class=\"base-margin\"&gt;                  \r\n                        &lt;p class=\"input-size-2\"&gt;\r\n                            &lt;label&gt;PB:&lt;/label&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"e1da53be-1d5f-11e0-b929-000c29ad1d07\" /&gt;\r\n                        &lt;/p&gt;\r\n\r\n                        &lt;p class=\"input-size-2\"&gt;\r\n                            &lt;label&gt;IMC (Kg/m2):&lt;/label&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"e1da52ba-1d5f-11e0-b929-000c29ad1d07\" /&gt;\r\n                        &lt;/p&gt;   \r\n                    &lt;/div&gt; \r\n\r\n                    &lt;div class=\"line-break\"&gt;&lt;/div&gt;\r\n\r\n                    &lt;div class=\"base-margin\"&gt;  \r\n                        &lt;p&gt;\r\n                            &lt;label&gt;Ava. Nutric. Indicador:&lt;/label&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"4b4280d6-976d-4b0d-90b3-e28adb431f61\" answerConceptIds=\"98d34752-3034-4d22-81d5-2ab0c646406e, d33778f5-9bc2-4e04-aa5a-0af6002c540a, e1da52ba-1d5f-11e0-b929-000c29ad1d07, e1da53be-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"IMC/IDADE, P/E, IMC, PB\" /&gt;\r\n                        &lt;/p&gt;\r\n\r\n                        &lt;p&gt;\r\n                            &lt;label&gt;Ava. Nutric. Grau:&lt;/label&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"0b1a2c8c-55d2-42a8-a3d6-62828f52d49a\" answerConceptIds=\"e1d85b22-1d5f-11e0-b929-000c29ad1d07, aa84f34d-11f7-4466-b784-0fdda716ace2,e1cf1422-1d5f-11e0-b929-000c29ad1d07, e1dec764-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"Normal, Ligeira, DAM, DAG\" /&gt;\r\n                        &lt;/p&gt;   \r\n                    &lt;/div&gt; \r\n\r\n                    &lt;div class=\"base-margin\"&gt;\r\n                        &lt;label&gt;&lt;/label&gt;                  \r\n                        &lt;p&gt;\r\n                            &lt;label&gt;Apoio/Educação Nutric.:&lt;/label&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"e1e205f0-1d5f-11e0-b929-000c29ad1d07\" answerConceptIds=\"e1d81c70-1d5f-11e0-b929-000c29ad1d07,e1d81b62-1d5f-11e0-b929-000c29ad1d07, 014
-76fb-c7ee-404c-b913-9795a108015e, e1e204ec-1d5f-11e0-b929-000c29ad1d07\"  answerLabels=\"Não, Educação, ATPU, Soja\" /&gt;\r\n                        &lt;/p&gt;\r\n\r\n                        &lt;p&gt;\r\n                            &lt;label&gt;Quantidade:&lt;/label&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"28eaa9c2-2519-4937-bd3c-ba52b2b49f2f\" /&gt;\r\n                        &lt;/p&gt;   \r\n                    &lt;/div&gt;\r\n\r\n                     &lt;div class=\"base-margin\"&gt;\r\n                        &lt;label class=\"label-tag\"&gt;Tuberculose:&lt;/label&gt;\r\n                        \r\n                        &lt;div class=\"space-between\"&gt;\r\n                            &lt;p&gt;\r\n                                &lt;label&gt;Tem Sintomas?&lt;/label&gt;&lt;br/&gt;\r\n                                &lt;obs conceptId=\"2eab4e55-d0d0-4fa8-8d23-b40eaaee44c8\" answerConceptIds=\"e1d81b62-1d5f-11e0-b929-000c29ad1d07, e1d81c70-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"Sim, Não\" /&gt;\r\n                            &lt;/p&gt;\r\n\r\n                            &lt;div class=\"base-margin\"&gt;         \r\n                                &lt;p&gt;\r\n                                    &lt;label&gt;Diagnótico TB activo&lt;/label&gt;&lt;br/&gt;\r\n                                    &lt;obs conceptId=\"63b15479-5a05-4bdc-a6e5-eab175743122\" answerConceptIds=\"e1d81b62-1d5f-11e0-b929-000c29ad1d07, e1d81c70-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"Sim, Não\" /&gt;\r\n                                &lt;/p&gt;\r\n        \r\n                                &lt;p class=\"input-size-2\"&gt;\r\n                                    &lt;label&gt;Tratamento TB:&lt;/label&gt;&lt;br/&gt;\r\n                                    &lt;obs conceptId=\"e1d9fbda-1d5f-11e0-b929-000c29ad1d07\" answerConceptIds=\"e1d9ef28-1d5f-11e0-b929-000c29ad1d07, e1d9f036-1d5f-11e0-b929-000c29ad1d07, e1d9facc-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"Início (I), Continua (C), Fim (F)\" dateLabel=\"Data:\"/&gt;\r\n                                &lt;/p&gt;   \r\n                            &lt;/div&gt; \r\n\r\n                        &lt;/div&gt;\r\n                        \r\n                        &lt;div&gt;\r\n                            &lt;label class=\"label-tag\"&gt;Quais sintomas de TB:&lt;/label&gt;\r\n    \r\n                            &lt;div class=\"space-between\"&gt;\r\n    \r\n                                &lt;div&gt;\r\n                                    &lt;p&gt;\r\n                                        &lt;obs conceptId=\"e1de6d1e-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1de6878-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"Febre (F)\"/&gt;&lt;br/&gt;\r\n                                        &lt;obs conceptId=\"e1de6d1e-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1de6a12-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"Emagrecimento (E)\"/&gt;&lt;br/&gt;\r\n                                        &lt;obs conceptId=\"e1de6d1e-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1de66e8-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"Sudorese Noturna (S)\"/&gt;&lt;br/&gt;\r\n                                        &lt;obs conceptId=\"e1de6d1e-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1de63d2-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"Tosse a mais de 2 semanas (T)\"/&gt;\r\n                                    &lt;/p&gt; \r\n                                &lt;/div&gt; \r\n                                \r\n                                &lt;div  class=\"base-margin\"&gt;\r\n                                    &lt;p&gt;\r\n                                        &lt;obs conceptId=\"e1de6d1e-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"44b63d4c-341b-48f0-baa0-ce88ed7afc71\" answerLabel=\"Astenia (A)\"/&gt;&lt;br/&gt;\r\n                                        &lt;obs conceptId=\"e1de6d1e-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1de6b98-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"Contacto com TB (C)\"/&gt;&lt;br/&gt;\r\n                                        &lt;obs conceptId=\"e1de6d1e-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1cfd43e-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"Adenopatia Cervical Indolor\"/&gt;\r\n                                    &lt;/p&gt;   \r\n                                &lt;/div&gt;\r\n    \r\n                            &lt;/div&gt;\r\n                        &lt;/div&gt;\r\n                    &lt;/div&gt;\r\n\r\n                    &lt;div class=\"base-margin\"&gt;\r\n                        &lt;p&gt;\r\n                            &lt;label&gt;Profilaxia (INH):&lt;/label&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"be4a76ca-662a-4c39-903b-71983f5f67c9\" answerConceptIds=\"e1d9ef28-1d5f-11e0-b929-000c29ad1d07, e1d9f036-1d5f-11e0-b929-000c29ad1d07, e1d9facc-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"Início (I), Continua (C), Fim (F)\"/&gt;\r\n                        &lt;/p&gt;\r\n\r\n                        &lt;p&gt;\r\n                            &lt;label&gt;Profilaxia (CTZ):&lt;/label&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"2616b3c9-9a99-4b9a-b673-10871f4a4c71\" answerConceptIds=\"e1d9ef28-1d5f-11e0-b929-000c29ad1d07, e1d9f036-1d5f-11e0-b929-000c29ad1d07, e1d9facc-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"Início (I), Continua (C), Fim (F)\"/&gt;\r\n                        &lt;/p&gt;   \r\n                    &lt;/div&gt;\r\n\r\n                    &lt;div  class=\"base-margin\"&gt;\r\n                        &lt;p&gt;\r\n                            &lt;label&gt;Efeitos Secundários (INH):&lt;/label&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"01ce78dd-074b-407c-ba30-27ec9336e0f8\" answerConceptIds=\"e1d81b62-1d5f-11e0-b929-000c29ad1d07, e1d81c70-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"Sim, Não\"/&gt;\r\n                        &lt;/p&gt;\r\n\r\n                        &lt;p&gt;\r\n                            &lt;label&gt;Efeitos Secundários (CTZ):&lt;/label&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"689cd895-eb45-4712-9b41-8756bc0514ed\" answerConceptIds=\"e1d81b62-1d5f-11e0-b929-000c29ad1d07, e1d81c70-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"Sim, Não\"/&gt;\r\n                        &lt;/p&gt;   \r\n                    &lt;/div&gt;\r\n\r\n                    &lt;div class=\"line-break\"&gt;&lt;/div&gt;\r\n\r\n                    &lt;div class=\"base-margin\"&gt;\r\n                        &lt;label class=\"label-tag\"&gt;ITS&lt;/label&gt;                    \r\n                        &lt;p&gt;\r\n                            &lt;label&gt;Tem sintomas?&lt;/label&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"794ef662-03bc-4e22-90ff-38742b82827a\" answerConceptIds=\"e1d81b62-1d5f-11e0-b929-000c29ad1d07, e1d81c70-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"Sim, Não\" /&gt;\r\n                        &lt;/p&gt;\r\n                        \r\n                        &lt;label class=\"label-tag\"&gt;Diagnóstico ITS:&lt;/label&gt;\r\n                        &lt;p&gt;\r\n                            &lt;obs conceptId=\"e1cfe1e0-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1d01584-1d5f-11e0-b929-000c29ad1d07\"  answerLabel=\"Sifilis (SIF)\"/&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"e1cfe1e0-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1eb356c-1d5f-11e0-b929-000c29ad1d07\"  answerLabel=\"Corrimento Vaginal (CV)\"/&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"e1cfe1e0-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1eb3792-1d5f-11e0-b929-000c29ad1d07\"  answerLabel=\"Corrimento Uretral (CUM)\"/&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"e1cfe1e0-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1d62cee-1d5f-11e0-b929-000c29ad1d07\"  answerLabel=\"Úlcera Genital (UG)\"/&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"e1cfe1e0-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1d689d2-1d5f-11e0-b929-000c29ad1d07\"  answerLabel=\"Dor no Baixo Ventre (DIP)\"/&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"e1cfe1e0-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"29c0b8c9-9086-11e6-a98e-000c29db4475\"  answerLabel=\"Escroto Inchado (ESI)\"/&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"e1cfe1e0-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"99fd3825-9082-11e6-a98e-000c29db4475\"  answerLabel=\"Bubão Inguinal (BI)\"/&gt;\r\n                        &lt;/p&gt;   \r\n                    &lt;/div&gt;\r\n\r\n                    &lt;div class=\"base-margin\"&gt;\r\n                        &lt;label class=\"label-tag\"&gt;Infecções oportunistas &lt;br/&gt; incluindo Sarcoma de &lt;br/&gt; Kaposi e outras doenças:&lt;/label&gt;           \r\n                        &lt;p&gt;\r\n                            &lt;obs conceptId=\"e1dae234-1d5f-11e0-b929-000c29ad1d07\" answerConceptIds=\"e1cda114-1d5f-11e0-b929-000c29ad1d07, \r\n                                                                                                    e1cff5d6-1d5f-11e0-b929-000c29ad1d07, \r\n                                                                                                    e1e529a6-1d5f-11e0-b929-000c29ad1d07, \r\n                                                                                                    e1e5232a-1d5f-11e0-b929-000c29ad1d07, \r\n                                                                                                    e1cf4e24-1d5f-11e0-b929-000c29ad1d07, \r\n                                                                                                    c3e82fe4-9086-11e6-a98e-000c29db4475, \r\n                                                                                                    e1e2530c-1d5f-11e0-b929-000c29ad1d07, \r\n                                                                                                    a8bc94b7-9082-11e6-a98e-000c29db4475, \r\n                                                                                                    c03d9343-9082-11e6-a98e-000c29db4475, \r\n                                                                                                    e1cfcdea-1d5f-11e0-b929-000c29ad1d07, \r\n                                                                                                    a02a1759-9082-11e6-a98e-000c29db4475, \r\n                                                                                                    e1eafbce-1d5f-11e0-b929-000c29ad1d07,\r\n                                                                                                    e1cffa18-1d5f-11e0-b929-000c29ad1d07,\r\n                                                                                                    e1cf5590-1d5f-11e0-b929-000c29ad1d07,\r\n                                                                                                    e1e52f28-1d5f-11e0-b929-000c29ad1d07,\r\n                                                                                                    e1d608cc-1d5f-11e0-b929-000c29ad1d07,\r\n                                                                                                    e1d69314-1d5f-11e0-b929-000c29ad1d07,\r\n                                                                                                    e1cf405a-1d5f-11e0-b929-000c29ad1d07,\r\n                                                                                                    e1cde53e-1d5f-11e0-b929-000c29ad1d07,\r\n                                                                                                    e1cdea3e-1d5f-11e0-b929-000c29ad1d07,\r\n                                                                                                    e1d90dce-1d5f-11e0-b929-000c29ad1d07, \r\n                                                                                                    e1d0103e-1d5f-11e0-b929-000c29ad1d07,\r\n                                                                                                    e1cdd490-1d5f-11e0-b929-000c29ad1d07,\r\n                                                                                                    e1d6412a-1d5f-11e0-b929-000c29ad1d07,\r\n                                                                                                    e1d2984a-1d5f-11e0-b929-000c29ad1d07,\r\n                                                                                                    61a93abd-9087-11e6-a98e-000c29db4475,\r\n                                                                                                    e1d01476-1d5f-11e0-b929-000c29ad1d07,\r\n                                                                                                    e1d607b4-1d5f-11e0-b929-000c29ad1d07,\r\n                                                                                                    de8f1eeb-9082-11e6-a98e-000c29db4475,\r\n                                                                                                    e1e2b07c-1d5f-11e0-b929-000c29ad1d07,\r\n                                                                                                    e1cdd38c-1d5f-11e0-b929-000c29ad1d07,\r\n                                                                                                    e1d657c8-1d5f-11e0-b929-000c29ad1d07,\r\ne1dc8ac6-1d5f-11e0-b929-000c29ad1d07\" \r\n\r\n                                                                                answerLabels=\"Anemia, \r\n                                                                                            Broncopneumonia, \r\n                                                                                            Candidiase esofágica, \r\n                                                                                            Candidiase Oral, \r\n                                                                                            Dermatite, \r\n                                                                                            Diabetes Mellitus, \r\n                                                                                            Diarreia crónica, \r\n                                                                                            Encefalite, \r\n                                                                                            Encefalopatia por HIV, \r\n                                                                                            Epilepsia, \r\n                                                                                            Estomatite, \r\n                                                                                            Febre Inexplicada,\r\n                                                                                            Gastroenterite aguda (GEA),\r\n                                                                                            Gengivite,\r\n                                                                                            Hérpes Simples,\r\n                                                                                            Hérpes Zoster,\r\n                                                                                            Hipertensão Arterial (HTA),\r\n                                                                                            Infecção das Vias Respiratórias Superiores (IVRS),\r\n                                                                                            Infecção Urinária,\r\n                                                                                            Meningite,\r\n                                                                                            Molusco Contagioso, \r\n                                                                                            Otite,\r\n                                                                                            Pneumonia,\r\n                                                                                            Prurigo,\r\n                                                                                            Sarcoma de Kaposi (SK),\r\n                                                                                            Síndrome de caquexia,\r\n                                                                                            Sinusite,\r\n                                                                                            Tinha,\r\n                                                                                            Toxoplasmose,\r\n                                                                                            Tuberculose Extrapulmonar,\r\n                                                                                            Tuberculose Pulmonar,\r\n                                                                                            Varicela,Cancro do Colo Uterino\"/&gt;&lt;br/&gt;\r\n                        &lt;/
-&gt;\r\n                        &lt;p</t>
+    <t xml:space="preserve">&lt;htmlform&gt;\r\n            &lt;html xmlns=\"http://www.w3.org/1999/xhtml\"&gt;\r\n            &lt;head&gt;\r\n            &lt;meta http-equiv=\"Content-Type\" content=\"text/html; charset=utf-8\" /&gt;\r\n            &lt;title&gt;FICHA CLÍNICA&lt;/title&gt;\r\n              \r\n              &lt;style&gt;\r\n\r\n                .main{\r\n                    display: flex;\r\n                    align-items: center;\r\n                    flex-direction: column;\r\n                    font-size: .9em;\r\n                    width: 100%;\r\n                }\r\n\r\n                .header-box{\r\n                    width: 85%;\r\n                    background: #1aac9b;\r\n                    padding: 1px !important;\r\n                    color: #fff;\r\n                    box-shadow: 0 0 .3em #000;\r\n                    margin-bottom: 10px;\r\n                }\r\n                \r\n                .content {\r\n                    display: flex;\r\n                    flex-flow: row wrap;\r\n                    width: 85%;\r\n                    border: 1px solid #1aac9b;\r\n                    box-shadow: 0 0 .3em #000;\r\n                }\r\n\r\n                .line-break {\r\n                    width: 100%;\r\n                }\r\n\r\n                .header, .space-between{\r\n                    display: flex;\r\n                    flex-flow: row wrap;\r\n                    justify-content: space-between;\r\n                    align-content: space-between;\r\n                    width: 100%;\r\n                }\r\n\r\n                .header-data{\r\n                  border: 1px solid #1aac9b;\r\n                  margin-bottom: 10px !important;\r\n                  padding: 0px 10px 0px 10px;\r\n                  box-shadow: 0 0 .1em #000;\r\n                  margin: 10px 10px;\r\n                  background: #dedede\r\n                }\r\n\r\n                .header-info{\r\n                  border: 1px solid #1aac9b;\r\n                  padding: 0px 10px 0px 10px;\r\n                  box-shadow: 0 0 .1em #000;\r\n                  margin: 10px 10px;\r\n                  background: #dedede\r\n                }\r\n\r\n                .header-box h2{\r\n                   padding-left: 10px;\r\n                   text-shadow: 0 0 .3em #000;\r\n                }\r\n\r\n\r\n                .header-info h3{\r\n                  text-align: center;\r\n                }\r\n\r\n                input[type=\"text\"]{\r\n                    width: 160px;\r\n                    margin-bottom: 4px;\r\n                }\r\n\r\n                .input-size input[type=\"text\"]{\r\n                    width: 50px !important;\r\n                }\r\n\r\n                .input-size-2 input[type=\"text\"]{\r\n                    width: 70px !important;\r\n                }\r\n\r\n                p select {\r\n                    width: 160px;\r\n                    margin-bottom: 4px;\r\n                }\r\n\r\n                .base-margin {\r\n                    margin-left: 15px;\r\n                }\r\n\r\n                .submit-btn {\r\n                    flex: 1;\r\n                    margin: 10px 15px;\r\n                }\r\n\r\n                 .submit-btn input{\r\n                   color: #fff;\r\n                   background: #1aac9b;\r\n                   padding: 8px;\r\n                   width: 12.8em;\r\n                   font-weight: bold;\r\n                   text-shadow: 0 0 .3em black;\r\n                   font-size: 9pt;\r\n                   border-radius: 5px 5px;\r\n                }\r\n\r\n                .label-tag {\r\n                   color: #fff;\r\n                   background: #1aac9b;\r\n                   padding: 7px;\r\n                   font-weight: bold;\r\n                   text-shadow: 0 0 .3em black;\r\n                   border-radius: 5px 5px;\r\n                   width: 95%;\r\n                   display: inline-block;\r\n                }\r\n\r\n                &lt;/style&gt;\r\n                \r\n                    &lt;script type=\"text/javascript\"&gt;\r\n\r\n      var estadoProgramaPTVConceptID = parseInt(\"&lt;lookup expression=\"fn.currentProgramWorkflowStatus(5).state.concept.id\" /&gt;\");\r\n\r\n      jQuery(function () {\r\n        getField(\'gravidez.value\').change(function () {\r\n          if (getValue(\'gravidez.value\') == 1465) {\r\n            $j(\"#dataUltimaMestruacao input\").attr(\'disabled\', false);\r\n            if (isNaN(estadoProgramaPTVConceptID)) {\r\n              window.alert(\'Deve admitir este paciente no programa PTV\');\r\n            } else {\r\n              if (!(estadoProgramaPTVConceptID == 1982)) {\r\n                window.alert(\'Este paciente não está no estado activo no programa PTV, coloque-o como activo primeiro\');\r\n              }\r\n            }\r\n          }\r\n          else {\r\n            $j(\"#dataUltimaMestruacao input\").attr(\'disabled\', true);\r\n            setValue(\'dataUltimaMestruacao.value\',\'\');\r\n          }\r\n        })\r\n      });\r\n\r\n      jQuery(function () {\r\n        getField(\'lactante.value\').change(function () {\r\n          if (getValue(\'lactante.value\') == 1065) {\r\n            $j(\"#dataUltimaMestruacao input\").attr(\'disabled\', false);\r\n            if (isNaN(estadoProgramaPTVConceptID)) {\r\n              window.alert(\'Deve admitir este paciente no programa PTV\');\r\n            } else {\r\n              if (!(estadoProgramaPTVConceptID == 1982)) {\r\n                window.alert(\'Este paciente não está no estado activo no programa PTV, coloque-o como activo primeiro\');\r\n              }\r\n            }\r\n          }\r\n        })\r\n      });\r\n\r\n      function disableDataUltimaMenstruacao() {\r\n        jQuery(function () {\r\n          $j(\"#dataUltimaMestruacao input\").attr(\'disabled\', true);\r\n        });\r\n      }\r\n\r\n      window.onload = disableDataUltimaMenstruacao();\r\n    &lt;/script&gt;\r\n\r\n            &lt;/head&gt;\r\n            &lt;body&gt;\r\n                \r\n            &lt;div class=\"main\"&gt;\r\n                \r\n                &lt;div class=\"header-box\"&gt;\r\n                    &lt;h2&gt;FICHA CLÍNICA&lt;/h2&gt;\r\n                &lt;/div&gt;\r\n\r\n                &lt;div class=\"content\"&gt;\r\n\r\n                    &lt;div class=\"header\"&gt;\r\n\r\n                        &lt;div class=\"header-data\"&gt;\r\n                                &lt;p&gt;\r\n                                &lt;label&gt;Nome:&lt;/label&gt;\r\n                                &lt;lookup expression=\"patient.personName\"/&gt;\r\n                            &lt;/p&gt;\r\n    \r\n                            &lt;p&gt;\r\n                                &lt;label&gt;Género/Data de Nasc./Idade:&lt;/label&gt;\r\n                                &lt;lookup expression=\"patient.gender\"/&gt; - &lt;lookup expression=\"patient.birthdate\"/&gt; - &lt;lookup expression=\"patient.age\"/&gt;\r\n                            &lt;/p&gt;\r\n                           &lt;p&gt;\r\n                               &lt;label&gt;Telefone celular: &lt;/label&gt;\r\n                              &lt;lookup expression=\"patient.getAttribute(9)\"/&gt;\r\n                          &lt;/p&gt;\r\n                        &lt;/div&gt;\r\n    \r\n                        &lt;div class=\"header-info\"&gt;\r\n                            &lt;h3&gt;REPÚBLICA DE MOÇAMBIQUE&lt;/h3&gt;\r\n                            &lt;h3&gt;SERVIÇO NACIONAL DE SAÚDE&lt;/h3&gt;\r\n                            &lt;p&gt;\r\n                                &lt;label&gt;NID/US: &lt;lookup expression=\"patient.getPatientIdentifier(2)\"/&gt;&lt;/label&gt;\r\n                            &lt;/p&gt;\r\n                        &lt;/div&gt;\r\n                    &lt;/div&gt;\r\n                    \r\n                    &lt;div class=\"line-break\"&gt;&lt;/div&gt;\r\n\r\n                    &lt;div class=\"base-margin\"&gt;\r\n                        &lt;p&gt;\r\n                            &lt;label&gt;Unidade Sanitária:&lt;/label&gt;\r\n                            &lt;encounterLocation id=\"localConsulta\" default=\"GlobalProperty:default_location\" type=\"autocomplete\"/&gt;\r\n                        &lt;/p&gt;\r\n\r\n                        &lt;p&gt;\r\n                            &lt;obs conceptId=\"c7c0b430-bbc1-4042-a365-ad78a13aef56\" labelText=\"População Chave:\" answerConceptIds=\"e1daa454-1d5f-11e0-b929-000c29ad1d07, 5bdb7ec1-908a-11e6-a98e-000c29db4475, 58021703-908a-11e6-a98e-000c29db4475, e1df1296-1d5f-11e0-b929-000c29ad1d07, e1e783ea-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"HSH, PID, REC, MTS, Outro\"/&gt;\r\n                            &lt;obs conceptId=\"e1e783ea-1d5f-11e0-b929-000c29ad1d07\" labelText=\"Outra (Especifique):\"/&gt;\r\n                        &lt;/p&gt;\r\n                        \r\n                        &lt;p&gt;\r\n                            &lt;obs labelText=\"População Vulnerável:\" conceptId=\"814a2be7-43db-49e5-a870-2ca1fedacb69\" answerConceptIds=\"95f393be-3853-4d63-8640-4a505f9ea81b, 2ccb7192-7321-4156-b25a-f656e065dcbc, e1e06ac4-1d5f-11e0-b929-000c29ad1d07, e1e051a6-1d5f-11e0-b929-000c29ad1d07, e1d8dffc-1d5f-11e0-b929-000c29ad1d07, cbb0baba-688d-4c7b-afb1-7d5be5d9a084, e1df3a8c-1d5f-11e0-b929-000c29ad1d07, e1df209c-1d5f-11e0-b929-000c29ad1d07, e1df2204-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"Rapariga entre os 10-14 anos, Mulher jovem entre 15-24, Casais serodiscordantes, Pessoas vivendo com HIV Sida (PVHS), Crianças órfãos e vulneráveis, Pessoa com deficiência, Mineiro, Camionista, Trabalhador sazonal\" /&gt;&lt;br/&gt;\r\n                        &lt;/p&gt;\r\n                    \r\n                    &lt;/div&gt;\r\n\r\n                    &lt;div class=\"line-break\"&gt;&lt;/div&gt;\r\n\r\n                    &lt;div class=\"base-margin\"&gt;\r\n                        &lt;p&gt;\r\n                            &lt;label&gt;Consulta Actual / Outros:&lt;/label&gt;&lt;br/&gt;\r\n                            &lt;encounterDate id=\"dataConsulta\" required=\"true\" /&gt;\r\n                        &lt;/p&gt;  \r\n                        \r\n                        &lt;p&gt;\r\n                            &lt;label&gt;Proxima Consulta:&lt;/label&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"e1dae630-1d5f-11e0-b929-000c29ad1d07\" allowFutureDates=\"true\" /&gt;\r\n                        &lt;/p&gt;     \r\n                    &lt;/div&gt;\r\n\r\n                    \r\n                    &lt;div class=\"base-margin\"&gt;\r\n                      &lt;p&gt;\r\n                        &lt;label&gt;&lt;/label&gt;&lt;br /&gt;\r\n                        &lt;obs id=\"gravidez\" conceptId=\"e1e056a6-1d5f-11e0-b929-000c29ad1d07\" style=\"checkbox\"\r\n                          answerConceptId=\"e1d81b62-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"Gravidez\" /&gt;\r\n                      &lt;/p&gt;\r\n\r\n                      &lt;p class=\"input-size\"&gt;\r\n                        &lt;label&gt;Tensão Arterial:&lt;/label&gt;&lt;br /&gt;\r\n                        &lt;obs conceptId=\"e1e2e3d0-1d5f-11e0-b929-000c29ad1d07\" /&gt; /\r\n                        &lt;obs conceptId=\"e1e2e4e8-1d5f-11e0-b929-000c29ad1d07\" /&gt;\r\n                      &lt;/p&gt;\r\n                    &lt;/div&gt;\r\n\r\n                    &lt;div class=\"base-margin\"&gt;\r\n                      &lt;p&gt;\r\n                        &lt;label id=\"labelMestruacao\"&gt;Data. última mestruação:&lt;/label&gt;&lt;br /&gt;\r\n                        &lt;obs class=\"dataUltimaMestruacao\" id=\"dataUltimaMestruacao\"\r\n                          conceptId=\"e1dc0dd0-1d5f-11e0-b929-000c29ad1d07\" /&gt;\r\n                      &lt;/p&gt;\r\n\r\n                      &lt;p&gt;\r\n                        &lt;label&gt;&lt;/label&gt;&lt;br /&gt;\r\n                        &lt;obs id=\"lactante\" conceptId=\"bc4fe755-fc8f-49b8-9956-baf2477e8313\" style=\"checkbox\"\r\n                          answerConceptId=\"e1d81b62-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"Lactante\" /&gt;\r\n                      &lt;/p&gt;\r\n\r\n                    &lt;/div&gt;\r\n\r\n                    &lt;div class=\"base-margin\"&gt;\r\n                            \r\n                        &lt;label class=\"label-tag\"&gt;Planeamento Familiar:&lt;/label&gt;\r\n\r\n                        &lt;div class=\"space-between\"&gt;\r\n\r\n                            &lt;div&gt;\r\n                                &lt;p&gt;\r\n &lt;obs conceptId=\"e1d1a6d8-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1d85294-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"Não\" /&gt;&lt;br/&gt;                                   \r\n&lt;obs conceptId=\"e1d1a6d8-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1cff2ac-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"Preservativo (PRESS)\" /&gt;&lt;br/&gt;\r\n                                    &lt;obs conceptId=\"e1d1a6d8-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1d5c786-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"Contraceptivo Oral (PIL)\" /&gt;&lt;br/&gt;\r\n                                    &lt;obs conceptId=\"e1d1a6d8-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1e492ca-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"Injectável (INJ)\" /&gt;&lt;br/&gt;\r\n                                    &lt;obs conceptId=\"e1d1a6d8-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"b69a31ae-ef74-4daa-b7fe-5a153948a2cd\" answerLabel=\"Implante (IMP)\" /&gt;&lt;br/&gt;\r\n                                &lt;/p&gt;\r\n                            &lt;/div&gt;\r\n\r\n                            &lt;div class=\"base-margin\"&gt;\r\n                                &lt;p&gt;\r\n                                    &lt;obs conceptId=\"e1d1a6d8-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1e485fa-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"Dispositivo Intra-uterino (DIU)\" /&gt;&lt;br/&gt;\r\n                                    &lt;obs conceptId=\"e1d1a6d8-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1e486f4-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"Laqueação das Trompas (LT)\" /&gt;&lt;br/&gt;\r\n                                    &lt;obs conceptId=\"e1d1a6d8-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"0b9a8904-3c82-4b9a-9f15-50a2509cacf9\" answerLabel=\"Vasectomia (VAS)\" /&gt;&lt;br/&gt;\r\n                                    &lt;obs conceptId=\"e1d1a6d8-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"908967c6-57be-4fa8-859c-51ad614e4307\" answerLabel=\"Método Amenorreia Lactacional (MAL)\"/&gt;&lt;br/&gt;\r\n                                    \r\n                                    &lt;label&gt;Outro:&lt;/label&gt;\r\n                                    &lt;obs conceptId=\"20ba316b-ef66-4f39-a1af-1e978aa02d18\"/&gt;\r\n                                &lt;/p&gt;\r\n                            &lt;/div&gt;\r\n\r\n                        &lt;/div&gt;\r\n                    &lt;/div&gt;\r\n\r\n                    &lt;div class=\"base-margin\"&gt;                    \r\n                        &lt;p&gt;\r\n                            &lt;label&gt;Estadio OMS:&lt;/label&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"e1e53c02-1d5f-11e0-b929-000c29ad1d07\" answerConceptIds=\"e1d9055e-1d5f-11e0-b929-000c29ad1d07, e1d9066c-1d5f-11e0-b929-000c29ad1d07, e1d9077a-1d5f-11e0-b929-000c29ad1d07, e1d90888-1d5f-11e0-b929-000c29ad1d07\" /&gt;\r\n                        &lt;/p&gt;\r\n\r\n                        &lt;p&gt;\r\n                            &lt;label&gt;Criança Edemas:&lt;/label&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"4de87b19-68b3-4efb-b591-769f11611247\" answerConceptIds=\"fa1768bf-0d59-45f6-8673-187e45f68bbc, 6e5f36df-42c0-42d5-aeb5-f447e76288c4, dc3faae7-be20-4919-b51f-3643650d49f9, 68c97735-5a99-4c0f-8ffc-d19674a39146\" /&gt;\r\n                        &lt;/p&gt;   \r\n                    &lt;/div&gt;\r\n\r\n                    &lt;div class=\"base-margin\"&gt;                \r\n                        \r\n                        &lt;p class=\"input-size-2\"&gt;\r\n                            &lt;label&gt;Peso (Kg):&lt;/label&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"e1e2e826-1d5f-11e0-b929-000c29ad1d07\" /&gt;\r\n                        &lt;/p&gt;\r\n\r\n                        &lt;p class=\"input-size-2\"&gt;\r\n                            &lt;label&gt;Comprimento &lt;br/&gt; ou Altura (cm):&lt;/label&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"e1e2e934-1d5f-11e0-b929-000c29ad1d07\" /&gt;\r\n                        &lt;/p&gt;   \r\n                    &lt;/div&gt; \r\n\r\n                    &lt;div class=\"base-margin\"&gt;                  \r\n                        &lt;p class=\"input-size-2\"&gt;\r\n                            &lt;label&gt;PB:&lt;/label&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"e1da53be-1d5f-11e0-b929-000c29ad1d07\" /&gt;\r\n                        &lt;/p&gt;\r\n\r\n                        &lt;p class=\"input-size-2\"&gt;\r\n                            &lt;label&gt;IMC (Kg/m2):&lt;/label&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"e1da52ba-1d5f-11e0-b929-000c29ad1d07\" /&gt;\r\n                        &lt;/p&gt;   \r\n                    &lt;/div&gt; \r\n\r\n                    &lt;div class=\"line-break\"&gt;&lt;/div&gt;\r\n\r\n                    &lt;div class=\"base-margin\"&gt;  \r\n                        &lt;p&gt;\r\n                            &lt;label&gt;Ava. Nutric. Indicador:&lt;/label&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"4b4280d6-976d-4b0d-90b3-e28adb431f61\" answerConceptIds=\"98d34752-3034-4d22-81d5-2ab0c646406e, d33778f5-9bc2-4e04-aa5a-0af6002c540a, e1da52ba-1d5f-11e0-b929-000c29ad1d07, e1da53be-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"IMC/IDADE, P/E, IMC, PB\" /&gt;\r\n                        &lt;/p&gt;\r\n\r\n                        &lt;p&gt;\r\n                            &lt;label&gt;Ava. Nutric. Grau:&lt;/label&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"0b1a2c8c-55d2-42a8-a3d6-62828f52d49a\" answerConceptIds=\"e1d85b22-1d5f-11e0-b929-000c29ad1d07, aa84f34d-11f7-4466-b784-0fdda716ace2,e1cf1422-1d5f-11e0-b929-000c29ad1d07, e1dec764-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"Normal, Ligeira, DAM, DAG\" /&gt;\r\n                        &lt;/p&gt;   \r\n                    &lt;/div&gt; \r\n\r\n                    &lt;div class=\"base-margin\"&gt;\r\n                        &lt;label&gt;&lt;/label&gt;                  \r\n                        &lt;p&gt;\r\n                            &lt;label&gt;Apoio/Educação Nutric.:&lt;/label&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"e1e205f0-1d5f-11e0-b929-000c29ad1d07\" answerConceptIds=\"e1d81c70-1d5f-11e0-b929-000c29ad1d07,e1d81b62-1d5f-11e0-b929-000c29ad1d07, 014b76fb-c7ee-404c-b913-9795a108015e, e1e204ec-1d5f-11e0-b929-000c29ad1d07\"  answerLabels=\"Não, Educação, ATPU, Soja\" /&gt;\r\n                        &lt;/p&gt;\r\n\r\n                        &lt;p&gt;\r\n                            &lt;label&gt;Quantidade:&lt;/label&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"28eaa9c2-2519-4937-bd3c-ba52b2b49f2f\" /&gt;\r\n                        &lt;/p&gt;   \r\n                    &lt;/div&gt;\r\n\r\n                     &lt;div class=\"base-margin\"&gt;\r\n                        &lt;label class=\"label-tag\"&gt;Tuberculose:&lt;/label&gt;\r\n                        \r\n                        &lt;div class=\"space-between\"&gt;\r\n                            &lt;p&gt;\r\n                                &lt;label&gt;Tem Sintomas?&lt;/label&gt;&lt;br/&gt;\r\n                                &lt;obs conceptId=\"2eab4e55-d0d0-4fa8-8d23-b40eaaee44c8\" answerConceptIds=\"e1d81b62-1d5f-11e0-b929-000c29ad1d07, e1d81c70-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"Sim, Não\" /&gt;\r\n                            &lt;/p&gt;\r\n\r\n                            &lt;div class=\"base-margin\"&gt;         \r\n                                &lt;p&gt;\r\n                                    &lt;label&gt;Diagnótico TB activo&lt;/label&gt;&lt;br/&gt;\r\n                                    &lt;obs conceptId=\"63b15479-5a05-4bdc-a6e5-eab175743122\" answerConceptIds=\"e1d81b62-1d5f-11e0-b929-000c29ad1d07, e1d81c70-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"Sim, Não\" /&gt;\r\n                                &lt;/p&gt;\r\n        \r\n                                &lt;p class=\"input-size-2\"&gt;\r\n                                    &lt;label&gt;Tratamento TB:&lt;/label&gt;&lt;br/&gt;\r\n                                    &lt;obs conceptId=\"e1d9fbda-1d5f-11e0-b929-000c29ad1d07\" answerConceptIds=\"e1d9ef28-1d5f-11e0-b929-000c29ad1d07, e1d9f036-1d5f-11e0-b929-000c29ad1d07, e1d9facc-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"Início (I), Continua (C), Fim (F)\" dateLabel=\"Data:\"/&gt;\r\n                                &lt;/p&gt;   \r\n                            &lt;/div&gt; \r\n\r\n                        &lt;/div&gt;\r\n                        \r\n                        &lt;div&gt;\r\n                            &lt;label class=\"label-tag\"&gt;Quais sintomas de TB:&lt;/label&gt;\r\n    \r\n                            &lt;div class=\"space-between\"&gt;\r\n    \r\n                                &lt;div&gt;\r\n                                    &lt;p&gt;\r\n                                        &lt;obs conceptId=\"e1de6d1e-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1de6878-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"Febre (F)\"/&gt;&lt;br/&gt;\r\n                                        &lt;obs conceptId=\"e1de6d1e-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1de6a12-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"Emagrecimento (E)\"/&gt;&lt;br/&gt;\r\n                                        &lt;obs conceptId=\"e1de6d1e-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1de66e8-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"Sudorese Noturna (S)\"/&gt;&lt;br/&gt;\r\n                                        &lt;obs conceptId=\"e1de6d1e-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1de63d2-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"Tosse a mais de 2 semanas (T)\"/&gt;\r\n                                    &lt;/p&gt; \r\n                                &lt;/div&gt; \r\n                                \r\n                                &lt;div  class=\"base-margin\"&gt;\r\n                                    &lt;p&gt;\r\n                                        &lt;obs conceptId=\"e1de6d1e-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"44b63d4c-341b-48f0-baa0-ce88ed7afc71\" answerLabel=\"Astenia (A)\"/&gt;&lt;br/&gt;\r\n                                        &lt;obs conceptId=\"e1de6d1e-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1de6b98-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"Contacto com TB (C)\"/&gt;&lt;br/&gt;\r\n                                        &lt;obs conceptId=\"e1de6d1e-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1cfd43e-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"Adenopatia Cervical Indolor\"/&gt;\r\n                                    &lt;/p&gt;   \r\n                                &lt;/div&gt;\r\n    \r\n                            &lt;/div&gt;\r\n                        &lt;/div&gt;\r\n                    &lt;/div&gt;\r\n\r\n                    &lt;div class=\"base-margin\"&gt;\r\n                        &lt;p&gt;\r\n                            &lt;label&gt;Profilaxia (INH):&lt;/label&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"be4a76ca-662a-4c39-903b-71983f5f67c9\" answerConceptIds=\"e1d9ef28-1d5f-11e0-b929-000c29ad1d07, e1d9f036-1d5f-11e0-b929-000c29ad1d07, e1d9facc-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"Início (I), Continua (C), Fim (F)\"/&gt;\r\n                        &lt;/p&gt;\r\n\r\n                        &lt;p&gt;\r\n                            &lt;label&gt;Profilaxia (CTZ):&lt;/label&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"2616b3c9-9a99-4b9a-b673-10871f4a4c71\" answerConceptIds=\"e1d9ef28-1d5f-11e0-b929-000c29ad1d07, e1d9f036-1d5f-11e0-b929-000c29ad1d07, e1d9facc-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"Início (I), Continua (C), Fim (F)\"/&gt;\r\n                        &lt;/p&gt;   \r\n                    &lt;/div&gt;\r\n\r\n                    &lt;div  class=\"base-margin\"&gt;\r\n                        &lt;p&gt;\r\n                            &lt;label&gt;Efeitos Secundários (INH):&lt;/label&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"01ce78dd-074b-407c-ba30-27ec9336e0f8\" answerConceptIds=\"e1d81b62-1d5f-11e0-b929-000c29ad1d07, e1d81c70-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"Sim, Não\"/&gt;\r\n                        &lt;/p&gt;\r\n\r\n                        &lt;p&gt;\r\n                            &lt;label&gt;Efeitos Secundários (CTZ):&lt;/label&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"689cd895-eb45-4712-9b41-8756bc0514ed\" answerConceptIds=\"e1d81b62-1d5f-11e0-b929-000c29ad1d07, e1d81c70-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"Sim, Não\"/&gt;\r\n                        &lt;/p&gt;   \r\n                    &lt;/div&gt;\r\n\r\n                    &lt;div class=\"line-break\"&gt;&lt;/div&gt;\r\n\r\n                    &lt;div class=\"base-margin\"&gt;\r\n                        &lt;label class=\"label-tag\"&gt;ITS&lt;/label&gt;                    \r\n                        &lt;p&gt;\r\n                            &lt;label&gt;Tem sintomas?&lt;/label&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"794ef662-03bc-4e22-90ff-38742b82827a\" answerConceptIds=\"e1d81b62-1d5f-11e0-b929-000c29ad1d07, e1d81c70-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"Sim, Não\" /&gt;\r\n                        &lt;/p&gt;\r\n                        \r\n                        &lt;label class=\"label-tag\"&gt;Diagnóstico ITS:&lt;/label&gt;\r\n                        &lt;p&gt;\r\n                            &lt;obs conceptId=\"e1cfe1e0-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1d01584-1d5f-11e0-b929-000c29ad1d07\"  answerLabel=\"Sifilis (SIF)\"/&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"e1cfe1e0-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1eb356c-1d5f-11e0-b929-000c29ad1d07\"  answerLabel=\"Corrimento Vaginal (CV)\"/&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"e1cfe1e0-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1eb3792-1d5f-11e0-b929-000c29ad1d07\"  answerLabel=\"Corrimento Uretral (CUM)\"/&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"e1cfe1e0-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1d62cee-1d5f-11e0-b929-000c29ad1d07\"  answerLabel=\"Úlcera Genital (UG)\"/&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"e1cfe1e0-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1d689d2-1d5f-11e0-b929-000c29ad1d07\"  answerLabel=\"Dor no Baixo Ventre (DIP)\"/&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"e1cfe1e0-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"29c0b8c9-9086-11e6-a98e-000c29db4475\"  answerLabel=\"Escroto Inchado (ESI)\"/&gt;&lt;br/&gt;\r\n                            &lt;obs conceptId=\"e1cfe1e0-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"99fd3825-9082-11e6-a98e-000c29db4475\"  answerLabel=\"Bubão Inguinal (BI)\"/&gt;\r\n                        &lt;/p&gt;   \r\n                    &lt;/div&gt;\r\n\r\n                    &lt;div class=\"base-margin\"&gt;\r\n                        &lt;label class=\"label-tag\"&gt;Infecções oportunistas &lt;br/&gt; incluindo Sarcoma de &lt;br/&gt; Kaposi e outras doenças:&lt;/label&gt;           \r\n                        &lt;p&gt;\r\n                            &lt;obs conceptId=\"e1dae234-1d5f-11e0-b929-000c29ad1d07\" answerConceptIds=\"e1cda114-1d5f-11e0-b929-000c29ad1d07, \r\n                                                                                                    e1cff5d6-1d5f-11e0-b929-000c29ad1d07, \r\n                                                                                                    e1e529a6-1d5f-11e0-b929-000c29ad1d07, \r\n                                                                                                    e1e5232a-1d5f-11e0-b929-000c29ad1d07, \r\n                                                                                                    e1cf4e24-1d5f-11e0-b929-000c29ad1d07, \r\n                                                                                                    c3e82fe4-9086-11e6-a98e-000c29db4475, \r\n                                                                                                    e1e2530c-1d5f-11e0-b929-000c29ad1d07, \r\n                                                                                                    a8bc94b7-9082-11e6-a98e-000c29db4475, \r\n                                                                                                    c03d9343-9082-11e6-a98e-000c29db4475, \r\n                                                                                                    e1cfcdea-1d5f-11e0-b929-000c29ad1d07, \r\n                                                                                                    a02a1759-9082-11e6-a98e-000c29db4475, \r\n                                                                                                    e1eafbce-1d5f-11e0-b929-000c29ad1d07,\r\n                                                                                                    e1cffa18-1d5f-11e0-b929-000c29ad1d07,\r\n                                                                                                    e1cf5590-1d5f-11e0-b929-000c29ad1d07,\r\n                                                                                                    e1e52f28-1d5f-11e0-b929-000c29ad1d07,\r\n                                                                                                    e1d608cc-1d5f-11e0-b929-000c29ad1d07,\r\n                                                                                                    e1d69314-1d5f-11e0-b929-000c29ad1d07,\r\n                                                                                                    e1cf405a-1d5f-11e0-b929-000c29ad1d07,\r\n                                                                                                    e1cde53e-1d5f-11e0-b929-000c29ad1d07,\r\n                                                                                                    e1cdea3e-1d5f-11e0-b929-000c29ad1d07,\r\n                                                                                                    e1d90dce-1d5f-11e0-b929-000c29ad1d07, \r\n                                                                                                    e1d0103e-1d5f-11e0-b929-000c29ad1d07,\r\n                                                                                                    e1cdd490-1d5f-11e0-b929-000c29ad1d07,\r\n                                                                                                    e1d6412a-1d5f-11e0-b929-000c29ad1d07,\r\n                                                                                                    e1d2984a-1d5f-11e0-b929-000c29ad1d07,\r\n                                                                                                    61a93abd-9087-11e6-a98e-000c29db4475,\r\n                                                                                                    e1d01476-1d5f-11e0-b929-000c29ad1d07,\r\n                                                                                                    e1d607b4-1d5f-11e0-b929-000c29ad1d07,\r\n                                                                                                    de8f1eeb-9082-11e6-a98e-000c29db4475,\r\n                                                                                                    e1e2b07c-1d5f-11e0-b929-000c29ad1d07,\r\n                                                                                                    e1cdd38c-1d5f-11e0-b929-000c29ad1d07,\r\n                                                                                                    e1d657c8-1d5f-11e0-b929-000c29ad1d07,\r\ne1dc8ac6-1d5f-11e0-b929-000c29ad1d07\" \r\n\r\n                                                                                answerLabels=\"Anemia, \r\n                                                                                            Broncopneumonia, \r\n                                                                                            Candidiase esofágica, \r\n                                                                                            Candidiase Oral, \r\n                                                                                            Dermatite, \r\n                                                                                            Diabetes Mellitus, \r\n                                                                                            Diarreia crónica, \r\n                                                                                            Encefalite, \r\n                                                                                            Encefalopatia por HIV, \r\n                                                                                            Epilepsia, \r\n                                                                                            Estomatite, \r\n                                                                                            Febre Inexplicada,\r\n                                                                                            Gastroenterite aguda (GEA),\r\n                                                                                            Gengivite,\r\n                                                                                            Hérpes Simples,\r\n                                                                                            Hérpes Zoster,\r\n                                                                                            Hipertensão Arterial (HTA),\r\n                                                                                            Infecção das Vias Respiratórias Superiores (IVRS),\r\n                                                                                            Infecção Urinária,\r\n                                                                                            Meningite,\r\n                                                                      </t>
   </si>
   <si>
     <t>1d10830e-0742-48c9-a982-b2aa39471926</t>
@@ -1443,6 +1439,18 @@
   <si>
     <t>51f31664-8ea1-457a-b573-927555565430</t>
   </si>
+  <si>
+    <t>&lt;htmlform id=\"PrepInitial\"&gt;\r\n\r\n  &lt;html xmlns=\"http://www.w3.org/1999/xhtml\"&gt;\r\n\r\n  &lt;head&gt;\r\n    &lt;meta http-equiv=\"Content-Type\" content=\"text/html; charset=utf-8\" /&gt;\r\n    &lt;title&gt;Registo de Proflaxia Pré-Exposaição(PrEP)&lt;/title&gt;\r\n\r\n    &lt;style&gt;\r\n      h2 {\r\n        border-bottom: 3px solid red;\r\n      }\r\n\r\n      p {\r\n        border: 1px solid black;\r\n      }\r\n\r\n      table {\r\n        border-color: #600;\r\n        border-width: 0 0 1px 1px;\r\n        border-style: solid;\r\n      }\r\n\r\n      td {\r\n        border-color: #600;\r\n        border-width: 1px 1px 0 0;\r\n        border-style: solid;\r\n        margin: 0;\r\n        padding: 4px;\r\n        background-color: #B2DFEE;\r\n      }\r\n\r\n      .style1 {\r\n        font-size: 14px;\r\n        font-weight: bold;\r\n      }\r\n\r\n      .section {\r\n        border: 1px solid $headerColor;\r\n        padding: 2px;\r\n        text-align: center;\r\n        margin-bottom: 1em;\r\n        border-width: thin;\r\n        width: 50%;\r\n        vertical-align: middle;\r\n        azimuth: center;\r\n      }\r\n\r\n      .sectionHeader {\r\n        background-color: $headerColor;\r\n        color: $fontOnHeaderColor;\r\n        display: block;\r\n        padding: 2px;\r\n        font-weight: bold;\r\n      }\r\n\r\n      .input-with-size input[type=\"text\"] {\r\n        width: 50px !important;\r\n      }\r\n\r\n      table.baseline-aligned td {\r\n        vertical-align: baseline;\r\n      }\r\n    &lt;/style&gt;\r\n    &lt;script type=\"text/javascript\"&gt;\r\n      $j(document).ready(function () {\r\n        var nidPrep = \"&lt;lookup expression=\"patient.getPatientIdentifier(17)\"/&gt;\";\r\n\r\n        if (nidPrep == null | nidPrep.length === 0) {\r\n          window.alert(\'Para registar este formulário o paciente deve ser registado como paciente PREP\');\r\n          $j(\"#PrepInitial input, #PrepInitial select\").attr(\'disabled\', true);\r\n            return false;\r\n        }\r\n\r\n        var estadoProgramaPREP = parseInt(\"&lt;lookup expression=\"fn.currentProgramWorkflowStatus(50).state.concept.id\" /&gt;\")\r\n        if (isNaN(estadoProgramaPREP)) {\r\n          window.alert(\'Para registar este formulário o paciente deve ser admitido no programa PREP!\');\r\n          $j(\"#PrepInitial input, #PrepInitial select\").attr(\'disabled\', true);\r\n            return false;\r\n        } else {\r\n          if (!((estadoProgramaPREP == 6269) || (estadoProgramaPREP == 1369))) {\r\n            window.alert(\'Este paciente não está no estado activo no programa PREP, coloque-o como activo primeiro!\');\r\n            $j(\"#PrepInitial input, #PrepInitial select\").attr(\'disabled\', true);\r\n              return false;\r\n          }\r\n        }\r\n\r\n        var nrFrascosMedPrep = $j(\"#outro-med-prep-frascos input\");\r\n        nrFrascosMedPrep.attr(\'disabled\', true);\r\n        $j(\'#outro-med-prep input[type=checkbox]\').live(\'change\', function () {\r\n          var outroMedPrep = $j(this);\r\n          if (outroMedPrep.attr(\'checked\') === \'checked\') {\r\n            nrFrascosMedPrep.attr(\'disabled\', false);\r\n          }\r\n          else {\r\n            nrFrascosMedPrep.attr(\'disabled\', true);\r\n            nrFrascosMedPrep.attr(\'value\', \'\');\r\n\r\n          }\r\n        });\r\n\r\n      });\r\n\r\n\r\n    &lt;/script&gt;\r\n\r\n  &lt;/head&gt;\r\n\r\n  &lt;body&gt;\r\n    &lt;table width=\"900\" border=\"0\" align=\"center\" style=\"background-color:white; border: none;\"&gt;\r\n      &lt;tbody align=\"right\" style=\"font-family:verdana; font-size:12px\"&gt;\r\n\r\n        &lt;tr&gt;\r\n          &lt;td colspan=\"3\" style=\"background-color:white; border:none; text-align: center;\"&gt;\r\n            &lt;p style=\"border:none; font-size:18px; font-weight:bold;\"&gt;Registo de Proflaxia Pré-Exposição(PrEP)&lt;/p&gt;\r\n          &lt;/td&gt;\r\n        &lt;/tr&gt;\r\n\r\n        &lt;tr&gt;\r\n          &lt;td style=\"background-color:white; border: none;\"&gt;&lt;/td&gt;\r\n          &lt;td style=\"background-color:white; border: none;\"&gt;\r\n            &lt;table width=\"300\" border=\"1\"&gt;\r\n              &lt;tbody align=\"left\" style=\"font-family:verdana; font-size:12px\"&gt;\r\n                &lt;tr&gt;\r\n                  &lt;td&gt;NID PREP&lt;br /&gt;\r\n                    &lt;lookup expression=\"patient.getPatientIdentifier(17)\" /&gt;\r\n                  &lt;/td&gt;\r\n                &lt;/tr&gt;\r\n              &lt;/tbody&gt;\r\n            &lt;/table&gt;\r\n          &lt;/td&gt;\r\n        &lt;/tr&gt;\r\n\r\n      &lt;/tbody&gt;\r\n    &lt;/table&gt;\r\n\r\n    &lt;table width=\"900\" border=\"1\" align=\"center\"&gt;\r\n      &lt;tbody align=\"left\" style=\"font-family:verdana; font-size:12px\"&gt;\r\n\r\n        &lt;tr&gt;\r\n          &lt;th colspan=\"3\"&gt;\r\n            &lt;div style=\"background-color: black; color: white; text-align: left;\"&gt;A. Informação sobre a Instituição\r\n            &lt;/div&gt;\r\n          &lt;/th&gt;\r\n        &lt;/tr&gt;\r\n        &lt;tr&gt;\r\n          &lt;td&gt;US:\r\n            &lt;encounterLocation id=\"localConsulta\" default=\"GlobalProperty:default_location\"  type=\"autocomplete\" /&gt;\r\n          &lt;/td&gt;\r\n          &lt;td&gt;Distrito/Cidade:\r\n            &lt;lookup complexExpression=\"#foreach( $addr in $patient.addresses ) $!addr.countyDistrict #end\"/&gt;\r\n          &lt;/td&gt;\r\n          &lt;td&gt;Sector:\r\n            &lt;obs conceptId=\"beb9f5d1-3365-4574-894e-445b82a81087\" answerConceptIds=\"e1daea2c-1d5f-11e0-b929-000c29ad1d07,\r\n        e1e05bc4-1d5f-11e0-b929-000c29ad1d07,\r\n        e1e0599e-1d5f-11e0-b929-000c29ad1d07,\r\n        e1dee38e-1d5f-11e0-b929-000c29ad1d07,\r\n        d6b884fc-c799-4c23-844a-5eb1c470ab62\" answerLabels=\"PNCT,GATV/SAAJ,GATV/PTV/CPN,CCR,CLINICA\" /&gt;\r\n          &lt;/td&gt;\r\n        &lt;/tr&gt;\r\n\r\n\r\n        &lt;tr&gt;\r\n          &lt;td&gt;Data da visita inicial do Utente (dd/mm/aaaa):\r\n            &lt;encounterDate id=\"dataConsulta\" /&gt;\r\n          &lt;/td&gt;\r\n          &lt;td colspan=\"2\"&gt;Provedor que preencheu o formulário:\r\n            &lt;encounterProvider role=\"Provider\" type=\"autocomplete\" /&gt;\r\n          &lt;/td&gt;\r\n        &lt;/tr&gt;\r\n\r\n      &lt;/tbody&gt;\r\n    &lt;/table&gt;\r\n    &lt;table width=\"900\" border=\"1\" align=\"center\"&gt;\r\n      &lt;tbody align=\"left\" style=\"font-family:verdana; font-size:12px\"&gt;\r\n\r\n        &lt;tr&gt;\r\n          &lt;th colspan=\"2\"&gt;\r\n            &lt;div style=\"background-color: black; color: white; text-align: left;\"&gt;B. Dados Demográficos&lt;/div&gt;\r\n          &lt;/th&gt;\r\n        &lt;/tr&gt;\r\n        &lt;tr&gt;\r\n          &lt;td colspan=\"2\"&gt;Nome do Utente:\r\n            &lt;lookup expression=\"patient.personName\" /&gt;\r\n          &lt;/td&gt;\r\n        &lt;/tr&gt;\r\n        &lt;tr&gt;\r\n          &lt;td&gt;\r\n            Endereço:\r\n            &lt;lookup complexExpression=\"#foreach( $addr in $patient.addresses ) $!addr.subregion #end\" /&gt;\r\n          &lt;/td&gt;\r\n          &lt;td&gt;\r\n            Telefone:\r\n            &lt;lookup expression=\"patient.getAttribute(9)\" /&gt;\r\n          &lt;/td&gt;\r\n        &lt;/tr&gt;\r\n        &lt;tr&gt;\r\n          &lt;td colspan=\"2\"&gt;Data de Nascimento:\r\n            &lt;lookup expression=\"patient.birthdate\" /&gt; Idade:\r\n            &lt;lookup expression=\"patient.age\" /&gt; Sexo:\r\n            &lt;lookup expression=\"patient.gender\" /&gt;\r\n          &lt;/td&gt;\r\n        &lt;/tr&gt;\r\n\r\n        &lt;tr&gt;\r\n          &lt;td&gt;Data do teste inicial de HIV:\r\n            &lt;obs id=\"dataDeTesteInicial\" conceptId=\"38575125-4aff-4894-be3d-7baac37e9ab5\" labelText=\"\"\r\n              allowFutureDates=\"false\" /&gt;\r\n          &lt;/td&gt;\r\n          &lt;td&gt;Estado Civil do Utente:\r\n            &lt;obs conceptId=\"e1d80fbe-1d5f-11e0-b929-000c29ad1d07\" style=\"radio\" answerConceptIds=\"\r\n      e1d812e8-1d5f-11e0-b929-000c29ad1d07,\r\n      e1e6f1c8-1d5f-11e0-b929-000c29ad1d07,\r\n      e1d813f6-1d5f-11e0-b929-000c29ad1d07,\r\n      e1d81504-1d5f-11e0-b929-000c29ad1d07,\r\n      e1d811da-1d5f-11e0-b929-000c29ad1d07,\r\n      e1d81612-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"Solteiro,Casado,Divorciado,Viúvo,Separado, União de Facto\" /&gt;\r\n          &lt;/td&gt;\r\n        &lt;/tr&gt;\r\n\r\n        &lt;tr&gt;\r\n          &lt;td colspan=\"2\"&gt;Nome do Parceiro:\r\n            &lt;obs conceptId=\"bc39b981-bde2-4486-b1b8-8cef5a3233e3\" labelText=\"\" /&gt;\r\n            NID do Parceiro:\r\n            &lt;obs conceptId=\"e1db0dea-1d5f-11e0-b929-000c29ad1d07\" labelText=\"\" /&gt;&lt;br /&gt;&lt;br /&gt;\r\n            Unidade Sanitária onde o parceiro HIV+ faz seguimento:\r\n            &lt;obs conceptId=\"3049d095-0dec-49e7-ac7b-1dea045adb3b\" labelText=\"\" /&gt;\r\n          &lt;/td&gt;\r\n        &lt;/tr&gt;\r\n        &lt;tr&gt;\r\n          &lt;td&gt; Grupo Alvo&lt;/td&gt;\r\n          &lt;td&gt;Casal Serodiscordante:\r\n            &lt;obs conceptId=\"279a7f80-b3cd-45c2-b16b-4706212416fd\" answerConceptId=\"d5645b60-feb4-4388-8910-77887da0e4ae\"\r\n              labelText=\"\" answerLabel=\"\" /&gt;Parceiro HIV Negativo /\r\n            &lt;obs conceptId=\"279a7f80-b3cd-45c2-b16b-4706212416fd\" answerConceptId=\"bfd6f84c-365c-433b-a54e-b568ee5027be\"\r\n              labelText=\"\" answerLabel=\"\" /&gt;Parceira HIV Negativa;&lt;br /&gt;\r\n            Adolescentes e Jovens:\r\n            &lt;obs conceptId=\"279a7f80-b3cd-45c2-b16b-4706212416fd\" answerConceptId=\"41a6e94f-c4b3-4959-a9e4-e03083900d4d\"\r\n              labelText=\"\" answerLabel=\"\" /&gt;Rapazes 15 - 24 Anos /\r\n            &lt;obs conceptId=\"279a7f80-b3cd-45c2-b16b-4706212416fd\" answerConceptId=\"19857885-f915-4715-b8fa-18203b967a0b\"\r\n              labelText=\"\" answerLabel=\"\" /&gt;Raparigas 15 - 24 Anos;&lt;br /&gt;\r\n            &lt;obs conceptId=\"279a7f80-b3cd-45c2-b16b-4706212416fd\" answerConceptId=\"b197cce5-08b6-4c22-9c92-37b7e3a01b0c\"\r\n              labelText=\"\" answerLabel=\"\" /&gt;Homens 25+ em Risco;&lt;br /&gt;\r\n            &lt;obs conceptId=\"279a7f80-b3cd-45c2-b16b-4706212416fd\" answerConceptId=\"e1e056a6-1d5f-11e0-b929-000c29ad1d07\"\r\n              labelText=\"\" answerLabel=\"\" /&gt;Outra MG em Risco;&lt;br /&gt;\r\n            &lt;obs conceptId=\"279a7f80-b3cd-45c2-b16b-4706212416fd\" answerConceptId=\"bc4fe755-fc8f-49b8-9956-baf2477e8313\"\r\n              labelText=\"\" answerLabel=\"\" /&gt;Outra ML em Risco;&lt;br /&gt;\r\n            &lt;obs conceptId=\"279a7f80-b3cd-45c2-b16b-4706212416fd\" answerConceptId=\"af817b6e-b3aa-44ba-8f1f-9ae8c2e442f9\"\r\n              answerLabel=\"\" commentFieldLabel=\"Outro: \" /&gt;\r\n            População chave:\r\n            &lt;obs conceptId=\"c7c0b430-bbc1-4042-a365-ad78a13aef56\" answerConceptIds=\"\r\n      e1daa454-1d5f-11e0-b929-000c29ad1d07,\r\n      e1df1296-1d5f-11e0-b929-000c29ad1d07,\r\n      5bdb7ec1-908a-11e6-a98e-000c29db4475,\r\n      58021703-908a-11e6-a98e-000c29db4475,\r\n      2b68aa87-2fc2-4c72-8c53-55c3fa265e6d\" labelText=\"\" answerLabels=\"HSH,PID,Recluso,TS,Transgênero\" /&gt;\r\n          &lt;/td&gt;\r\n        &lt;/tr&gt;\r\n\r\n        &lt;tr&gt;\r\n          &lt;td&gt; Proveniência do Utente&lt;/td&gt;\r\n          &lt;td&gt;\r\n            &lt;obs conceptId=\"e1dca2ea-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1e052aa-1d5f-11e0-b929-000c29ad1d07\"\r\n              labelText=\"\" answerLabel=\"\" /&gt;CPN\r\n            &lt;obs conceptId=\"e1dca2ea-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1e05bc4-1d5f-11e0-b929-000c29ad1d07\"\r\n              labelText=\"\" answerLabel=\"\" /&gt;SAAJ\r\n            &lt;obs conceptId=\"e1dca2ea-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"0aeaf088-8bc8-4485-87a5-427e7d138fe0\"\r\n              labelText=\"\" answerLabel=\"\" /&gt;Doenças Crónicas\r\n            &lt;obs conceptId=\"e1dca2ea-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"1b7ff519-1ec3-4b6d-aeae-6f6381b70a62\"\r\n              labelText=\"\" answerLabel=\"\" /&gt;Triagem Adulto\r\n            &lt;obs conceptId=\"e1dca2ea-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1e67fcc-1d5f-11e0-b929-000c29ad1d07\"\r\n              labelText=\"\" answerLabel=\"\" /&gt;CPF\r\n            &lt;obs conceptId=\"e1dca2ea-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1dca5e2-1d5f-11e0-b929-000c29ad1d07\"\r\n              labelText=\"\" answerLabel=\"\" /&gt;UATS\r\n            &lt;obs conceptId=\"e1dca2ea-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"cf6e0b75-d0b4-403a-a886-0c06e1e9ea77\"\r\n              labelText=\"\" answerLabel=\"\" /&gt;ATS-C &lt;br /&gt;\r\n            &lt;obs conceptId=\"e1dca2ea-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1dee38e-1d5f-11e0-b929-000c29ad1d07\"\r\n              labelText=\"\" answerLabel=\"\" /&gt;CCR &lt;br /&gt;\r\n            &lt;obs conceptId=\"e1dca2ea-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1e783ea-1d5f-11e0-b929-000c29ad1d07\"\r\n              answerLabel=\"\" commentFieldLabel=\"Outro(especificar): \" /&gt;\r\n          &lt;/td&gt;\r\n        &lt;/tr&gt;\r\n\r\n      &lt;/tbody&gt;\r\n    &lt;/table&gt;\r\n\r\n\r\n    &lt;table width=\"900\" border=\"1\" align=\"center\"&gt;\r\n      &lt;tbody align=\"left\" style=\"font-family:verdana; font-size:12px\"&gt;\r\n\r\n        &lt;tr&gt;\r\n          &lt;th&gt;\r\n            &lt;div style=\"background-color: black; color: white; text-align: left;\"&gt;C. Gravidez e Lactância\r\n            &lt;/div&gt;\r\n          &lt;/th&gt;\r\n          &lt;th&gt;\r\n            &lt;div style=\"background-color: black; color: white; text-align: left;\"&gt;D. Testes laboratoriais e Sinais\r\n              Vitais&lt;/div&gt;\r\n          &lt;/th&gt;\r\n        &lt;/tr&gt;\r\n\r\n        &lt;tr&gt;\r\n          &lt;td&gt;\r\n            &lt;obs conceptId=\"e1e056a6-1d5f-11e0-b929-000c29ad1d07\"\r\n              answerConceptIds=\"e1cdd58a-1d5f-11e0-b929-000c29ad1d07,e1d81c70-1d5f-11e0-b929-000c29ad1d07\"\r\n              labelText=\"Utente actualmente grávida?\" answerLabels=\"Sim,Não\" style=\"radio\" /&gt;&lt;br /&gt;\r\n            &lt;obs conceptId=\"bc4fe755-fc8f-49b8-9956-baf2477e8313\"\r\n              answerConceptIds=\"e1d81b62-1d5f-11e0-b929-000c29ad1d07,e1d81c70-1d5f-11e0-b929-000c29ad1d07\"\r\n              labelText=\"Utente actualmente amamentando?\" answerLabels=\"Sim,Não\" style=\"radio\" /&gt;\r\n          &lt;/td&gt;\r\n          &lt;td&gt;\r\n            Creatinina\r\n            &lt;obs conceptId=\"e1d5d21c-1d5f-11e0-b929-000c29ad1d07\" labelText=\"\" dateLabel=\" | Data:\" /&gt;&lt;br /&gt;&lt;br /&gt;\r\n            Tensão Arterial: Sistolica\r\n            &lt;obs conceptId=\"e1e2e3d0-1d5f-11e0-b929-000c29ad1d07\" labelText=\"\" /&gt;\r\n            Diastolica\r\n            &lt;obs conceptId=\"e1e2e4e8-1d5f-11e0-b929-000c29ad1d07\" labelText=\"\" dateLabel=\" | Data:\" /&gt;\r\n          &lt;/td&gt;\r\n        &lt;/tr&gt;\r\n\r\n      &lt;/tbody&gt;\r\n    &lt;/table&gt;\r\n\r\n    &lt;table width=\"900\" border=\"1\" align=\"center\"&gt;\r\n      &lt;tbody align=\"left\" style=\"font-family:verdana; font-size:12px\"&gt;\r\n\r\n        &lt;tr&gt;\r\n          &lt;th colspan=\"2\"&gt;\r\n            &lt;div style=\"background-color: black; color: white; text-align: left;\"&gt;E. Exame de Hepatite B e Tratamento\r\n            &lt;/div&gt;\r\n          &lt;/th&gt;\r\n        &lt;/tr&gt;\r\n\r\n        &lt;tr&gt;\r\n          &lt;td&gt;Teste de HBsAg\r\n          &lt;/td&gt;\r\n          &lt;td&gt;\r\n            &lt;obs conceptId=\"e1da3e7e-1d5f-11e0-b929-000c29ad1d07\"\r\n              answerConceptIds=\"e1d446cc-1d5f-11e0-b929-000c29ad1d07,e1d47386-1d5f-11e0-b929-000c29ad1d07,e1d85e2e-1d5f-11e0-b929-000c29ad1d07\"\r\n              labelText=\"Resultado do teste\" answerLabels=\"Negativo,Positivo,Não realizado\" style=\"radio\"\r\n              dateLabel=\"| Data:\" /&gt;\r\n          &lt;/td&gt;\r\n        &lt;/tr&gt;\r\n\r\n        &lt;tr&gt;\r\n          &lt;td colspan=\"2\"&gt;\r\n            &lt;obs conceptId=\"7bd44a2f-29ac-40dc-838f-7536445c6075\"\r\n              answerConceptIds=\"e1cdd58a-1d5f-11e0-b929-000c29ad1d07,e1d81c70-1d5f-11e0-b929-000c29ad1d07,e1d81d7e-1d5f-11e0-b929-000c29ad1d07\"\r\n              labelText=\"Se positivo é utente em tratamento\" answerLabels=\"Sim,Não,Desconhecido\" style=\"radio\" /&gt;\r\n          &lt;/td&gt;\r\n        &lt;/tr&gt;\r\n\r\n      &lt;/tbody&gt;\r\n    &lt;/table&gt;\r\n\r\n\r\n    &lt;table width=\"900\" border=\"1\" align=\"center\"&gt;\r\n      &lt;tbody align=\"left\" style=\"font-family:verdana; font-size:12px\"&gt;\r\n\r\n        &lt;tr&gt;\r\n          &lt;th colspan=\"2\"&gt;\r\n            &lt;div style=\"background-color: black; color: white; text-align: left;\"&gt;F. Infecções sexualmente\r\n              Transmissíveis (ITS)\r\n            &lt;/div&gt;\r\n          &lt;/th&gt;\r\n        &lt;/tr&gt;\r\n\r\n        &lt;tr&gt;\r\n          &lt;td colspan=\"2\"&gt;\r\n            Teste de VDRL/Sífilis\r\n            &lt;obs conceptId=\"e1d14ce2-1d5f-11e0-b929-000c29ad1d07\"\r\n              answerConceptIds=\"e1d446cc-1d5f-11e0-b929-000c29ad1d07,e1d47386-1d5f-11e0-b929-000c29ad1d07,e1d85e2e-1d5f-11e0-b929-000c29ad1d07\"\r\n              labelText=\"Resultado:\" answerLabels=\"Negativo,Positivo,Não Realizado\" style=\"radio\" dateLabel=\"| Data:\" /&gt;\r\n            &lt;br /&gt;&lt;br /&gt;\r\n            Rastreio de ITS: Sinais e sintomas de ITS\r\n            &lt;obs conceptId=\"794ef662-03bc-4e22-90ff-38742b82827a\" dateLabel=\"| Data:\"\r\n              answerConceptIds=\"e1cdd58a-1d5f-11e0-b929-000c29ad1d07,e1d81c70-1d5f-11e0-b929-000c29ad1d07\"\r\n              answerLabels=\"Sim,Não\" style=\"radio\" /&gt;&lt;br /&gt; &lt;br /&gt;\r\n            Diagnóstico de ITS(seleccionar todos que se apliquem)\r\n            &lt;obs conceptId=\"e1d835ca-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1eb3792-1d5f-11e0-b929-000c29ad1d07\"\r\n              labelText=\"\" answerLabel=\"CUM = Corrimento Uretral\" /&gt;\r\n            &lt;obs conceptId=\"e1d835ca-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1d62cee-1d5f-11e0-b929-000c29ad1d07\"\r\n              labelText=\"\" answerLabel=\"UG = Úlceras Genitais\" /&gt;\r\n            &lt;obs conceptId=\"e1d835ca-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"99fd3825-9082-11e6-a98e-000c29db4475\"\r\n              labelText=\"\" answerLabel=\"BI = Bubo Inguinal\" /&gt;&lt;br /&gt;\r\n            &lt;obs conceptId=\"e1d835ca-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1eb356c-1d5f-11e0-b929-000c29ad1d07\"\r\n              labelText=\"\" answerLabel=\"CV = Corrimento Vaginal\" /&gt;\r\n            &lt;obs conceptId=\"e1d835ca-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"e1d689d2-1d5f-11e0-b929-000c29ad1d07\"\r\n              labelText=\"\" answerLabel=\"DIP = Dor no baixo ventre\" /&gt;\r\n            &lt;obs conceptId=\"e1d835ca-1d5f-11e0-b929-000c29ad1d07\" answerConceptId=\"29c0b8c9-9086-11e6-a98e-000c29db4475\"\r\n              labelText=\"\" answerLabel=\"ESI = Inchaço Escrotal\" /&gt;\r\n            &lt;obs conceptId=\"e1d835ca-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"\"\r\n              commentFieldLabel=\"O = Outros(especifique): \" answerConceptId=\"246fcc9d-3dd8-4a42-99d5-048c4176bd43\" /&gt;\r\n            &lt;br /&gt;&lt;br /&gt;\r\n            Em caso de diagnóstico de ITS, início do tratamento (dd/mm/aa):\r\n            &lt;obs id=\"dataInicioTratITS\" conceptId=\"a07cc91f-1b83-46da-a63b-d39ebe22b14a\" labelText=\"\"\r\n              allowFutureDates=\"false\" /&gt;\r\n          &lt;/td&gt;\r\n\r\n        &lt;/tr&gt;\r\n\r\n      &lt;/tbody&gt;\r\n    &lt;/table&gt;\r\n\r\n\r\n    &lt;table width=\"900\" border=\"1\" align=\"center\"&gt;\r\n      &lt;tbody align=\"left\" style=\"font-family:verdana; font-size:12px\"&gt;\r\n\r\n        &lt;tr&gt;\r\n          &lt;th colspan=\"2\"&gt;\r\n            &lt;div style=\"background-color: black; color: white; text-align: left;\"&gt;G. Início ou Reinício da\r\n              PrEP\r\n            &lt;/div&gt;\r\n          &lt;/th&gt;\r\n        &lt;/tr&gt;\r\n\r\n        &lt;tr&gt;\r\n          &lt;td&gt;Se o utente está a iniciar a PrEP pela 1a vez\r\n          &lt;/td&gt;\r\n          &lt;td&gt;\r\n            Data de início PrEP (dd/mm/aa):\r\n            &lt;obs id=\"dataInicioPrep\" conceptId=\"d835e77a-10c6-40e7-b4f6-2b1d93fbac2a\" labelText=\"\"\r\n              allowFutureDates=\"true\" /&gt;\r\n          &lt;/td&gt;\r\n        &lt;/tr&gt;\r\n        &lt;tr&gt;\r\n          &lt;td&gt;Se o utente está a Reiniciar a PrEP\r\n          &lt;/td&gt;\r\n          &lt;td&gt;\r\n            Data de reinício PrEP (dd/mm/aa):\r\n            &lt;obs id=\"dataInicioPrep\" conceptId=\"f240cc3c-0a4e-4d0f-9170-b1cc9c7adf12\" labelText=\"\"\r\n              allowFutureDates=\"true\" /&gt;\r\n          &lt;/td&gt;\r\n        &lt;/tr&gt;\r\n\r\n        &lt;tr&gt;\r\n          &lt;td&gt;Regime da PrEP prescrita (ARVs)\r\n          &lt;/td&gt;\r\n          &lt;td&gt;\r\n            &lt;obs conceptId=\"0bfae0d8-e2aa-48e4-b4a4-c157021b4f15\" answerLabel=\"\"\r\n              commentFieldLabel=\"TDF/3TC - N° de frascos: \" answerConceptId=\"8c8d5c95-bd54-4fe9-a544-30277396e903\"\r\n              class=\"input-with-size\" /&gt;&lt;br /&gt;\r\n            &lt;obs conceptId=\"0bfae0d8-e2aa-48e4-b4a4-c157021b4f15\" answerLabel=\"\"\r\n              commentFieldLabel=\"TDF/FTC - N° de frascos: \" answerConceptId=\"17247380-ec48-46b3-8159-5ee50c84129a\"\r\n              class=\"input-with-size\" /&gt;&lt;br /&gt;\r\n            &lt;obs conceptId=\"0bfae0d8-e2aa-48e4-b4a4-c157021b4f15\" answerLabel=\"\"\r\n              commentFieldLabel=\"Outro(especifique): \" answerConceptId=\"37789777-a352-472c-be11-13f661d4a94c\"\r\n              id=\"outro-med-prep\" /&gt;\r\n            &lt;obs conceptId=\"18d4175b-df7c-4659-a266-38e9ff60278e\" labelText=\"N° de frascos:\"\r\n              id=\"outro-med-prep-frascos\" /&gt;\r\n          &lt;/td&gt;\r\n        &lt;/tr&gt;\r\n\r\n        &lt;tr&gt;\r\n          &lt;td colspan=\"2\"&gt;\r\n            &lt;div align=\"center\"&gt;\r\n              &lt;submit submitLabel=\"Submeter\" /&gt;\r\n            &lt;/div&gt;\r\n          &lt;/td&gt;\r\n        &lt;/tr&gt;\r\n\r\n      &lt;/tbody&gt;\r\n    &lt;/table&gt;\r\n\r\n  &lt;/body&gt;\r\n\r\n  &lt;/html&gt;\r\n&lt;/htmlform&gt;</t>
+  </si>
+  <si>
+    <t>dede8b78-9e1d-497a-ad75-030d5bd140e4</t>
+  </si>
+  <si>
+    <t>&lt;htmlform id = \"PrepInitial\"&gt;\r\n  &lt;script type=\"text/javascript\"&gt;\r\n  &lt;/script&gt;\r\n  &lt;html xmlns=\"http://www.w3.org/1999/xhtml\"&gt;\r\n  &lt;head&gt;\r\n  &lt;meta http-equiv=\"Content-Type\" content=\"text/html; charset=utf-8\" /&gt;\r\n  &lt;title&gt;Registo de Consulta de Seguimento Pré-Exposição(PrEP)&lt;/title&gt;\r\n    &lt;style&gt;\r\n       h2 { border-bottom: 3px solid red; }\r\n        p { border: 1px solid black; }\r\n        table{\r\n          border-color: #600;\r\n         border-width: 0 0 1px 1px;\r\n          border-style: solid;}\r\n       td{\r\n         border-color: #600;\r\n         border-width: 1px 1px 0 0;\r\n          border-style: solid;\r\n          margin: 0;\r\n          padding: 4px;\r\n         background-color: #B2DFEE;}\r\n       .style1 {\r\n         font-size: 14px;\r\n          font-weight: bold;}\r\n       .section {\r\n          border: 1px solid $headerColor;\r\n         padding: 2px;\r\n         text-align: center;\r\n         margin-bottom: 1em;\r\n         border-width:thin;\r\n          width:50%;\r\n          vertical-align:middle;\r\n          azimuth:center;}\r\n        .sectionHeader {\r\n          background-color: $headerColor;\r\n         color: $fontOnHeaderColor;\r\n          display: block;\r\n         padding: 2px;\r\n         font-weight: bold;}\r\n       table.baseline-aligned td {\r\n         vertical-align: baseline;}\r\n    &lt;/style&gt;\r\n    &lt;script type=\"text/javascript\"&gt;\r\n      $j(document).ready(function() {\r\n        var nidPrep = \"&lt;lookup expression=\"patient.getPatientIdentifier(17)\"/&gt;\";\r\n \r\n        if(nidPrep == null | nidPrep.length === 0){\r\n          window.alert(\'Para registar este formulário o paciente deve ser registado como paciente PREP\');\r\n          $j(\"#PrepInitial input, #PrepInitial select\").attr(\'disabled\',true);\r\n         return false;\r\n        }\r\n\r\n        var estadoProgramaPREP = parseInt(\"&lt;lookup expression=\"fn.currentProgramWorkflowStatus(50).state.concept.id\" /&gt;\");\r\n        if (isNaN(estadoProgramaPREP)) {\r\n          window.alert(\'Para registar este formulário o paciente deve ser admitido no programa PREP!\');\r\n          $j(\"#PrepInitial input, #PrepInitial select\").attr(\'disabled\', true);\r\n             return false;\r\n        } else {\r\n          if (!((estadoProgramaPREP == 6269) || (estadoProgramaPREP == 1369))) {\r\n            window.alert(\'Este paciente não está no estado activo no programa PREP, coloque-o como activo primeiro!\');\r\n            $j(\"#PrepInitial input, #PrepInitial select\").attr(\'disabled\', true);\r\n                return false;\r\n          }\r\n        }\r\n\r\n        var gender = \"&lt;lookup expression=\"patient.gender\" /&gt;\";\r\n\r\n        if(gender ===\'F\'){\r\n          $j(\'.estadoDaMulher\').show();\r\n        }else{\r\n          $j(\'.estadoDaMulher\').hide();\r\n        }\r\n\r\n      });\r\n    &lt;/script&gt;\r\n  &lt;/head&gt;\r\n  &lt;body&gt;\r\n  &lt;table width=\"900\" border=\"0\" align=\"center\" style=\"background-color:white; border: none;\"&gt;\r\n    &lt;tbody align=\"right\" style=\"font-family:verdana; font-size:12px\"&gt;\r\n      &lt;tr&gt;\r\n        &lt;td colspan=\"3\" style=\"background-color:white; border:none; text-align: center;\"&gt;\r\n          &lt;p style=\"border:none; font-size:18px; font-weight:bold;\"&gt;Consulta de Seguimento Pré-Exposição(PrEP)&lt;/p&gt;\r\n        &lt;/td&gt;\r\n      &lt;/tr&gt; \r\n    &lt;/tbody&gt;\r\n  &lt;/table&gt;\r\n  &lt;table width=\"900\" border=\"1\" align=\"center\"&gt;\r\n  &lt;tbody align=\"left\" style=\"font-family:verdana; font-size:12px\"&gt;\r\n  &lt;tr&gt;\r\n     &lt;td&gt;&lt;div align=\"right\"&gt;NOME DO PROVEDOR:&lt;/div&gt;&lt;/td&gt;\r\n      &lt;td colspan=\"2\"&gt;&lt;encounterProvider role=\"Provider\"/&gt;&lt;/td&gt;\r\n  &lt;/tr&gt;\r\n  &lt;tr&gt;\r\n      &lt;td&gt;&lt;div align=\"right\"&gt;UNIDADE SANITARIA:&lt;/div&gt;&lt;/td&gt;\r\n      &lt;td colspan=\"2\"&gt;&lt;encounterLocation id=\"localConsulta\" default=\"GlobalProperty:default_location\"  type=\"autocomplete\" /&gt;&lt;/td&gt;\r\n       &lt;/tr&gt;\r\n   &lt;tr&gt;\r\n      &lt;td&gt;&lt;div align=\"right\"&gt;Data da consulta (dd/mm/aa)&lt;/div&gt;&lt;/td&gt;\r\n      &lt;td colspan=\"2\"&gt;&lt;encounterDate id=\"dataConsulta\"/&gt;&lt;/td&gt;\r\n   &lt;/tr&gt;\r\n   &lt;tr&gt;\r\n    &lt;td&gt;&lt;div align=\"right\"&gt;População chave&lt;/div&gt;&lt;/td&gt;\r\n    &lt;td colspan=\"2\"&gt;&lt;obs conceptId=\"c7c0b430-bbc1-4042-a365-ad78a13aef56\" answerConceptId=\"e1daa454-1d5f-11e0-b929-000c29ad1d07\" labelText=\"\" answerLabel=\"HSH\" /&gt;\r\n      &lt;obs conceptId=\"c7c0b430-bbc1-4042-a365-ad78a13aef56\" answerConceptId=\"e1df1296-1d5f-11e0-b929-000c29ad1d07\" labelText=\"\" answerLabel=\"TS\" /&gt;\r\n      &lt;obs conceptId=\"c7c0b430-bbc1-4042-a365-ad78a13aef56\" answerConceptId=\"5bdb7ec1-908a-11e6-a98e-000c29db4475\" labelText=\"\" answerLabel=\"PID\" /&gt;\r\n      &lt;obs conceptId=\"c7c0b430-bbc1-4042-a365-ad78a13aef56\" answerConceptId=\"58021703-908a-11e6-a98e-000c29db4475\" labelText=\"\" answerLabel=\"REC\" /&gt;\r\n      &lt;obs conceptId=\"c7c0b430-bbc1-4042-a365-ad78a13aef56\" answerConceptId=\"2b68aa87-2fc2-4c72-8c53-55c3fa265e6d\" labelText=\"\" answerLabel=\"TG\" /&gt;&lt;/td&gt;\r\n &lt;/tr&gt;\r\n   &lt;tr&gt;\r\n    &lt;td&gt;&lt;div align=\"right\"&gt;Repetir Teste de HIV: Resultado do Teste&lt;/div&gt;&lt;/td&gt;\r\n    &lt;td colspan=\"2\"&gt;\r\n         &lt;obs id=\"repetirTestHIV\" conceptId=\"e1d800dc-1d5f-11e0-b929-000c29ad1d07\" answerConceptIds=\"e1d446cc-1d5f-11e0-b929-000c29ad1d07,e1d47386-1d5f-11e0-b929-000c29ad1d07,e1d89f2e-1d5f-11e0-b929-000c29ad1d07,e1d85e2e-1d5f-11e0-b929-000c29ad1d07\" labelText=\"\" answerLabels=\"Negativo,Positivo,Indeterminado,NF\" style=\"radio\" dateLabel=\" | Data:\"/&gt;\r\n   &lt;/td&gt;\r\n   &lt;/tr&gt;\r\n   &lt;tr&gt;\r\n    &lt;td&gt;&lt;div align=\"right\"&gt;Apresenta sinais e sintomas de infecção aguda pelo HIV&lt;/div&gt;&lt;/td&gt;\r\n    &lt;td colspan=\"2\"&gt;&lt;obs conceptId=\"33a3bfcc-348e-429f-9667-769e0c11b5c4\" labelText=\"\" answerConceptIds=\"e1d81b62-1d5f-11e0-b929-000c29ad1d07,e1d81c70-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"Sim,Não\" style=\"radio\"/&gt;&lt;br/&gt;&lt;/td&gt;\r\n     &lt;/tr&gt;\r\n    &lt;tr&gt;\r\n    &lt;td&gt;&lt;div align=\"right\"&gt;Uso do preservativo como método de prevenção&lt;/div&gt;&lt;/td&gt;\r\n    &lt;td colspan=\"2\"&gt;&lt;obs conceptId=\"e1e74736-1d5f-11e0-b929-000c29ad1d07\" labelText=\"\" answerConceptIds=\"e1d81b62-1d5f-11e0-b929-000c29ad1d07,e1d81c70-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"Sim,Não\" style=\"radio\"/&gt;&lt;br/&gt;&lt;/td&gt;\r\n     &lt;/tr&gt;\r\n    &lt;tr&gt;\r\n    &lt;td&gt;&lt;div align=\"right\"&gt;Efeitos colaterais (ver os códigos dos efeitos colaterais abaixo)&lt;/div&gt;&lt;/td&gt;\r\n    &lt;td&gt;\r\n      1.&lt;obs conceptId=\"e1e07ece-1d5f-11e0-b929-000c29ad1d07\" labelText=\"\" answerConceptId=\"44d63565-9087-11e6-a98e-000c29db4475\" answerLabel=\"Náuseas,Vômitos/Dor Abdominal\"/&gt;&lt;br/&gt;\r\n      2.&lt;obs conceptId=\"e1e07ece-1d5f-11e0-b929-000c29ad1d07\" labelText=\"\" answerConceptId=\"e1cdb97e-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"Diarreia\"/&gt;&lt;br/&gt;\r\n      3.&lt;obs conceptId=\"e1e07ece-1d5f-11e0-b929-000c29ad1d07\" labelText=\"\" answerConceptId=\"48328d2d-350b-432a-9621-7f91a7325575\" answerLabel=\"Neuropsiquiátrico/Comportamento\"/&gt;&lt;br/&gt;\r\n      4.&lt;obs conceptId=\"e1e07ece-1d5f-11e0-b929-000c29ad1d07\" labelText=\"\" answerConceptId=\"e1d5f8be-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"Neuropatia Periférica\"/&gt;&lt;br/&gt;\r\n      5.&lt;obs conceptId=\"e1e07ece-1d5f-11e0-b929-000c29ad1d07\" labelText=\"\" answerConceptId=\"740dff18-9085-11e6-a98e-000c29db4475\" answerLabel=\"Erupção Cutânea/Dermatite\"/&gt;&lt;br/&gt;\r\n      6.&lt;obs conceptId=\"e1e07ece-1d5f-11e0-b929-000c29ad1d07\" labelText=\"\" answerConceptId=\"63aa3de4-9087-11e6-a98e-000c29db4475\" answerLabel=\"Hiperglicémia\"/&gt;&lt;br/&gt;\r\n      7.&lt;obs conceptId=\"e1e07ece-1d5f-11e0-b929-000c29ad1d07\" labelText=\"\" answerConceptId=\"1fc95721-0c2a-41c5-ba05-8f8ca484fc2f\" answerLabel=\"Dislipidemia\"/&gt;&lt;br/&gt;\r\n      8.&lt;obs conceptId=\"e1e07ece-1d5f-11e0-b929-000c29ad1d07\" labelText=\"\" answerConceptId=\"06637aa6-aeda-4b15-b86c-bd555f69c9af\" answerLabel=\"Lipodistrofia\"/&gt;&lt;br/&gt;       \r\n    &lt;/td&gt;\r\n    &lt;td&gt;\r\n      9.&lt;obs conceptId=\"e1e07ece-1d5f-11e0-b929-000c29ad1d07\" labelText=\"\" answerConceptId=\"b9fe8ecb-a41d-49d3-b6f6-2c381715262d\" answerLabel=\"Citopenia\"/&gt;&lt;br/&gt; \r\n        10.&lt;obs conceptId=\"e1e07ece-1d5f-11e0-b929-000c29ad1d07\" labelText=\"\" answerConceptId=\"20627f0d-858e-4465-a1e1-04f83a962224\" answerLabel=\"Pancreatite\"/&gt;&lt;br/&gt; \r\n        11.&lt;obs conceptId=\"e1e07ece-1d5f-11e0-b929-000c29ad1d07\" labelText=\"\" answerConceptId=\"8956c7ea-847a-4f70-91e8-e1cf325b85df\" answerLabel=\"Nefrotoxicidade\"/&gt;&lt;br/&gt; \r\n      12.&lt;obs conceptId=\"e1e07ece-1d5f-11e0-b929-000c29ad1d07\" labelText=\"\" answerConceptId=\"e1cdc68a-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"Hepatite\"/&gt;&lt;br/&gt;\r\n      13.&lt;obs conceptId=\"e1e07ece-1d5f-11e0-b929-000c29ad1d07\" labelText=\"\" answerConceptId=\"d0d485d3-3082-4b1b-a450-6cad31eb56b3\" answerLabel=\"Síndrome de Stevens-Johnson\"/&gt;&lt;br/&gt;\r\n      14.&lt;obs conceptId=\"e1e07ece-1d5f-11e0-b929-000c29ad1d07\" labelText=\"\" answerConceptId=\"833aba0d-430a-4537-b202-94c32e9a1317\" answerLabel=\"Hipersensibilidade a ABC/RAL\"/&gt;&lt;br/&gt;\r\n      15.&lt;obs conceptId=\"e1e07ece-1d5f-11e0-b929-000c29ad1d07\" labelText=\"\" answerConceptId=\"c7089026-9135-4cd8-af18-596e14e4c512\" answerLabel=\"Acidose Láctica\"/&gt;&lt;br/&gt;\r\n      16.&lt;obs conceptId=\"e1e07ece-1d5f-11e0-b929-000c29ad1d07\" labelText=\"\" answerConceptId=\"da3dea8e-9b35-4025-ad5e-cd9aad7707aa\" answerLabel=\"Esteatose Hepática c/Hiperlactemia\"/&gt;\r\n    &lt;/td&gt;\r\n   &lt;/tr&gt;\r\n    &lt;tr&gt;\r\n    &lt;td&gt;&lt;div align=\"right\"&gt;Valor de Creatinina Sérica&lt;/div&gt;&lt;/td&gt;\r\n    &lt;td colspan=\"2\"&gt;\r\n      &lt;obs conceptId=\"1a6ffe36-df25-4cb4-a2cd-d7368fa5b027\" labelText=\"Pedido:\" answerConceptIds=\"e1d81b62-1d5f-11e0-b929-000c29ad1d07,e1d81c70-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"Sim,Não\" style=\"radio\"/&gt;&lt;br/&gt;&lt;br/&gt;\r\n      Resultado:\r\n      &lt;obs conceptId=\"e1d5d21c-1d5f-11e0-b929-000c29ad1d07\" dateLabel=\" | Data:\"/&gt;\r\n    &lt;/td&gt;\r\n     &lt;/tr&gt;\r\n    &lt;tr&gt;\r\n    &lt;td&gt;&lt;div align=\"right\"&gt;Tem sinais e sintomas sugestivos de ITS? (S/N)&lt;/div&gt;&lt;/td&gt;\r\n    &lt;td colspan=\"2\"&gt;&lt;obs conceptId=\"794ef662-03bc-4e22-90ff-38742b82827a\" labelText=\"\" answerConceptIds=\"e1d81b62-1d5f-11e0-b929-000c29ad1d07,e1d81c70-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"Sim,Não\" style=\"radio\"/&gt;&lt;/td&gt;\r\n     &lt;/tr&gt;\r\n    &lt;tr&gt;\r\n    &lt;td&gt;&lt;div align=\"right\"&gt;Adesão: Saldo de comprimidos na consulta&lt;/div&gt;&lt;/td&gt;\r\n    &lt;td colspan=\"2\"&gt;&lt;obs conceptId=\"e1de2aa2-1d5f-11e0-b929-000c29ad1d07\" labelText=\"Total comprimidos que sobraram\"/&gt;&lt;/td&gt;\r\n     &lt;/tr&gt;\r\n    &lt;tr&gt;\r\n    &lt;td&gt;&lt;div align=\"right\"&gt;Feito aconselhamento para a adesão? (assinalar)&lt;/div&gt;&lt;/td&gt;\r\n    &lt;td colspan=\"2\"&gt;&lt;obs conceptId=\"bd2f81f6-89f6-44ae-9df2-c9b18ad49f35\" labelText=\"\" answerConceptIds=\"e1d81b62-1d5f-11e0-b929-000c29ad1d07,e1d81c70-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"Sim,Não\" style=\"radio\"/&gt;&lt;/td&gt;\r\n     &lt;/tr&gt;\r\n    &lt;tr&gt;\r\n    &lt;td&gt;&lt;div align=\"right\"&gt;Feito aconselhamento para redução de risco? (assinalar)&lt;/div&gt;&lt;/td&gt;\r\n    &lt;td colspan=\"2\"&gt;&lt;obs conceptId=\"caa7703a-56d7-4383-b365-80de1e1812ea\" labelText=\"\" answerConceptIds=\"e1d81b62-1d5f-11e0-b929-000c29ad1d07,e1d81c70-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"Sim,Não\" style=\"radio\"/&gt;&lt;/td&gt;\r\n     &lt;/tr&gt;\r\n    &lt;tr&gt;\r\n    &lt;td&gt;&lt;div align=\"right\"&gt;Preservativos e lubrificantes fornecidos? &lt;/div&gt;&lt;/td&gt;\r\n    &lt;td colspan=\"2\"&gt;&lt;obs conceptId=\"b7c1d7b4-1e7b-44db-873e-6c96118969ce\" labelText=\"Preservativo\" answerConceptIds=\"e1d81b62-1d5f-11e0-b929-000c29ad1d07,e1d81c70-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"Sim,Não\" style=\"radio\"/&gt;&lt;br/&gt;\r\n      &lt;obs conceptId=\"3397b23a-5d7f-4312-9dd6-96950b5313f4\" labelText=\"Lubrificante\" answerConceptIds=\"e1d81b62-1d5f-11e0-b929-000c29ad1d07,e1d81c70-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"Sim,Não\" style=\"radio\"/&gt;\r\n    &lt;/td&gt;\r\n     &lt;/tr&gt;\r\n    &lt;tr&gt;\r\n    &lt;td&gt;&lt;div align=\"right\"&gt;Se mulher, indique o estado de Gravidez /Lactação? (assinalar)&lt;/div&gt;&lt;/td&gt;\r\n    &lt;td colspan=\"2\"&gt;&lt;span class=\"estadoDaMulher\"&gt;&lt;obs conceptId=\"f9d3e8d1-99f0-48f2-82cc-8bae6c72a023\" labelText=\"\" answerConceptId=\"e1e056a6-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"Grávida\"/&gt;\r\n      &lt;obs conceptId=\"f9d3e8d1-99f0-48f2-82cc-8bae6c72a023\" labelText=\"\" answerConceptId=\"bc4fe755-fc8f-49b8-9956-baf2477e8313\" answerLabel=\"Lactante\"/&gt;\r\n      &lt;obs conceptId=\"f9d3e8d1-99f0-48f2-82cc-8bae6c72a023\" labelText=\"\" answerConceptId=\"e1d8e10a-1d5f-11e0-b929-000c29ad1d07\" answerLabels=\"Não Aplicável\"/&gt;&lt;/span&gt;&lt;/td&gt;\r\n    &lt;/tr&gt;\r\n    &lt;tr&gt;\r\n    &lt;td&gt;&lt;div align=\"right\"&gt;Repetir a Prescrição da PrEP: ARVs prescritos (assinalar) Número de comprimidos&lt;/div&gt;&lt;/td&gt;\r\n    &lt;td colspan=\"2\"&gt;&lt;obs conceptId=\"0bfae0d8-e2aa-48e4-b4a4-c157021b4f15\" labelText=\"\" answerConceptIds=\"8c8d5c95-bd54-4fe9-a544-30277396e903,17247380-ec48-46b3-8159-5ee50c84129a,2ea7b406-f963-408c-b8ab-1b745974222f\" answerLabels=\"TDF/3TC,TDF/FTC,Sem prescrição\" style=\"radio\"/&gt;&lt;br/&gt;\r\n                    &lt;obs conceptId=\"18d4175b-df7c-4659-a266-38e9ff60278e\" labelText=\"# de frascos:\"/&gt;  \r\n    &lt;/td&gt;\r\n     &lt;/tr&gt;\r\n    &lt;tr&gt;\r\n    &lt;td&gt;&lt;div align=\"right\"&gt;Caso não prescreva a PREP, indique o motivo (ver a lista e os códigos abaixo)&lt;/div&gt;&lt;/td&gt;\r\n    &lt;td&gt;\r\n      1.&lt;obs conceptId=\"157fba33-7504-477a-aa02-b3cb0f639403\" labelText=\"\" answerConceptId=\"e1d8dab6-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"Testado HIV+\"/&gt;&lt;br/&gt;\r\n      2.&lt;obs conceptId=\"157fba33-7504-477a-aa02-b3cb0f639403\" labelText=\"\" answerConceptId=\"dad6ca9b-e15e-4773-8f18-c7805cda9b6b\" answerLabel=\"Sem mais riscos substanciais\"/&gt;&lt;br/&gt;\r\n      3.&lt;obs conceptId=\"157fba33-7504-477a-aa02-b3cb0f639403\" labelText=\"\" answerConceptId=\"e1e07ece-1d5f-11e0-b929-000c29ad1d07\" answerLabel=\"Efeitos colaterais\"/&gt;&lt;br/&gt;\r\n    &lt;/td&gt;\r\n    &lt;td&gt;\r\n      4.&lt;obs conceptId=\"157fba33-7504-477a-aa02-b3cb0f639403\" answerConceptId=\"16810d18-2c75-47a0-9b00-7aa21fb4667f\" labelText=\"\" answerLabel=\"Preferência do utente\"/&gt;&lt;br/&gt;\r\n       5.&lt;obs conceptId=\"157fba33-7504-477a-aa02-b3cb0f639403\" answerLabel=\"\" commentFieldLabel=\"Outro(especifique): \" answerConceptId=\"e1e783ea-1d5f-11e0-b929-000c29ad1d07\" /&gt;&lt;br/&gt;\r\n      6.&lt;obs conceptId=\"157fba33-7504-477a-aa02-b3cb0f639403\" answerConceptId=\"e1d8e10a-1d5f-11e0-b929-000c29ad1d07\" labelText=\"\" answerLabel=\"Não aplicável\"/&gt; \r\n    &lt;/td&gt;\r\n&lt;/tr&gt;\r\n    &lt;tr&gt;\r\n    &lt;td&gt;&lt;div align=\"right\"&gt;Data da próxima visita marcada (dd/mm/aa)&lt;/div&gt;&lt;/td&gt;\r\n        &lt;td colspan=\"2\"&gt;&lt;obs id=\"dataProxima\" conceptId=\"a5103b5d-c64e-4761-aa78-e85c2af8a4af\" labelText=\"\" allowFutureDates=\"true\" required=\"true\"/&gt;&lt;/td&gt;  \r\n     &lt;/tr&gt;\r\n    &lt;tr&gt;\r\n    &lt;td&gt;&lt;div align=\"right\"&gt;OBS:&lt;/div&gt;&lt;/td&gt;\r\n    &lt;td colspan=\"2\"&gt;&lt;obs conceptId=\"506bc615-81ee-4aa5-9f81-11167b45aabf\" labelText=\"\"  style=\"textarea\"/&gt;&lt;/td&gt;\r\n    &lt;/tr&gt;\r\n    &lt;tr&gt;\r\n      &lt;td colspan=\"3\"&gt;&lt;div align=\"center\"&gt;\r\n        &lt;submit submitLabel=\"Submeter\"/&gt;\r\n      &lt;/div&gt;&lt;/td&gt;\r\n    &lt;/tr&gt;\r\n    &lt;/tbody&gt;\r\n  &lt;/table&gt;\r\n  &lt;/body&gt;\r\n  &lt;/html&gt;\r\n  &lt;/htmlform&gt;</t>
+  </si>
+  <si>
+    <t>e8abe96b-4e00-4d32-af7a-085343bff120</t>
+  </si>
 </sst>
 </file>
 
@@ -1450,10 +1458,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="d/m/yyyy\ h:mm"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -1471,17 +1479,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1491,9 +1498,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1504,6 +1526,14 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1523,14 +1553,6 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -1539,29 +1561,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1575,8 +1575,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1589,14 +1605,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -1604,18 +1612,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1628,7 +1636,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1640,7 +1762,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1652,43 +1792,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1700,115 +1816,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1819,21 +1827,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1870,21 +1863,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1896,11 +1874,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1919,140 +1903,164 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -2392,8 +2400,8 @@
   <sheetPr/>
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -3873,8 +3881,64 @@
         <v>111</v>
       </c>
     </row>
-    <row r="51" ht="13.5" customHeight="1"/>
-    <row r="52" ht="13.5" customHeight="1"/>
+    <row r="51" ht="13.5" customHeight="1" spans="1:10">
+      <c r="A51">
+        <v>100</v>
+      </c>
+      <c r="B51">
+        <v>190</v>
+      </c>
+      <c r="D51" t="s">
+        <v>112</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51" s="5">
+        <v>44273.435</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+      <c r="H51" s="5">
+        <v>44273.435</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
+      </c>
+      <c r="J51" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="52" ht="13.5" customHeight="1" spans="1:10">
+      <c r="A52">
+        <v>101</v>
+      </c>
+      <c r="B52">
+        <v>191</v>
+      </c>
+      <c r="D52" t="s">
+        <v>114</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52" s="5">
+        <v>44273.435</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
+      </c>
+      <c r="H52" s="5">
+        <v>44273.435</v>
+      </c>
+      <c r="I52">
+        <v>0</v>
+      </c>
+      <c r="J52" t="s">
+        <v>115</v>
+      </c>
+    </row>
     <row r="53" ht="13.5" customHeight="1"/>
     <row r="54" ht="13.5" customHeight="1"/>
     <row r="55" ht="13.5" customHeight="1"/>

</xml_diff>